<commit_message>
fixed default value of maximumPenaltyFreeDisbursement term #4
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2080" uniqueCount="940">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">2020-03-27</t>
   </si>
   <si>
-    <t xml:space="preserve">Added maturityDate state variable</t>
+    <t xml:space="preserve">Added maturityDate state variable and fixed default value of maximumPenaltyFreeDisbursement</t>
   </si>
   <si>
     <t xml:space="preserve">Identifier</t>
@@ -2256,6 +2256,9 @@
   </si>
   <si>
     <t xml:space="preserve">MPFD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ the value of notionalPrincipal ]</t>
   </si>
   <si>
     <t xml:space="preserve">Defines the notional amount which can be withdrawn before XDN without penalty</t>
@@ -3546,7 +3549,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5508,9 +5511,9 @@
   <dimension ref="A1:AA115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10775,11 +10778,11 @@
         <v>306</v>
       </c>
       <c r="G93" s="19" t="s">
-        <v>430</v>
+        <v>665</v>
       </c>
       <c r="H93" s="20"/>
       <c r="I93" s="18" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="J93" s="20"/>
       <c r="K93" s="18" t="s">
@@ -10804,16 +10807,16 @@
     </row>
     <row r="94" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="18" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="B94" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C94" s="18" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="E94" s="18" t="s">
         <v>237</v>
@@ -10824,34 +10827,34 @@
       <c r="G94" s="19"/>
       <c r="H94" s="18"/>
       <c r="I94" s="18" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="J94" s="18"/>
       <c r="K94" s="18" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="L94" s="18" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="M94" s="18" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="N94" s="18" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="O94" s="20"/>
       <c r="P94" s="18" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="Q94" s="18" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="R94" s="18"/>
       <c r="S94" s="18"/>
       <c r="T94" s="18"/>
       <c r="U94" s="18"/>
       <c r="V94" s="18" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="W94" s="20"/>
       <c r="X94" s="20"/>
@@ -10861,16 +10864,16 @@
     </row>
     <row r="95" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="18" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C95" s="18" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="E95" s="18" t="s">
         <v>384</v>
@@ -10879,7 +10882,7 @@
       <c r="G95" s="21"/>
       <c r="H95" s="18"/>
       <c r="I95" s="18" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="J95" s="18"/>
       <c r="K95" s="20"/>
@@ -10887,7 +10890,7 @@
       <c r="M95" s="20"/>
       <c r="N95" s="20"/>
       <c r="O95" s="18" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="P95" s="20"/>
       <c r="Q95" s="20"/>
@@ -10904,16 +10907,16 @@
     </row>
     <row r="96" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="18" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="E96" s="18" t="s">
         <v>356</v>
@@ -10922,34 +10925,34 @@
       <c r="G96" s="19"/>
       <c r="H96" s="18"/>
       <c r="I96" s="18" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="J96" s="18"/>
       <c r="K96" s="18" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="L96" s="18" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="M96" s="18" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="N96" s="18" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="O96" s="20"/>
       <c r="P96" s="18" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="Q96" s="18" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="R96" s="18"/>
       <c r="S96" s="18"/>
       <c r="T96" s="18"/>
       <c r="U96" s="18"/>
       <c r="V96" s="18" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="W96" s="20"/>
       <c r="X96" s="20"/>
@@ -10959,16 +10962,16 @@
     </row>
     <row r="97" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="18" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="B97" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C97" s="18" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D97" s="18" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="E97" s="18" t="s">
         <v>394</v>
@@ -10977,7 +10980,7 @@
       <c r="G97" s="21"/>
       <c r="H97" s="18"/>
       <c r="I97" s="18" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="J97" s="18"/>
       <c r="K97" s="20"/>
@@ -10985,7 +10988,7 @@
       <c r="M97" s="20"/>
       <c r="N97" s="20"/>
       <c r="O97" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="P97" s="20"/>
       <c r="Q97" s="20"/>
@@ -11002,16 +11005,16 @@
     </row>
     <row r="98" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="18" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B98" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="E98" s="18" t="s">
         <v>305</v>
@@ -11022,24 +11025,24 @@
       </c>
       <c r="H98" s="18"/>
       <c r="I98" s="18" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="J98" s="18"/>
       <c r="K98" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="L98" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="M98" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="N98" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="O98" s="20"/>
       <c r="P98" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="Q98" s="18" t="s">
         <v>233</v>
@@ -11059,16 +11062,16 @@
     </row>
     <row r="99" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="18" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="B99" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C99" s="18" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="E99" s="18" t="s">
         <v>551</v>
@@ -11077,7 +11080,7 @@
       <c r="G99" s="21"/>
       <c r="H99" s="18"/>
       <c r="I99" s="18" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="J99" s="18"/>
       <c r="K99" s="20"/>
@@ -11085,7 +11088,7 @@
       <c r="M99" s="20"/>
       <c r="N99" s="20"/>
       <c r="O99" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="P99" s="20"/>
       <c r="Q99" s="20"/>
@@ -11102,27 +11105,27 @@
     </row>
     <row r="100" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="18" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="B100" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C100" s="18" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="E100" s="18" t="s">
         <v>321</v>
       </c>
       <c r="F100" s="18" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="G100" s="21"/>
       <c r="H100" s="18"/>
       <c r="I100" s="18" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="J100" s="18"/>
       <c r="K100" s="20"/>
@@ -11130,7 +11133,7 @@
       <c r="M100" s="20"/>
       <c r="N100" s="20"/>
       <c r="O100" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="P100" s="20"/>
       <c r="Q100" s="20"/>
@@ -11147,16 +11150,16 @@
     </row>
     <row r="101" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="18" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B101" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C101" s="18" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="D101" s="18" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="E101" s="18" t="s">
         <v>249</v>
@@ -11165,26 +11168,26 @@
       <c r="G101" s="19"/>
       <c r="H101" s="18"/>
       <c r="I101" s="18" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="J101" s="18"/>
       <c r="K101" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="L101" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="M101" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="N101" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="O101" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="P101" s="18" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="Q101" s="18" t="s">
         <v>233</v>
@@ -11204,16 +11207,16 @@
     </row>
     <row r="102" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="18" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B102" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C102" s="18" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="E102" s="18" t="s">
         <v>305</v>
@@ -11222,25 +11225,25 @@
       <c r="G102" s="19"/>
       <c r="H102" s="18"/>
       <c r="I102" s="18" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="J102" s="18"/>
       <c r="K102" s="18"/>
       <c r="L102" s="20"/>
       <c r="M102" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="N102" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="O102" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="P102" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="Q102" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="R102" s="18"/>
       <c r="S102" s="18"/>
@@ -11257,16 +11260,16 @@
     </row>
     <row r="103" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="18" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B103" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C103" s="18" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="E103" s="18" t="s">
         <v>305</v>
@@ -11275,25 +11278,25 @@
       <c r="G103" s="19"/>
       <c r="H103" s="18"/>
       <c r="I103" s="18" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="J103" s="18"/>
       <c r="K103" s="18"/>
       <c r="L103" s="20"/>
       <c r="M103" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="N103" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="O103" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="P103" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="Q103" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="R103" s="18"/>
       <c r="S103" s="18"/>
@@ -11310,16 +11313,16 @@
     </row>
     <row r="104" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="18" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C104" s="18" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="E104" s="18" t="s">
         <v>305</v>
@@ -11330,25 +11333,25 @@
       <c r="G104" s="19"/>
       <c r="H104" s="18"/>
       <c r="I104" s="18" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="J104" s="18"/>
       <c r="K104" s="18"/>
       <c r="L104" s="20"/>
       <c r="M104" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="N104" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="O104" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="P104" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="Q104" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="R104" s="18"/>
       <c r="S104" s="18"/>
@@ -11363,16 +11366,16 @@
     </row>
     <row r="105" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="18" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C105" s="18" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="E105" s="18" t="s">
         <v>305</v>
@@ -11383,25 +11386,25 @@
       <c r="G105" s="19"/>
       <c r="H105" s="18"/>
       <c r="I105" s="18" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="J105" s="18"/>
       <c r="K105" s="18"/>
       <c r="L105" s="20"/>
       <c r="M105" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="N105" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="O105" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="P105" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="Q105" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="R105" s="18"/>
       <c r="S105" s="18"/>
@@ -11416,41 +11419,41 @@
     </row>
     <row r="106" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="18" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="E106" s="18" t="s">
         <v>210</v>
       </c>
       <c r="F106" s="18" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="G106" s="19" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="H106" s="18"/>
       <c r="I106" s="18" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="J106" s="18"/>
       <c r="K106" s="18"/>
       <c r="L106" s="20"/>
       <c r="M106" s="18" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="N106" s="18" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="O106" s="18" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="P106" s="20"/>
       <c r="Q106" s="20"/>
@@ -11459,7 +11462,7 @@
       <c r="T106" s="18"/>
       <c r="U106" s="18"/>
       <c r="V106" s="18" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="W106" s="20"/>
       <c r="X106" s="20"/>
@@ -11469,16 +11472,16 @@
     </row>
     <row r="107" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="18" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C107" s="18" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="E107" s="18" t="s">
         <v>290</v>
@@ -11489,34 +11492,34 @@
       </c>
       <c r="H107" s="18"/>
       <c r="I107" s="18" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="J107" s="18"/>
       <c r="K107" s="18"/>
       <c r="L107" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="M107" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="N107" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="O107" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="P107" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="Q107" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="R107" s="18"/>
       <c r="S107" s="18"/>
       <c r="T107" s="18"/>
       <c r="U107" s="18"/>
       <c r="V107" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="W107" s="20"/>
       <c r="X107" s="20"/>
@@ -11526,16 +11529,16 @@
     </row>
     <row r="108" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="18" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B108" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C108" s="18" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="D108" s="18" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="E108" s="18" t="s">
         <v>305</v>
@@ -11544,34 +11547,34 @@
       <c r="G108" s="19"/>
       <c r="H108" s="18"/>
       <c r="I108" s="18" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="J108" s="18"/>
       <c r="K108" s="18"/>
       <c r="L108" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="M108" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="N108" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="O108" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="P108" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="Q108" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="R108" s="18"/>
       <c r="S108" s="18"/>
       <c r="T108" s="18"/>
       <c r="U108" s="18"/>
       <c r="V108" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="W108" s="20"/>
       <c r="X108" s="20"/>
@@ -11581,16 +11584,16 @@
     </row>
     <row r="109" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="18" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B109" s="18" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C109" s="18" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="D109" s="18" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="E109" s="18" t="s">
         <v>305</v>
@@ -11601,34 +11604,34 @@
       </c>
       <c r="H109" s="18"/>
       <c r="I109" s="18" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="J109" s="18"/>
       <c r="K109" s="18"/>
       <c r="L109" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="M109" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="N109" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="O109" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="P109" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="Q109" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="R109" s="18"/>
       <c r="S109" s="18"/>
       <c r="T109" s="18"/>
       <c r="U109" s="18"/>
       <c r="V109" s="18" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="W109" s="20"/>
       <c r="X109" s="20"/>
@@ -11638,16 +11641,16 @@
     </row>
     <row r="110" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="18" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B110" s="18" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="D110" s="18" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="E110" s="18" t="s">
         <v>237</v>
@@ -11658,7 +11661,7 @@
       <c r="G110" s="19"/>
       <c r="H110" s="18"/>
       <c r="I110" s="18" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="J110" s="18"/>
       <c r="K110" s="18"/>
@@ -11671,36 +11674,36 @@
       <c r="R110" s="18"/>
       <c r="S110" s="18"/>
       <c r="T110" s="18" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="U110" s="18" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="V110" s="20"/>
       <c r="W110" s="20"/>
       <c r="X110" s="18" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="Y110" s="18" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="Z110" s="18" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="AA110" s="18"/>
     </row>
     <row r="111" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="18" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="B111" s="18" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C111" s="18" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="D111" s="18" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="E111" s="18" t="s">
         <v>305</v>
@@ -11711,7 +11714,7 @@
         <v>339</v>
       </c>
       <c r="I111" s="18" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="J111" s="18"/>
       <c r="K111" s="18"/>
@@ -11724,36 +11727,36 @@
       <c r="R111" s="18"/>
       <c r="S111" s="18"/>
       <c r="T111" s="18" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="U111" s="18" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="V111" s="20"/>
       <c r="W111" s="20"/>
       <c r="X111" s="18" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="Y111" s="18" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="Z111" s="18" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="AA111" s="18"/>
     </row>
     <row r="112" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="18" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B112" s="18" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C112" s="18" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="D112" s="18" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="E112" s="18" t="s">
         <v>290</v>
@@ -11764,7 +11767,7 @@
       </c>
       <c r="H112" s="18"/>
       <c r="I112" s="18" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="J112" s="18"/>
       <c r="K112" s="18"/>
@@ -11797,29 +11800,29 @@
     </row>
     <row r="113" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="18" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B113" s="18" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C113" s="18" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="D113" s="18" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="E113" s="18" t="s">
         <v>210</v>
       </c>
       <c r="F113" s="18" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="G113" s="19" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="H113" s="18"/>
       <c r="I113" s="18" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="J113" s="18"/>
       <c r="K113" s="18"/>
@@ -11852,16 +11855,16 @@
     </row>
     <row r="114" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="18" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B114" s="18" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C114" s="18" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="D114" s="18" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="E114" s="18" t="s">
         <v>305</v>
@@ -11870,7 +11873,7 @@
       <c r="G114" s="19"/>
       <c r="H114" s="18"/>
       <c r="I114" s="18" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="J114" s="18"/>
       <c r="K114" s="18"/>
@@ -11895,16 +11898,16 @@
     </row>
     <row r="115" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="18" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B115" s="18" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C115" s="18" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="D115" s="18" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="E115" s="18" t="s">
         <v>249</v>
@@ -11915,7 +11918,7 @@
       <c r="G115" s="19"/>
       <c r="H115" s="18"/>
       <c r="I115" s="18" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="J115" s="18"/>
       <c r="K115" s="18" t="s">
@@ -12033,7 +12036,7 @@
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9"/>
       <c r="B2" s="29" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -12091,7 +12094,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="29"/>
       <c r="B4" s="29" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -12149,10 +12152,10 @@
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="29"/>
       <c r="B6" s="29" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="29"/>
@@ -12182,7 +12185,7 @@
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="29" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -12239,10 +12242,10 @@
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="29"/>
       <c r="B9" s="29" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="29"/>
@@ -12272,11 +12275,11 @@
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="29" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="29" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -12331,12 +12334,12 @@
     <row r="12" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
       <c r="B12" s="29" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="20" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -12391,14 +12394,14 @@
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
       <c r="B14" s="29" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="20" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -12455,10 +12458,10 @@
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="29" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
@@ -12487,10 +12490,10 @@
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="29" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
@@ -12519,10 +12522,10 @@
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="29" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -12578,11 +12581,11 @@
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="29" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="20" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -12639,10 +12642,10 @@
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="29" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -12671,10 +12674,10 @@
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="29" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
@@ -12730,11 +12733,11 @@
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="29" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="20" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -12791,10 +12794,10 @@
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="30" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
@@ -12823,10 +12826,10 @@
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="30" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
@@ -12855,10 +12858,10 @@
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
       <c r="D29" s="30" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -12887,10 +12890,10 @@
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="30" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
@@ -12919,10 +12922,10 @@
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="30" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -12978,11 +12981,11 @@
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="29" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="20" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
@@ -13039,10 +13042,10 @@
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
       <c r="D35" s="29" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
@@ -13071,10 +13074,10 @@
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="29" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
@@ -13103,10 +13106,10 @@
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
       <c r="D37" s="29" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -13135,10 +13138,10 @@
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
       <c r="D38" s="29" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
@@ -13167,10 +13170,10 @@
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
       <c r="D39" s="29" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
@@ -13226,11 +13229,11 @@
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="20" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
@@ -13287,10 +13290,10 @@
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="29" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="E43" s="29" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
@@ -13319,10 +13322,10 @@
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
       <c r="D44" s="30" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
@@ -13351,10 +13354,10 @@
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
       <c r="D45" s="29" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
@@ -13409,14 +13412,14 @@
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="29"/>
       <c r="B47" s="29" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="D47" s="29"/>
       <c r="E47" s="20" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="F47" s="29"/>
       <c r="G47" s="29"/>
@@ -13446,7 +13449,7 @@
       <c r="C48" s="29"/>
       <c r="D48" s="29"/>
       <c r="E48" s="20" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="F48" s="29"/>
       <c r="G48" s="29"/>
@@ -13476,7 +13479,7 @@
       <c r="C49" s="29"/>
       <c r="D49" s="29"/>
       <c r="E49" s="20" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="F49" s="29"/>
       <c r="G49" s="29"/>
@@ -14469,7 +14472,7 @@
   </sheetPr>
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -14513,7 +14516,7 @@
         <v>236</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>237</v>
@@ -14533,7 +14536,7 @@
         <v>273</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>210</v>
@@ -14553,7 +14556,7 @@
         <v>285</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>237</v>
@@ -14573,7 +14576,7 @@
         <v>430</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>305</v>
@@ -14590,7 +14593,7 @@
         <v>511</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>305</v>
@@ -14607,7 +14610,7 @@
         <v>398</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>305</v>
@@ -14624,7 +14627,7 @@
         <v>402</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>305</v>
@@ -14641,7 +14644,7 @@
         <v>411</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>305</v>
@@ -14649,16 +14652,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>305</v>
@@ -14675,7 +14678,7 @@
         <v>371</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>305</v>
@@ -14689,10 +14692,10 @@
         <v>427</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>305</v>
@@ -14700,16 +14703,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>305</v>
@@ -14717,16 +14720,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>305</v>
@@ -14740,10 +14743,10 @@
         <v>545</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>305</v>
@@ -14751,16 +14754,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>237</v>
@@ -14771,16 +14774,16 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>305</v>
@@ -14797,7 +14800,7 @@
         <v>570</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>237</v>
@@ -14817,7 +14820,7 @@
         <v>505</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>237</v>
@@ -14871,21 +14874,21 @@
         <v>10</v>
       </c>
       <c r="E1" s="31" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>497</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>1</v>
@@ -14893,16 +14896,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>2</v>
@@ -14910,16 +14913,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>3</v>
@@ -14927,16 +14930,16 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>4</v>
@@ -14944,16 +14947,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>273</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>5</v>
@@ -14961,16 +14964,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>6</v>
@@ -14978,16 +14981,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>7</v>
@@ -14995,16 +14998,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="E9" s="4" t="n">
         <v>8</v>
@@ -15012,16 +15015,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>9</v>
@@ -15029,16 +15032,16 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="E11" s="4" t="n">
         <v>10</v>
@@ -15046,16 +15049,16 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="E12" s="4" t="n">
         <v>11</v>
@@ -15063,16 +15066,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="E13" s="4" t="n">
         <v>12</v>
@@ -15080,16 +15083,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="E14" s="4" t="n">
         <v>13</v>
@@ -15097,16 +15100,16 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>560</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="E15" s="4" t="n">
         <v>14</v>
@@ -15114,16 +15117,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>15</v>
@@ -15131,16 +15134,16 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>570</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="E17" s="4" t="n">
         <v>16</v>
@@ -15148,16 +15151,16 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="E18" s="4" t="n">
         <v>17</v>
@@ -15165,16 +15168,16 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>428</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="E19" s="4" t="n">
         <v>18</v>
@@ -15182,16 +15185,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>505</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>19</v>
@@ -15199,16 +15202,16 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="E21" s="4" t="n">
         <v>20</v>
@@ -15216,16 +15219,16 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="E22" s="4" t="n">
         <v>21</v>
@@ -15233,16 +15236,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="E23" s="4" t="n">
         <v>22</v>
@@ -15278,7 +15281,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="514.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
     </row>
   </sheetData>
@@ -15310,7 +15313,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added accronym to enum types
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -676,8 +676,8 @@
     <t xml:space="preserve">Enum</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: noCalendar, name: No Calendar, description: No holidays defined
-option: 1, identifier: mondayToFriday, name: MondayToFriday, description: Saturdays and Sundays are holidays</t>
+    <t xml:space="preserve">option: 0, identifier: noCalendar, name: No Calendar, accronym: NC, description: No holidays defined
+option: 1, identifier: mondayToFriday, name: MondayToFriday, accronym: MF, description: Saturdays and Sundays are holidays</t>
   </si>
   <si>
     <t xml:space="preserve">noCalendar</t>
@@ -698,15 +698,15 @@
     <t xml:space="preserve">BDC</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: nos, name: No Shift, description: No shift applied to non-business days.
-option: 1, identifier: scf, name: Shift-Calculate Following, description: Shift event dates first then calculate accruals etc. Strictly shift to the next following business day.
-option: 2, identifier: scmf, name: Shift-Calculate Modified-Following, description: Shift event dates first then calculate accruals etc. Shift to the next following business day if this falls in the same month. Shift to the most recent preceding business day otherwise.
-option: 3, identifier: csf, name: Calculate-Shift Following, description: Calculate accruals etc. first then shift event dates. Strictly shift to the next following business day.
-option: 4, identifier: scmf, name: Shift-Calculate Modified-Following, description: Calculate accruals etc. first then shift event dates. Shift to the next following business day if this falls in the same month. Shift to the most recent preceding business day otherwise.
-option: 5, identifier: scp, name: Shift-Calculate Preceding, description: Shift event dates first then calculate accruals etc. Strictly shift to the most recent preceding business day.
-option: 6, identifier: scmp, name: Shift-Calculate Modified-Preceding, description: Shift event dates first then calculate accruals etc. Shift to the most recent preceding business day if this falls in the same month. Shift to the next following business day otherwise.
-option: 7, identifier: csp, name: Calculate-Shift Preceding, description: Calculate accruals etc. first then shift event dates. Strictly shift to the most recent preceding business day.
-option: 8, identifier: scmp, name: Shift-Calculate Modified-Preceding, description: Calculate accruals etc. first then shift event dates. Shift to the most recent preceding business day if this falls in the same month. Shift to the next following business day otherwise.</t>
+    <t xml:space="preserve">option: 0, identifier: noShift, name: No Shift, accronym: NOS, description: No shift applied to non-business days.
+option: 1, identifier: shiftCalculateFollowing, name: Shift-Calculate Following, accronym: SCF, description: Shift event dates first then calculate accruals etc. Strictly shift to the next following business day.
+option: 2, identifier: shiftCalculateModifiedFollowing, name: Shift-Calculate Modified-Following, accronym: SCMF, description: Shift event dates first then calculate accruals etc. Shift to the next following business day if this falls in the same month. Shift to the most recent preceding business day otherwise.
+option: 3, identifier: calculateShiftFollowing, name: Calculate-Shift Following, accronym: CSF, description: Calculate accruals etc. first then shift event dates. Strictly shift to the next following business day.
+option: 4, identifier: calculateShiftModifiedFollowing, name: Calculate-Shift Modified-Following, accronym: CSMF, description: Calculate accruals etc. first then shift event dates. Shift to the next following business day if this falls in the same month. Shift to the most recent preceding business day otherwise.
+option: 5, identifier: shiftCalculatePreceding, name: Shift-Calculate Preceding, accronym: SCP, description: Shift event dates first then calculate accruals etc. Strictly shift to the most recent preceding business day.
+option: 6, identifier: shiftCalculateModifiedPreceding, name: Shift-Calculate Modified-Preceding, accronym: SCMP, description: Shift event dates first then calculate accruals etc. Shift to the most recent preceding business day if this falls in the same month. Shift to the next following business day otherwise.
+option: 7, identifier: calculateShiftPreceding, name: Calculate-Shift Preceding, accronym: CSP, description: Calculate accruals etc. first then shift event dates. Strictly shift to the most recent preceding business day.
+option: 8, identifier: calculateShiftModifiedPreceding, name: Calculate-Shift Modified-Preceding, accronym: SCMP, description: Calculate accruals etc. first then shift event dates. Shift to the most recent preceding business day if this falls in the same month. Shift to the next following business day otherwise.</t>
   </si>
   <si>
     <t xml:space="preserve">nos</t>
@@ -728,8 +728,8 @@
     <t xml:space="preserve">EOMC</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: sd, name: Same Day, description: Schedule times always fall on the schedule anchor date day of the month.
-option: 1, identifier: eom, name: End of Month, description: Schedule times fall on the end of every month if the anchor date represents the last day of the respective month.</t>
+    <t xml:space="preserve">option: 0, identifier: sameDay, name: Same Day, accronym: SD, description: Schedule times always fall on the schedule anchor date day of the month.
+option: 1, identifier: endOfMonth, name: End of Month, accronym: EOM, description: Schedule times fall on the end of every month if the anchor date represents the last day of the respective month.</t>
   </si>
   <si>
     <t xml:space="preserve">sd</t>
@@ -751,24 +751,24 @@
     <t xml:space="preserve">CT</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: pam, name: Principal at Maturity, description: Lending agreements with full amortization at maturity.
-option: 1, identifier: ann, name: Annuity, description: Lending agreements with fixed periodic payments consisting of an interest and principal portion. The periodic payments are adjusted for variable rate instruments such that maturity remains fixed.
-option: 2, identifier: nam, name: Negative Amortizer, description: Lending agreements with fixed periodic payments consisting of an interest and principal portion. Maturity changes for variable rate instruments. 
-option: 3, identifier: lam, name: Linear Amortizer, description: Lending agreements with fixed principal repayment amounts and variable interest payments.
-option: 4, identifier: lax, name: Exotic Linear Amortizer, description: Lending agreements with exotic repayment schedules.
-option: 5, identifier: clm, name: Call Money, description: Lonas that are rolled over as long as they are not called. Once called it has to be paid back after the stipulated notice period.
-option: 6, identifier: ump, name: Undefined Maturity Profile, description: Interest paying cash accounts (current / savings / etc.). 
-option: 7, identifier: csh, name: Cash, description: Represents cash holdings. 
-option: 8, identifier: stk, name: Stock, description: Represents stocks/shares/equity. 
-option: 9, identifier: com, name: Commodity, description: Represents commodities. 
-option: 10, identifier: swaps, name: Swap, description: An agreement of swapping two legs such as fixed against variable, currency 1 against currency 2, etc. 
-option: 11, identifier: swppv, name: Plain Vanilla Swap, description: Plain vanilla interest rate swaps. 
-option: 12, identifier: fxout, name: Foreign Exchange Outright, description: An agreement of swapping two cash flows in different currencies at a future point in time. 
-option: 13, identifier: capfl, name: Cap and Floor, description: An agreement of paying the differential (cap or floor) of a reference rate versus a fixed rate. 
-option: 14, identifier: futur, name: Future, description: An agreement of exchanging an underlying instrument against a fixed price in the future. 
-option: 15, identifier: option, name: Option, description: Different types of options on buying an underlying instrument at a fixed price in the future. 
-option: 16, identifier: ceg, name: Credit Enhancement Guarantee, description: A guarantee / letter of credit by a third party on the scheduled payment obligations of an underlying instrument 
-option: 17, identifier: cec, name: Credit Enhancement Collateral, description: A collateral securing the scheduled payment obligations of an underlying instrument</t>
+    <t xml:space="preserve">option: 0, identifier: principalAtMaturity, name: Principal at Maturity, accronym: PAM, description: Lending agreements with full amortization at maturity.
+option: 1, identifier: annuity, name: Annuity, accronym: ANN, description: Lending agreements with fixed periodic payments consisting of an interest and principal portion. The periodic payments are adjusted for variable rate instruments such that maturity remains fixed.
+option: 2, identifier: negativeAmortizer, name: Negative Amortizer, accronym: NAM, description: Lending agreements with fixed periodic payments consisting of an interest and principal portion. Maturity changes for variable rate instruments. 
+option: 3, identifier: linearAmortizer, name: Linear Amortizer, accronym: LAM, description: Lending agreements with fixed principal repayment amounts and variable interest payments.
+option: 4, identifier: exoticLinearAmortizer, name: Exotic Linear Amortizer, accronym: LAX, description: Lending agreements with exotic repayment schedules.
+option: 5, identifier: callMoney, name: Call Money, accronym: CLM, description: Lonas that are rolled over as long as they are not called. Once called it has to be paid back after the stipulated notice period.
+option: 6, identifier: undefinedMaturityProfile, name: Undefined Maturity Profile, accronym: UMP, description: Interest paying cash accounts (current / savings / etc.). 
+option: 7, identifier: cash, name: Cash, accronym: CSH, description: Represents cash holdings. 
+option: 8, identifier: stock, name: Stock, accronym: STK, description: Represents stocks/shares/equity. 
+option: 9, identifier: commodity, name: Commodity, accronym: COM, description: Represents commodities. 
+option: 10, identifier: swap, name: Swap, accronym: SWAPS, description: An agreement of swapping two legs such as fixed against variable, currency 1 against currency 2, etc. 
+option: 11, identifier: plainVanillaSwap, name: Plain Vanilla Swap, accronym: SWPPV, description: Plain vanilla interest rate swaps. 
+option: 12, identifier: foreignExchangeOutright, name: Foreign Exchange Outright, accronym: FXOUT, description: An agreement of swapping two cash flows in different currencies at a future point in time. 
+option: 13, identifier: capFloor, name: Cap and Floor, accronym: CAPFL, description: An agreement of paying the differential (cap or floor) of a reference rate versus a fixed rate. 
+option: 14, identifier: future, name: Future, accronym: FUTUR, description: An agreement of exchanging an underlying instrument against a fixed price in the future. 
+option: 15, identifier: option, name: Option, accronym: OPTNS, description: Different types of options on buying an underlying instrument at a fixed price in the future. 
+option: 16, identifier: creditEnhancementGuarantee, name: Credit Enhancement Guarantee, accronym: CEG, description: A guarantee / letter of credit by a third party on the scheduled payment obligations of an underlying instrument 
+option: 17, identifier: creditEnhancementCollateral, name: Credit Enhancement Collateral, accronym: CEC, description: A collateral securing the scheduled payment obligations of an underlying instrument</t>
   </si>
   <si>
     <t xml:space="preserve">The ContractType is the most important information. It defines the cash flow generating pattern of a contract. The ContractType information in combination with a given state of the risk factors will produce a deterministic sequence of cash flows which are the basis of any financial analysis.</t>
@@ -807,19 +807,19 @@
     <t xml:space="preserve">CNTRL</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: rpa, name: Real Position Asset, description: Contract creator takes the asset or lender side.
-option: 1, identifier: rpl, name: Real Position Liability, description: Contract creator takes the liability or borrower side. 
-option: 2, identifier: rfl, name: Receive First Leg, description: Contract creator receives the first leg. 
-option: 3, identifier: pfl, name: Pay First Leg, description: Contract creator pays the first leg.
-option: 4, identifier: rf, name: Receive Fix, description: Contract creator receives the fixed leg.
-option: 5, identifier: pf, name: Pay Fix, description: Contract creator pays the fixed leg.
-option: 6, identifier: buy, name: Buy underlying / protection, description: Contract creator holds the right to buy the underlying / exercise the option. 
-option: 7, identifier: sel, name: Sell underlying / protection, description: Contract creator holds the obligation to sell the underlying / deliver the option. 
-option: 8, identifier: col, name: Collateral position, description: Contract represents a collateral to an underlying instrument
-option: 9, identifier: cno, name: Close out Netting, description: Contract creator and counterparty agree on netting payment obligations of underlying instruments in case of default. 
-option: 10, identifier: udl, name: Underlying, description: Contract represents the underlying to a composed contract. Role of the underlying is derived from the parent. 
-option: 11, identifier: udlp, name: Underlying Plus, description: Contract represents the underlying to a composed contract. Role of the underlying is derived from the parent. When considered a standalone contract the underlying’s creator takes the asset side. 
-option: 12, identifier: udlm, name: Underlying Minus, description: Contract represents the underlying to a composed contract. Role of the underlying is derived from the parent. When considered a standalone contract the underlying’s creator takes the liability side.</t>
+    <t xml:space="preserve">option: 0, identifier: realPositionAsset, name: Real Position Asset, accronym: RPA, description: Contract creator takes the asset or lender side.
+option: 1, identifier: realPositionLiability, name: Real Position Liability, accronym: RPL, description: Contract creator takes the liability or borrower side. 
+option: 2, identifier: receiveFirstLegl, name: Receive First Leg, accronym: RFL, description: Contract creator receives the first leg. 
+option: 3, identifier: payFirstLeg, name: Pay First Leg, accronym: PFL, description: Contract creator pays the first leg.
+option: 4, identifier: receiveFix, name: Receive Fix, accronym: RF, description: Contract creator receives the fixed leg.
+option: 5, identifier: payFix, name: Pay Fix, accronym: PF, description: Contract creator pays the fixed leg.
+option: 6, identifier: buyer, name: Buyer, accronym: BUY, description: Contract creator holds the right to buy the underlying / exercise the option. 
+option: 7, identifier: seller, name: Seller, accronym: SEL, description: Contract creator holds the obligation to sell the underlying / deliver the option. 
+option: 8, identifier: collateralPosition, name: Collateral Position, accronym: COL, description: Contract represents a collateral to an underlying instrument
+option: 9, identifier: closeOutNetting, name: Close out Netting, accronym: CNO, description: Contract creator and counterparty agree on netting payment obligations of underlying instruments in case of default. 
+option: 10, identifier: underlying, name: Underlying, accronym: UDL, description: Contract represents the underlying to a composed contract. Role of the underlying is derived from the parent. 
+option: 11, identifier: underlyingPlus, name: Underlying Plus, accronym: UDLP, description: Contract represents the underlying to a composed contract. Role of the underlying is derived from the parent. When considered a standalone contract the underlying’s creator takes the asset side. 
+option: 12, identifier: underlyingMinus, name: Underlying Minus, accronym: UDLM, description: Contract represents the underlying to a composed contract. Role of the underlying is derived from the parent. When considered a standalone contract the underlying’s creator takes the liability side.</t>
   </si>
   <si>
     <t xml:space="preserve">CNTRL defines which position the CRID ( the creator of the contract record ) takes in a contract. For example, whether the contract is an asset or liability, a long or short position for the CRID. 
@@ -916,10 +916,10 @@
     <t xml:space="preserve">PRF</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: pf, name: Performant, description: Contract is performing according to terms and conditions.
-option: 1, identifier: dl, name: Delayed, description: Contractual payment obligations are delayed according to the Grace Period.
-option: 2, identifier: dq, name: Delinquent, description: Contractual payment obligations are delinquent according to the Delinquency Period.
-option: 3, identifier: df, name: Default, description: Contract defaulted on payment obligations according to Delinquency Period.</t>
+    <t xml:space="preserve">option: 0, identifier: performant, name: Performant, accronym: PF, description: Contract is performing according to terms and conditions.
+option: 1, identifier: delayed, name: Delayed, accronym: DL, description: Contractual payment obligations are delayed according to the Grace Period.
+option: 2, identifier: delinquent, name: Delinquent, accronym: DQ, description: Contractual payment obligations are delinquent according to the Delinquency Period.
+option: 3, identifier: default, name: Default, accronym: DF, description: Contract defaulted on payment obligations according to Delinquency Period.</t>
   </si>
   <si>
     <t xml:space="preserve">PF</t>
@@ -940,8 +940,8 @@
     <t xml:space="preserve">SEN</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: s, name: Senior, description: Contract represents senior debt.
-option: 1, identifier: j, name: Junior, description: Contract represents junior debt.</t>
+    <t xml:space="preserve">option: 0, identifier: senior, name: Senior, accronym: S, description: Contract represents senior debt.
+option: 1, identifier: junior, name: Junior, accronym: J, description: Contract represents junior debt.</t>
   </si>
   <si>
     <t xml:space="preserve">Refers to the order of repayment in the event of a sale or default of the issuer. </t>
@@ -1031,9 +1031,9 @@
     <t xml:space="preserve">CEGE</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: no, name: Nominal Value, description: Nominal value of the exposure is covered.
-option: 1, identifier: ni, name: Nominal Value plus Interest, description: Nominal value of the exposure plus interest accrued is covered.
-option: 2, identifier: mv, name: Market Value, description: Market value of the exposure is covered.</t>
+    <t xml:space="preserve">option: 0, identifier: nominalValue, name: Nominal Value, accronym: NO, description: Nominal value of the exposure is covered.
+option: 1, identifier: nominalValuePlusInterest, name: Nominal Value plus Interest, accronym: NI, description: Nominal value of the exposure plus interest accrued is covered.
+option: 2, identifier: marketValue, name: Market Value, accronym: MV, description: Market value of the exposure is covered.</t>
   </si>
   <si>
     <t xml:space="preserve">Defines which value of the exposure is covered:
@@ -1069,9 +1069,9 @@
     <t xml:space="preserve">Enum[]</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: dl, name: Delayed, description: Delay of the underlying represents a credit event.
-option: 1, identifier: dq, name: Delinquent, description: Delinquency of the underlying represents a credit event.
-option: 2, identifier: df, name: Default, description: Default of the underlying represents a credit event.</t>
+    <t xml:space="preserve">option: 0, identifier: delayed, name: Delayed, accronym: DL, description: Delay of the underlying represents a credit event.
+option: 1, identifier: delinquent, name: Delinquent, accronym: DQ, description: Delinquency of the underlying represents a credit event.
+option: 2, identifier: default, name: Default, accronym: DF, description: Default of the underlying represents a credit event.</t>
   </si>
   <si>
     <t xml:space="preserve">DF</t>
@@ -1188,8 +1188,8 @@
     <t xml:space="preserve">FEB</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: a, name: Absolute Value, description: The fee rate represents an absolute value.
-option: 1, identifier: n, name: Nominal Value of the Underlying, description: The fee rate represents a rate that accrues fees on the basis of the nominal value of the underlying.</t>
+    <t xml:space="preserve">option: 0, identifier: absoluteValue, name: Absolute Value, accronym: A, description: The fee rate represents an absolute value.
+option: 1, identifier: nonimalValueOfTheUnderlying, name: Nominal Value of the Underlying, accronym: N, description: The fee rate represents a rate that accrues fees on the basis of the nominal value of the underlying.</t>
   </si>
   <si>
     <t xml:space="preserve">Basis, on which Fee is calculated. For FEB=’A’, FER is interpreted as an absolute amount to be paid at every FP event and for FEB=’N’, FER represents a rate at which FP amounts accrue on the basis of the contract’s NT.</t>
@@ -1372,12 +1372,12 @@
     <t xml:space="preserve">IPDC</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: aAISDA, name: Actual/Actual, description: Year fractions accrue on the basis of the actual number of days per month and per year in the respective period.
-option: 1, identifier: a360, name: Actual/360, description: Year fractions accrue on the basis of the actual number of days per month and 360 days per year in the respective period.
-option: 2, identifier: a365, name: Actual/365, description: Year fractions accrue on the basis of the actual number of days per month and 365 days per year in the respective period.
-option: 3, identifier: 30E360ISDA, name: 30E/360 ISDA, description: Year fractions accrue on the basis of 30 days per month and 360 days per year in the respective period (ISDA method).
-option: 4, identifier: 30E360, name: 30E/365, description: Year fractions accrue on the basis of 30 days per month and 360 days per year in the respective period.
-option: 5, identifier: 28E336, name: 28/336, description: Year fractions accrue on the basis of 28 days per month and 336 days per year in the respective period.</t>
+    <t xml:space="preserve">option: 0, identifier: actualActual, name: Actual/Actual, accronym: AA, description: Year fractions accrue on the basis of the actual number of days per month and per year in the respective period.
+option: 1, identifier: actualThreeSixty, name: Actual Three Sixty, accronym: A360, description: Year fractions accrue on the basis of the actual number of days per month and 360 days per year in the respective period.
+option: 2, identifier: actualThreeSixtyFive, name: Actual Three Sixty Five, accronym: A365, description: Year fractions accrue on the basis of the actual number of days per month and 365 days per year in the respective period.
+option: 3, identifier: thirtyEThreeSixtyISDA, name: Thirty E Three Sixty ISDA, accronym: 30E360ISDA, description: Year fractions accrue on the basis of 30 days per month and 360 days per year in the respective period (ISDA method).
+option: 4, identifier: thirtyEThreeSixty, name: Thirty E Three Sixty, accronym: 30E360, description: Year fractions accrue on the basis of 30 days per month and 360 days per year in the respective period.
+option: 5, identifier: twentyEightEThreeThirtySix, name: Twenty Eight E Three Thirty Six, accronym: 28E336, description: Year fractions accrue on the basis of 28 days per month and 336 days per year in the respective period.</t>
   </si>
   <si>
     <t xml:space="preserve">Method defining how days are counted between two dates. This finally defines the year fraction in accrual calculations.</t>
@@ -1444,9 +1444,9 @@
     <t xml:space="preserve">IPCB</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: nt, name: Notional Outstanding, description: Interest accrues on the basis of the notional outstanding.
-option: 1, identifier: ntied, name: Notional at Initial Exchange, description: Interest accrues on the basis of the notional value at initial exchange.
-option: 2, identifier: ntl, name: Notional Outstanding Lagged, description: Interest accrues on the basis of the lagged notional outstanding.</t>
+    <t xml:space="preserve">option: 0, identifier: notioalOutstanding, name: Notional Outstanding, accronym: NT, description: Interest accrues on the basis of the notional outstanding.
+option: 1, identifier: notionalAtInitialExchange, name: Notional at Initial Exchange, accronym: NTIED, description: Interest accrues on the basis of the notional value at initial exchange.
+option: 2, identifier: notionalLagged, name: Notional Outstanding Lagged, accronym: NTL, description: Interest accrues on the basis of the lagged notional outstanding.</t>
   </si>
   <si>
     <t xml:space="preserve">NT</t>
@@ -1484,8 +1484,8 @@
     <t xml:space="preserve">IPPNT</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: b, name: Beginning, description: Interest is paid upfront of the interest period.
-option: 1, identifier: e, name: End, description: Interest is paid at the end of the interest period.
+    <t xml:space="preserve">option: 0, identifier: beginning, name: Beginning, accronym: B, description: Interest is paid upfront of the interest period.
+option: 1, identifier: end, name: End, accronym: E, description: Interest is paid at the end of the interest period.
 </t>
   </si>
   <si>
@@ -1507,8 +1507,8 @@
     <t xml:space="preserve">MRCLH</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: y, name: Is Clearing House, description: Contract creator is the clearing house.
-option: 1, identifier: n, name: Is Not Clearing House, description: Contract creator is not the clearing house.</t>
+    <t xml:space="preserve">option: 0, identifier: isClearingHouse, name: Is Clearing House, accronym: Y, description: Contract creator is the clearing house.
+option: 1, identifier: isNotClearingHouse, name: Is Not Clearing House, accronym: N, description: Contract creator is not the clearing house.</t>
   </si>
   <si>
     <t xml:space="preserve">Indicates wheter CRID takes a clearing house function or not. In other word, whether CRID receive margins (MRIM, MRVM).</t>
@@ -1740,15 +1740,15 @@
     <t xml:space="preserve">UT</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: brl, name: Barrel, description: Physical unit of the contract is Barrels.
-option: 1, identifier: bsh, name: Bushel, description: Physical unit of the contract is Bushel.
-option: 2, identifier: gln, name: Gallon, description: Physical unit of the contract is Gallons.
-option: 3, identifier: cuu, name: Currency Unit, description: Physical unit of the contract is Currency Units.
-option: 4, identifier: mwh, name: Mega Watt Hours, description: Physical unit of the contract is Mega Watt Hours.
-option: 5, identifier: pnd, name: Pounds, description: Physical unit of the contract is Pounds.
-option: 6, identifier: stn, name: Short Tons, description: Physical unit of the contract is Short Tons.
-option: 7, identifier: ton, name: Tons, description: Physical unit of the contract is Tons.
-option: 8, identifier: tro, name: Troy Ounce, description: Physical unit of the contract is Troy Ounces.</t>
+    <t xml:space="preserve">option: 0, identifier: barrel, name: Barrel, accronym: BRL, description: Physical unit of the contract is Barrels.
+option: 1, identifier: bushel, name: Bushel, accronym: BSH, description: Physical unit of the contract is Bushel.
+option: 2, identifier: gallon, name: Gallon, accronym: GLN, description: Physical unit of the contract is Gallons.
+option: 3, identifier: currencyUnit, name: Currency Unit, accronym: CUU, description: Physical unit of the contract is Currency Units.
+option: 4, identifier: megaWattHours, name: Mega Watt Hours, accronym: MWH, description: Physical unit of the contract is Mega Watt Hours.
+option: 5, identifier: pounds, name: Pounds, accronym: PND, description: Physical unit of the contract is Pounds.
+option: 6, identifier: shortTons, name: Short Tons, accronym: STN, description: Physical unit of the contract is Short Tons.
+option: 7, identifier: tons, name: Tons, accronym: TON, description: Physical unit of the contract is Tons.
+option: 8, identifier: troyOunce, name: Troy Ounce, accronym: TRO, description: Physical unit of the contract is Troy Ounces.</t>
   </si>
   <si>
     <t xml:space="preserve">The physical unit of the contract. Example: Barrels for an Oil COM CT.</t>
@@ -1912,8 +1912,8 @@
     <t xml:space="preserve">ARINCDEC</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: inc, name: Increase, description: Notional is increased in this period.
-option: 1, identifier: dec, name: Decrease, description: Notional is decreased in this period.</t>
+    <t xml:space="preserve">option: 0, identifier: increase, name: Increase, accronym: INC, description: Notional is increased in this period.
+option: 1, identifier: decrease, name: Decrease, accronym: DEC, description: Notional is decreased in this period.</t>
   </si>
   <si>
     <t xml:space="preserve">Indicates whether a certain PRNXT element in ARPRNX increases the principal (NT) or decreases it.
@@ -2068,10 +2068,10 @@
     <t xml:space="preserve">SCEF</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: 000, name: No Scaling, description: No scaling applies.
-option: 1, identifier: i00, name: Interest is scaled, description: Scaling applies only to interest.
-option: 2, identifier: 0n0, name: Principal is scaled, description: Scaling applies only to principal.
-option: 3, identifier: in0, name: Interest and Principal is scaled, description: Scaling applies to interest and principal.
+    <t xml:space="preserve">option: 0, identifier: noScaling, name: No Scaling, accronym: 000, description: No scaling applies.
+option: 1, identifier: interestIsScaled, name: Interest is Scaled, accronym: I00, description: Scaling applies only to interest.
+option: 2, identifier: principalIsScaled, name: Principal is Scaled, accronym: 0N0, description: Scaling applies only to principal.
+option: 3, identifier: interestAndPrincipalIsScaled, name: Interest and Principal is Scaled, accronym: IN0, description: Scaling applies to interest and principal.
 </t>
   </si>
   <si>
@@ -2109,9 +2109,9 @@
     <t xml:space="preserve">OPXT</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: e, name: European, description: European-type exercise.
-option: 1, identifier: b, name: Bermudan, description: Bermudan-type exercise.
-option: 2, identifier: a, name: American, description: American-type exercise.</t>
+    <t xml:space="preserve">option: 0, identifier: european, name: European, accronym: E, description: European-type exercise.
+option: 1, identifier: bermudan, name: Bermudan, accronym: B, description: Bermudan-type exercise.
+option: 2, identifier: american, name: American, accronym: A, description: American-type exercise.</t>
   </si>
   <si>
     <t xml:space="preserve">Defines whether the option is European (exercised at a specific date), American (exercised during a span of time) or Bermudan (exercised at certain points during a span of time).</t>
@@ -2166,9 +2166,9 @@
     <t xml:space="preserve">OPTP</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: c, name: Call, description: Call option.
-option: 1, identifier: p, name: Put, description: Put option.
-option: 2, identifier: cp, name: Call-Put, description: Combination of call and put option.</t>
+    <t xml:space="preserve">option: 0, identifier: call, name: Call, accronym: C, description: Call option.
+option: 1, identifier: put, name: Put, accronym: P, description: Put option.
+option: 2, identifier: callPut, name: Call-Put, accronym: CP, description: Combination of call and put option.</t>
   </si>
   <si>
     <t xml:space="preserve">Defines whether the option is a call or put or a combination of it. This field has to be seen in combination with CNTRL where it is defined whether CRID is the buyer or the seller.</t>
@@ -2211,10 +2211,10 @@
     <t xml:space="preserve">PYTP</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: o, name: No Penalty, description: No penalty applies.
-option: 1, identifier: a, name: Fixed Penalty, description: A fixed amount applies as penalty.
-option: 2, identifier: n, name: Relative Penalty, description: A penalty relative to the notional outstanding applies.
-option: 3, identifier: i, name: Interest Rate Differential, description: A penalty based on the current interest rate differential relative to the notional outstanding applies.</t>
+    <t xml:space="preserve">option: 0, identifier: noPenalty, name: No Penalty, accronym: N, description: No penalty applies.
+option: 1, identifier: fixedPenalty, name: Fixed Penalty, accronym: A, description: A fixed amount applies as penalty.
+option: 2, identifier: relativePenalty, name: Relative Penalty, accronym: N, description: A penalty relative to the notional outstanding applies.
+option: 3, identifier: interestRateDifferential, name: Interest Rate Differential, accronym: I, description: A penalty based on the current interest rate differential relative to the notional outstanding applies.</t>
   </si>
   <si>
     <t xml:space="preserve">O</t>
@@ -2244,9 +2244,9 @@
     <t xml:space="preserve">PPEF</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: n, name: No Prepayment, description: Prepayment is not allowed under the agreement.
-option: 1, identifier: a, name: Prepayment reduces redemption amount, description: Prepayment is allowed and reduces the redemption amount for the remaining period up to maturity.
-option: 2, identifier: m, name: Prepayment reduces maturity, description: Prepayment is allowed and reduces the maturity.</t>
+    <t xml:space="preserve">option: 0, identifier: noPrepayment, name: No Prepayment, accronym: N, description: Prepayment is not allowed under the agreement.
+option: 1, identifier: prepaymentReducesRedemptionAmount, name: Prepayment Reduces Redemption Amount, accronym: A, description: Prepayment is allowed and reduces the redemption amount for the remaining period up to maturity.
+option: 2, identifier: prepaymentReducesMaturity, name: Prepayment Reduces Maturity, accronym: M, description: Prepayment is allowed and reduces the maturity.</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
@@ -2375,8 +2375,8 @@
     <t xml:space="preserve">ARFIXVAR</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: f, name: Fixed Rate, description: Rate spread represents a fixed rate.
-option: 1, identifier: v, name: Variable Rate, description: Rate spread represents the spread on top of a reference rate.</t>
+    <t xml:space="preserve">option: 0, identifier: fixedRate, name: Fixed Rate, accronym: F, description: Rate spread represents a fixed rate.
+option: 1, identifier: variableRate, name: Variable Rate, accronym: V, description: Rate spread represents the spread on top of a reference rate.</t>
   </si>
   <si>
     <t xml:space="preserve">For array-type rate reset schedules, this attributes defines the meaning of ARRATE.</t>
@@ -2454,8 +2454,8 @@
     <t xml:space="preserve">RRPNT</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: b, name: Beginning, description: The new rate is applied at the beginning of the reset period.
-option: 1, identifier: e, name: End, description: The new rate is applied at the end of the reset period.
+    <t xml:space="preserve">option: 0, identifier: beginning, name: Beginning, accronym: B, description: The new rate is applied at the beginning of the reset period.
+option: 1, identifier: end, name: End, accronym: E, description: The new rate is applied at the end of the reset period.
 </t>
   </si>
   <si>
@@ -2561,8 +2561,8 @@
     <t xml:space="preserve">DS</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: s, name: Cash Settlement, description: The market value of the underlying is settled.
-option: 1, identifier: d, name: Physical Settlement, description: The underlying is delivered physically.
+    <t xml:space="preserve">option: 0, identifier: cashSettlement, name: Cash Settlement, accronym: S, description: The market value of the underlying is settled.
+option: 1, identifier: physicalSettlement, name: Physical Settlement, accronym: D, description: The underlying is delivered physically.
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
fixed duplicate penaltyType acronym #17
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -2224,7 +2224,7 @@
   <si>
     <t xml:space="preserve">option: 0, identifier: noPenalty, name: No Penalty, acronym: N, description: No penalty applies.
 option: 1, identifier: fixedPenalty, name: Fixed Penalty, acronym: A, description: A fixed amount applies as penalty.
-option: 2, identifier: relativePenalty, name: Relative Penalty, acronym: N, description: A penalty relative to the notional outstanding applies.
+option: 2, identifier: relativePenalty, name: Relative Penalty, acronym: R, description: A penalty relative to the notional outstanding applies.
 option: 3, identifier: interestRateDifferential, name: Interest Rate Differential, acronym: I, description: A penalty based on the current interest rate differential relative to the notional outstanding applies.</t>
   </si>
   <si>
@@ -3580,7 +3580,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5576,10 +5576,10 @@
   </sheetPr>
   <dimension ref="A1:AA115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fixed big in generating contractType Enum options #16
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -770,7 +770,7 @@
 option: 7, identifier: cash, name: Cash, acronym: CSH, description: Represents cash holdings. 
 option: 8, identifier: stock, name: Stock, acronym: STK, description: Represents stocks/shares/equity. 
 option: 9, identifier: commodity, name: Commodity, acronym: COM, description: Represents commodities. 
-option: 10, identifier: swap, name: Swap, acronym: SWAPS, description: An agreement of swapping two legs such as fixed against variable, currency 1 against currency 2, etc. 
+option: 10, identifier: swap, name: Swap, acronym: SWAPS, description: An agreement of swapping two legs such as fixed against variable or currency 1 against currency 2 etc. 
 option: 11, identifier: plainVanillaSwap, name: Plain Vanilla Swap, acronym: SWPPV, description: Plain vanilla interest rate swaps. 
 option: 12, identifier: foreignExchangeOutright, name: Foreign Exchange Outright, acronym: FXOUT, description: An agreement of swapping two cash flows in different currencies at a future point in time. 
 option: 13, identifier: capFloor, name: Cap and Floor, acronym: CAPFL, description: An agreement of paying the differential (cap or floor) of a reference rate versus a fixed rate. 
@@ -3580,7 +3580,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5576,7 +5576,7 @@
   </sheetPr>
   <dimension ref="A1:AA115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>

</xml_diff>

<commit_message>
fixed interestCalculationBase -> interestCalculationBaseAmount state variable
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -2845,7 +2845,7 @@
     <t xml:space="preserve">The current value of accrued fees</t>
   </si>
   <si>
-    <t xml:space="preserve">ICB</t>
+    <t xml:space="preserve">ICBA</t>
   </si>
   <si>
     <t xml:space="preserve">The basis at which interest is being accrued. Potentially different from NVL.</t>
@@ -3039,7 +3039,7 @@
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="HH:MM:SS\ AM/PM"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3126,12 +3126,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <vertAlign val="subscript"/>
@@ -3239,7 +3233,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3344,19 +3338,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3376,11 +3362,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3388,7 +3374,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5445,9 +5431,9 @@
   <dimension ref="A1:AA115"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A43" activeCellId="0" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6593,7 +6579,7 @@
       <c r="E16" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="24" t="s">
         <v>299</v>
       </c>
       <c r="G16" s="20" t="s">
@@ -6652,7 +6638,7 @@
       <c r="E17" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="24" t="s">
         <v>299</v>
       </c>
       <c r="G17" s="20" t="s">
@@ -6725,7 +6711,7 @@
       <c r="E18" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F18" s="24" t="s">
         <v>299</v>
       </c>
       <c r="G18" s="20" t="s">
@@ -7061,7 +7047,7 @@
       <c r="E24" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="24" t="s">
         <v>344</v>
       </c>
       <c r="G24" s="22"/>
@@ -7259,7 +7245,7 @@
       <c r="E28" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F28" s="21" t="s">
         <v>344</v>
       </c>
       <c r="G28" s="22"/>
@@ -7593,7 +7579,7 @@
       <c r="E34" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="F34" s="27" t="s">
+      <c r="F34" s="21" t="s">
         <v>344</v>
       </c>
       <c r="G34" s="20"/>
@@ -7650,7 +7636,7 @@
       <c r="E35" s="19" t="s">
         <v>404</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="20"/>
       <c r="H35" s="22"/>
       <c r="I35" s="19" t="s">
@@ -8013,7 +7999,7 @@
       <c r="E42" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="F42" s="27" t="s">
+      <c r="F42" s="21" t="s">
         <v>344</v>
       </c>
       <c r="G42" s="22"/>
@@ -8452,7 +8438,7 @@
       <c r="E51" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="F51" s="27" t="s">
+      <c r="F51" s="21" t="s">
         <v>344</v>
       </c>
       <c r="G51" s="22"/>
@@ -8681,7 +8667,7 @@
       <c r="P55" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="Q55" s="28"/>
+      <c r="Q55" s="26"/>
       <c r="R55" s="22"/>
       <c r="S55" s="22"/>
       <c r="T55" s="22"/>
@@ -8816,7 +8802,7 @@
       <c r="Q57" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="R57" s="29"/>
+      <c r="R57" s="27"/>
       <c r="S57" s="22"/>
       <c r="T57" s="22"/>
       <c r="U57" s="22"/>
@@ -9146,7 +9132,7 @@
       <c r="O63" s="22"/>
       <c r="P63" s="22"/>
       <c r="Q63" s="22"/>
-      <c r="R63" s="30"/>
+      <c r="R63" s="28"/>
       <c r="S63" s="19" t="s">
         <v>241</v>
       </c>
@@ -9267,7 +9253,7 @@
       <c r="E66" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="F66" s="27" t="s">
+      <c r="F66" s="21" t="s">
         <v>344</v>
       </c>
       <c r="G66" s="20"/>
@@ -9786,7 +9772,7 @@
       <c r="E75" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="F75" s="26" t="s">
+      <c r="F75" s="24" t="s">
         <v>299</v>
       </c>
       <c r="G75" s="20"/>
@@ -9836,7 +9822,7 @@
       <c r="F76" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="G76" s="31"/>
+      <c r="G76" s="29"/>
       <c r="H76" s="23" t="s">
         <v>350</v>
       </c>
@@ -10039,7 +10025,7 @@
       <c r="E80" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="F80" s="27" t="s">
+      <c r="F80" s="21" t="s">
         <v>344</v>
       </c>
       <c r="G80" s="22"/>
@@ -10510,7 +10496,7 @@
       <c r="E89" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="F89" s="27" t="s">
+      <c r="F89" s="21" t="s">
         <v>344</v>
       </c>
       <c r="G89" s="22"/>
@@ -10879,7 +10865,7 @@
       <c r="E96" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="F96" s="27" t="s">
+      <c r="F96" s="21" t="s">
         <v>344</v>
       </c>
       <c r="G96" s="20"/>
@@ -11446,7 +11432,7 @@
       <c r="E107" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="F107" s="26" t="s">
+      <c r="F107" s="24" t="s">
         <v>299</v>
       </c>
       <c r="G107" s="20" t="s">
@@ -11723,7 +11709,7 @@
       <c r="E112" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="F112" s="27" t="s">
+      <c r="F112" s="21" t="s">
         <v>299</v>
       </c>
       <c r="G112" s="20" t="s">
@@ -11970,36 +11956,36 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="32"/>
+      <c r="A1" s="30"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10"/>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="30" t="s">
         <v>780</v>
       </c>
       <c r="C2" s="10"/>
@@ -12022,10 +12008,10 @@
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
       <c r="V2" s="10"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30"/>
+      <c r="Z2" s="30"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10"/>
@@ -12050,40 +12036,40 @@
       <c r="T3" s="10"/>
       <c r="U3" s="10"/>
       <c r="V3" s="10"/>
-      <c r="W3" s="32"/>
-      <c r="X3" s="32"/>
-      <c r="Y3" s="32"/>
-      <c r="Z3" s="32"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="30"/>
+      <c r="Y3" s="30"/>
+      <c r="Z3" s="30"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32" t="s">
+      <c r="A4" s="30"/>
+      <c r="B4" s="30" t="s">
         <v>781</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="32"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10"/>
@@ -12109,46 +12095,46 @@
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
-      <c r="X5" s="32"/>
-      <c r="Y5" s="32"/>
-      <c r="Z5" s="32"/>
+      <c r="X5" s="30"/>
+      <c r="Y5" s="30"/>
+      <c r="Z5" s="30"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32" t="s">
+      <c r="A6" s="30"/>
+      <c r="B6" s="30" t="s">
         <v>782</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="30" t="s">
         <v>783</v>
       </c>
       <c r="D6" s="10"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
-      <c r="T6" s="32"/>
-      <c r="U6" s="32"/>
-      <c r="V6" s="32"/>
-      <c r="W6" s="32"/>
-      <c r="X6" s="32"/>
-      <c r="Y6" s="32"/>
-      <c r="Z6" s="32"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
+      <c r="T6" s="30"/>
+      <c r="U6" s="30"/>
+      <c r="V6" s="30"/>
+      <c r="W6" s="30"/>
+      <c r="X6" s="30"/>
+      <c r="Y6" s="30"/>
+      <c r="Z6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="30" t="s">
         <v>784</v>
       </c>
       <c r="D7" s="10"/>
@@ -12171,9 +12157,9 @@
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
-      <c r="X7" s="32"/>
-      <c r="Y7" s="32"/>
-      <c r="Z7" s="32"/>
+      <c r="X7" s="30"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10"/>
@@ -12199,50 +12185,50 @@
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
-      <c r="X8" s="32"/>
-      <c r="Y8" s="32"/>
-      <c r="Z8" s="32"/>
+      <c r="X8" s="30"/>
+      <c r="Y8" s="30"/>
+      <c r="Z8" s="30"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="30" t="s">
         <v>785</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="30" t="s">
         <v>786</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="32"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="32"/>
-      <c r="V9" s="32"/>
-      <c r="W9" s="32"/>
-      <c r="X9" s="32"/>
-      <c r="Y9" s="32"/>
-      <c r="Z9" s="32"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+      <c r="T9" s="30"/>
+      <c r="U9" s="30"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="30"/>
+      <c r="X9" s="30"/>
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="30"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="30" t="s">
         <v>787</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="30" t="s">
         <v>788</v>
       </c>
       <c r="F10" s="10"/>
@@ -12265,7 +12251,7 @@
       <c r="W10" s="10"/>
       <c r="X10" s="10"/>
       <c r="Y10" s="10"/>
-      <c r="Z10" s="32"/>
+      <c r="Z10" s="30"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
@@ -12293,11 +12279,11 @@
       <c r="W11" s="10"/>
       <c r="X11" s="10"/>
       <c r="Y11" s="10"/>
-      <c r="Z11" s="32"/>
+      <c r="Z11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="30" t="s">
         <v>789</v>
       </c>
       <c r="C12" s="10"/>
@@ -12325,42 +12311,42 @@
       <c r="W12" s="10"/>
       <c r="X12" s="10"/>
       <c r="Y12" s="10"/>
-      <c r="Z12" s="32"/>
+      <c r="Z12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="32"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="32"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="30"/>
+      <c r="Y13" s="30"/>
+      <c r="Z13" s="30"/>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="30" t="s">
         <v>791</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="30" t="s">
         <v>792</v>
       </c>
       <c r="D14" s="10"/>
@@ -12387,7 +12373,7 @@
       <c r="W14" s="10"/>
       <c r="X14" s="10"/>
       <c r="Y14" s="10"/>
-      <c r="Z14" s="32"/>
+      <c r="Z14" s="30"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="10"/>
@@ -12415,13 +12401,13 @@
       <c r="W15" s="10"/>
       <c r="X15" s="10"/>
       <c r="Y15" s="10"/>
-      <c r="Z15" s="32"/>
+      <c r="Z15" s="30"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="30" t="s">
         <v>794</v>
       </c>
       <c r="E16" s="21" t="s">
@@ -12447,13 +12433,13 @@
       <c r="W16" s="10"/>
       <c r="X16" s="10"/>
       <c r="Y16" s="10"/>
-      <c r="Z16" s="32"/>
+      <c r="Z16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="30" t="s">
         <v>796</v>
       </c>
       <c r="E17" s="21" t="s">
@@ -12479,13 +12465,13 @@
       <c r="W17" s="10"/>
       <c r="X17" s="10"/>
       <c r="Y17" s="10"/>
-      <c r="Z17" s="32"/>
+      <c r="Z17" s="30"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="30" t="s">
         <v>798</v>
       </c>
       <c r="E18" s="21" t="s">
@@ -12511,7 +12497,7 @@
       <c r="W18" s="10"/>
       <c r="X18" s="10"/>
       <c r="Y18" s="10"/>
-      <c r="Z18" s="32"/>
+      <c r="Z18" s="30"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10"/>
@@ -12539,12 +12525,12 @@
       <c r="W19" s="10"/>
       <c r="X19" s="10"/>
       <c r="Y19" s="10"/>
-      <c r="Z19" s="32"/>
+      <c r="Z19" s="30"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="30" t="s">
         <v>800</v>
       </c>
       <c r="D20" s="10"/>
@@ -12571,7 +12557,7 @@
       <c r="W20" s="10"/>
       <c r="X20" s="10"/>
       <c r="Y20" s="10"/>
-      <c r="Z20" s="32"/>
+      <c r="Z20" s="30"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10"/>
@@ -12599,13 +12585,13 @@
       <c r="W21" s="10"/>
       <c r="X21" s="10"/>
       <c r="Y21" s="10"/>
-      <c r="Z21" s="32"/>
+      <c r="Z21" s="30"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="30" t="s">
         <v>794</v>
       </c>
       <c r="E22" s="21" t="s">
@@ -12631,13 +12617,13 @@
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
       <c r="Y22" s="10"/>
-      <c r="Z22" s="32"/>
+      <c r="Z22" s="30"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="30" t="s">
         <v>803</v>
       </c>
       <c r="E23" s="21" t="s">
@@ -12663,40 +12649,40 @@
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
       <c r="Y23" s="10"/>
-      <c r="Z23" s="32"/>
+      <c r="Z23" s="30"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="32"/>
+      <c r="A24" s="30"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="32"/>
-      <c r="S24" s="32"/>
-      <c r="T24" s="32"/>
-      <c r="U24" s="32"/>
-      <c r="V24" s="32"/>
-      <c r="W24" s="32"/>
-      <c r="X24" s="32"/>
-      <c r="Y24" s="32"/>
-      <c r="Z24" s="32"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="30"/>
+      <c r="K24" s="30"/>
+      <c r="L24" s="30"/>
+      <c r="M24" s="30"/>
+      <c r="N24" s="30"/>
+      <c r="O24" s="30"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="30"/>
+      <c r="W24" s="30"/>
+      <c r="X24" s="30"/>
+      <c r="Y24" s="30"/>
+      <c r="Z24" s="30"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="30" t="s">
         <v>805</v>
       </c>
       <c r="D25" s="10"/>
@@ -12723,41 +12709,41 @@
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
-      <c r="Z25" s="32"/>
+      <c r="Z25" s="30"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="32"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="32"/>
-      <c r="Q26" s="32"/>
-      <c r="R26" s="32"/>
-      <c r="S26" s="32"/>
-      <c r="T26" s="32"/>
-      <c r="U26" s="32"/>
-      <c r="V26" s="32"/>
-      <c r="W26" s="32"/>
-      <c r="X26" s="32"/>
-      <c r="Y26" s="32"/>
-      <c r="Z26" s="32"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="30"/>
+      <c r="T26" s="30"/>
+      <c r="U26" s="30"/>
+      <c r="V26" s="30"/>
+      <c r="W26" s="30"/>
+      <c r="X26" s="30"/>
+      <c r="Y26" s="30"/>
+      <c r="Z26" s="30"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="31" t="s">
         <v>807</v>
       </c>
       <c r="E27" s="21" t="s">
@@ -12783,13 +12769,13 @@
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
       <c r="Y27" s="10"/>
-      <c r="Z27" s="32"/>
+      <c r="Z27" s="30"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="31" t="s">
         <v>809</v>
       </c>
       <c r="E28" s="21" t="s">
@@ -12815,13 +12801,13 @@
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
       <c r="Y28" s="10"/>
-      <c r="Z28" s="32"/>
+      <c r="Z28" s="30"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="31" t="s">
         <v>811</v>
       </c>
       <c r="E29" s="21" t="s">
@@ -12847,13 +12833,13 @@
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
       <c r="Y29" s="10"/>
-      <c r="Z29" s="32"/>
+      <c r="Z29" s="30"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
-      <c r="D30" s="33" t="s">
+      <c r="D30" s="31" t="s">
         <v>813</v>
       </c>
       <c r="E30" s="21" t="s">
@@ -12879,13 +12865,13 @@
       <c r="W30" s="10"/>
       <c r="X30" s="10"/>
       <c r="Y30" s="10"/>
-      <c r="Z30" s="32"/>
+      <c r="Z30" s="30"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="31" t="s">
         <v>815</v>
       </c>
       <c r="E31" s="21" t="s">
@@ -12911,40 +12897,40 @@
       <c r="W31" s="10"/>
       <c r="X31" s="10"/>
       <c r="Y31" s="10"/>
-      <c r="Z31" s="32"/>
+      <c r="Z31" s="30"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="32"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="32"/>
-      <c r="N32" s="32"/>
-      <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="32"/>
-      <c r="R32" s="32"/>
-      <c r="S32" s="32"/>
-      <c r="T32" s="32"/>
-      <c r="U32" s="32"/>
-      <c r="V32" s="32"/>
-      <c r="W32" s="32"/>
-      <c r="X32" s="32"/>
-      <c r="Y32" s="32"/>
-      <c r="Z32" s="32"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="30"/>
+      <c r="T32" s="30"/>
+      <c r="U32" s="30"/>
+      <c r="V32" s="30"/>
+      <c r="W32" s="30"/>
+      <c r="X32" s="30"/>
+      <c r="Y32" s="30"/>
+      <c r="Z32" s="30"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="30" t="s">
         <v>817</v>
       </c>
       <c r="D33" s="10"/>
@@ -12971,41 +12957,41 @@
       <c r="W33" s="10"/>
       <c r="X33" s="10"/>
       <c r="Y33" s="10"/>
-      <c r="Z33" s="32"/>
+      <c r="Z33" s="30"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="32"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
       <c r="D34" s="10"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-      <c r="M34" s="32"/>
-      <c r="N34" s="32"/>
-      <c r="O34" s="32"/>
-      <c r="P34" s="32"/>
-      <c r="Q34" s="32"/>
-      <c r="R34" s="32"/>
-      <c r="S34" s="32"/>
-      <c r="T34" s="32"/>
-      <c r="U34" s="32"/>
-      <c r="V34" s="32"/>
-      <c r="W34" s="32"/>
-      <c r="X34" s="32"/>
-      <c r="Y34" s="32"/>
-      <c r="Z34" s="32"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+      <c r="L34" s="30"/>
+      <c r="M34" s="30"/>
+      <c r="N34" s="30"/>
+      <c r="O34" s="30"/>
+      <c r="P34" s="30"/>
+      <c r="Q34" s="30"/>
+      <c r="R34" s="30"/>
+      <c r="S34" s="30"/>
+      <c r="T34" s="30"/>
+      <c r="U34" s="30"/>
+      <c r="V34" s="30"/>
+      <c r="W34" s="30"/>
+      <c r="X34" s="30"/>
+      <c r="Y34" s="30"/>
+      <c r="Z34" s="30"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
-      <c r="D35" s="32" t="s">
+      <c r="D35" s="30" t="s">
         <v>794</v>
       </c>
       <c r="E35" s="21" t="s">
@@ -13031,13 +13017,13 @@
       <c r="W35" s="10"/>
       <c r="X35" s="10"/>
       <c r="Y35" s="10"/>
-      <c r="Z35" s="32"/>
+      <c r="Z35" s="30"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="32" t="s">
+      <c r="D36" s="30" t="s">
         <v>820</v>
       </c>
       <c r="E36" s="21" t="s">
@@ -13063,13 +13049,13 @@
       <c r="W36" s="10"/>
       <c r="X36" s="10"/>
       <c r="Y36" s="10"/>
-      <c r="Z36" s="32"/>
+      <c r="Z36" s="30"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
-      <c r="D37" s="32" t="s">
+      <c r="D37" s="30" t="s">
         <v>822</v>
       </c>
       <c r="E37" s="21" t="s">
@@ -13095,13 +13081,13 @@
       <c r="W37" s="10"/>
       <c r="X37" s="10"/>
       <c r="Y37" s="10"/>
-      <c r="Z37" s="32"/>
+      <c r="Z37" s="30"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="30" t="s">
         <v>824</v>
       </c>
       <c r="E38" s="21" t="s">
@@ -13127,13 +13113,13 @@
       <c r="W38" s="10"/>
       <c r="X38" s="10"/>
       <c r="Y38" s="10"/>
-      <c r="Z38" s="32"/>
+      <c r="Z38" s="30"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="30" t="s">
         <v>826</v>
       </c>
       <c r="E39" s="21" t="s">
@@ -13159,7 +13145,7 @@
       <c r="W39" s="10"/>
       <c r="X39" s="10"/>
       <c r="Y39" s="10"/>
-      <c r="Z39" s="32"/>
+      <c r="Z39" s="30"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10"/>
@@ -13187,7 +13173,7 @@
       <c r="W40" s="10"/>
       <c r="X40" s="10"/>
       <c r="Y40" s="10"/>
-      <c r="Z40" s="32"/>
+      <c r="Z40" s="30"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10"/>
@@ -13219,7 +13205,7 @@
       <c r="W41" s="10"/>
       <c r="X41" s="10"/>
       <c r="Y41" s="10"/>
-      <c r="Z41" s="32"/>
+      <c r="Z41" s="30"/>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10"/>
@@ -13247,16 +13233,16 @@
       <c r="W42" s="10"/>
       <c r="X42" s="10"/>
       <c r="Y42" s="10"/>
-      <c r="Z42" s="32"/>
+      <c r="Z42" s="30"/>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
-      <c r="D43" s="32" t="s">
+      <c r="D43" s="30" t="s">
         <v>794</v>
       </c>
-      <c r="E43" s="32" t="s">
+      <c r="E43" s="30" t="s">
         <v>830</v>
       </c>
       <c r="F43" s="10"/>
@@ -13279,13 +13265,13 @@
       <c r="W43" s="10"/>
       <c r="X43" s="10"/>
       <c r="Y43" s="10"/>
-      <c r="Z43" s="32"/>
+      <c r="Z43" s="30"/>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
-      <c r="D44" s="33" t="s">
+      <c r="D44" s="31" t="s">
         <v>831</v>
       </c>
       <c r="E44" s="21" t="s">
@@ -13311,13 +13297,13 @@
       <c r="W44" s="10"/>
       <c r="X44" s="10"/>
       <c r="Y44" s="10"/>
-      <c r="Z44" s="32"/>
+      <c r="Z44" s="30"/>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
-      <c r="D45" s="32" t="s">
+      <c r="D45" s="30" t="s">
         <v>833</v>
       </c>
       <c r="E45" s="19" t="s">
@@ -13343,129 +13329,129 @@
       <c r="W45" s="10"/>
       <c r="X45" s="10"/>
       <c r="Y45" s="10"/>
-      <c r="Z45" s="32"/>
+      <c r="Z45" s="30"/>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="32"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32"/>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="32"/>
-      <c r="O46" s="32"/>
-      <c r="P46" s="32"/>
-      <c r="Q46" s="32"/>
-      <c r="R46" s="32"/>
-      <c r="S46" s="32"/>
-      <c r="T46" s="32"/>
-      <c r="U46" s="32"/>
-      <c r="V46" s="32"/>
-      <c r="W46" s="32"/>
-      <c r="X46" s="32"/>
-      <c r="Y46" s="32"/>
-      <c r="Z46" s="32"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
+      <c r="K46" s="30"/>
+      <c r="L46" s="30"/>
+      <c r="M46" s="30"/>
+      <c r="N46" s="30"/>
+      <c r="O46" s="30"/>
+      <c r="P46" s="30"/>
+      <c r="Q46" s="30"/>
+      <c r="R46" s="30"/>
+      <c r="S46" s="30"/>
+      <c r="T46" s="30"/>
+      <c r="U46" s="30"/>
+      <c r="V46" s="30"/>
+      <c r="W46" s="30"/>
+      <c r="X46" s="30"/>
+      <c r="Y46" s="30"/>
+      <c r="Z46" s="30"/>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="32"/>
-      <c r="B47" s="32" t="s">
+      <c r="A47" s="30"/>
+      <c r="B47" s="30" t="s">
         <v>835</v>
       </c>
-      <c r="C47" s="32" t="s">
+      <c r="C47" s="30" t="s">
         <v>836</v>
       </c>
-      <c r="D47" s="32"/>
+      <c r="D47" s="30"/>
       <c r="E47" s="21" t="s">
         <v>837</v>
       </c>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="32"/>
-      <c r="M47" s="32"/>
-      <c r="N47" s="32"/>
-      <c r="O47" s="32"/>
-      <c r="P47" s="32"/>
-      <c r="Q47" s="32"/>
-      <c r="R47" s="32"/>
-      <c r="S47" s="32"/>
-      <c r="T47" s="32"/>
-      <c r="U47" s="32"/>
-      <c r="V47" s="32"/>
-      <c r="W47" s="32"/>
-      <c r="X47" s="32"/>
-      <c r="Y47" s="32"/>
-      <c r="Z47" s="32"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="30"/>
+      <c r="L47" s="30"/>
+      <c r="M47" s="30"/>
+      <c r="N47" s="30"/>
+      <c r="O47" s="30"/>
+      <c r="P47" s="30"/>
+      <c r="Q47" s="30"/>
+      <c r="R47" s="30"/>
+      <c r="S47" s="30"/>
+      <c r="T47" s="30"/>
+      <c r="U47" s="30"/>
+      <c r="V47" s="30"/>
+      <c r="W47" s="30"/>
+      <c r="X47" s="30"/>
+      <c r="Y47" s="30"/>
+      <c r="Z47" s="30"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="32"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="21" t="s">
         <v>838</v>
       </c>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
-      <c r="I48" s="32"/>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="32"/>
-      <c r="N48" s="32"/>
-      <c r="O48" s="32"/>
-      <c r="P48" s="32"/>
-      <c r="Q48" s="32"/>
-      <c r="R48" s="32"/>
-      <c r="S48" s="32"/>
-      <c r="T48" s="32"/>
-      <c r="U48" s="32"/>
-      <c r="V48" s="32"/>
-      <c r="W48" s="32"/>
-      <c r="X48" s="32"/>
-      <c r="Y48" s="32"/>
-      <c r="Z48" s="32"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="30"/>
+      <c r="J48" s="30"/>
+      <c r="K48" s="30"/>
+      <c r="L48" s="30"/>
+      <c r="M48" s="30"/>
+      <c r="N48" s="30"/>
+      <c r="O48" s="30"/>
+      <c r="P48" s="30"/>
+      <c r="Q48" s="30"/>
+      <c r="R48" s="30"/>
+      <c r="S48" s="30"/>
+      <c r="T48" s="30"/>
+      <c r="U48" s="30"/>
+      <c r="V48" s="30"/>
+      <c r="W48" s="30"/>
+      <c r="X48" s="30"/>
+      <c r="Y48" s="30"/>
+      <c r="Z48" s="30"/>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="32"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
       <c r="E49" s="21" t="s">
         <v>839</v>
       </c>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="32"/>
-      <c r="M49" s="32"/>
-      <c r="N49" s="32"/>
-      <c r="O49" s="32"/>
-      <c r="P49" s="32"/>
-      <c r="Q49" s="32"/>
-      <c r="R49" s="32"/>
-      <c r="S49" s="32"/>
-      <c r="T49" s="32"/>
-      <c r="U49" s="32"/>
-      <c r="V49" s="32"/>
-      <c r="W49" s="32"/>
-      <c r="X49" s="32"/>
-      <c r="Y49" s="32"/>
-      <c r="Z49" s="32"/>
+      <c r="F49" s="30"/>
+      <c r="G49" s="30"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="30"/>
+      <c r="J49" s="30"/>
+      <c r="K49" s="30"/>
+      <c r="L49" s="30"/>
+      <c r="M49" s="30"/>
+      <c r="N49" s="30"/>
+      <c r="O49" s="30"/>
+      <c r="P49" s="30"/>
+      <c r="Q49" s="30"/>
+      <c r="R49" s="30"/>
+      <c r="S49" s="30"/>
+      <c r="T49" s="30"/>
+      <c r="U49" s="30"/>
+      <c r="V49" s="30"/>
+      <c r="W49" s="30"/>
+      <c r="X49" s="30"/>
+      <c r="Y49" s="30"/>
+      <c r="Z49" s="30"/>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -14437,7 +14423,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14450,22 +14436,22 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="32" t="s">
         <v>203</v>
       </c>
     </row>
@@ -14650,10 +14636,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>853</v>
@@ -14826,22 +14812,22 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="32" t="s">
         <v>203</v>
       </c>
     </row>
@@ -14861,7 +14847,7 @@
       <c r="E2" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="33" t="s">
         <v>246</v>
       </c>
     </row>
@@ -14881,7 +14867,7 @@
       <c r="E3" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="33" t="s">
         <v>246</v>
       </c>
     </row>
@@ -14901,7 +14887,7 @@
       <c r="E4" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="34" t="s">
         <v>881</v>
       </c>
     </row>
@@ -15019,22 +15005,22 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="32" t="s">
         <v>203</v>
       </c>
     </row>
@@ -15071,7 +15057,7 @@
       <c r="E3" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="35" t="s">
         <v>899</v>
       </c>
     </row>
@@ -15091,7 +15077,7 @@
       <c r="E4" s="0" t="s">
         <v>218</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="35" t="s">
         <v>904</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed cycle format definition
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -1138,7 +1138,7 @@
     <t xml:space="preserve">Cycle</t>
   </si>
   <si>
-    <t xml:space="preserve">[ISO8601 Duration]I[s={‘+’,’-’}]</t>
+    <t xml:space="preserve">[ISO8601 Duration]L[s={‘+’,’-’}]</t>
   </si>
   <si>
     <t xml:space="preserve">Defines in combination with DVANX the payment points of dividends. The dividend payment schedule will start at DVANX and end at MaximumProjectionPeriod (cf. sheet Modeling Parameters).</t>
@@ -3401,7 +3401,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5441,10 +5441,10 @@
   </sheetPr>
   <dimension ref="A1:AA115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7256,7 +7256,7 @@
       <c r="E28" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F28" s="24" t="s">
         <v>346</v>
       </c>
       <c r="G28" s="22"/>
@@ -7590,7 +7590,7 @@
       <c r="E34" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="F34" s="24" t="s">
         <v>346</v>
       </c>
       <c r="G34" s="20"/>
@@ -8010,7 +8010,7 @@
       <c r="E42" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="F42" s="21" t="s">
+      <c r="F42" s="24" t="s">
         <v>346</v>
       </c>
       <c r="G42" s="22"/>
@@ -8449,7 +8449,7 @@
       <c r="E51" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="F51" s="24" t="s">
         <v>346</v>
       </c>
       <c r="G51" s="22"/>
@@ -9264,7 +9264,7 @@
       <c r="E66" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="F66" s="21" t="s">
+      <c r="F66" s="24" t="s">
         <v>346</v>
       </c>
       <c r="G66" s="20"/>
@@ -10036,7 +10036,7 @@
       <c r="E80" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="F80" s="21" t="s">
+      <c r="F80" s="24" t="s">
         <v>346</v>
       </c>
       <c r="G80" s="22"/>
@@ -10507,7 +10507,7 @@
       <c r="E89" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="F89" s="21" t="s">
+      <c r="F89" s="24" t="s">
         <v>346</v>
       </c>
       <c r="G89" s="22"/>
@@ -10876,7 +10876,7 @@
       <c r="E96" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="F96" s="21" t="s">
+      <c r="F96" s="24" t="s">
         <v>346</v>
       </c>
       <c r="G96" s="20"/>
@@ -14434,7 +14434,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
streamlined cycle stub format
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -1138,7 +1138,7 @@
     <t xml:space="preserve">Cycle</t>
   </si>
   <si>
-    <t xml:space="preserve">[ISO8601 Duration]L[s={‘+’,’-’}]</t>
+    <t xml:space="preserve">[ISO8601 Duration]L[s={0,1}]</t>
   </si>
   <si>
     <t xml:space="preserve">Defines in combination with DVANX the payment points of dividends. The dividend payment schedule will start at DVANX and end at MaximumProjectionPeriod (cf. sheet Modeling Parameters).</t>
@@ -3401,7 +3401,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5441,10 +5441,10 @@
   </sheetPr>
   <dimension ref="A1:AA115"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
added contractID to the event object
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2055" uniqueCount="891">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2060" uniqueCount="893">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -2946,6 +2946,12 @@
   </si>
   <si>
     <t xml:space="preserve">The post-event state. Results from applying the event’s state transition function to the pre-event state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contract ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Contract ID of the contract which created the event.</t>
   </si>
   <si>
     <t xml:space="preserve">object</t>
@@ -14637,7 +14643,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14782,6 +14788,23 @@
       </c>
       <c r="E7" s="0" t="s">
         <v>874</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>877</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>878</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -14865,16 +14888,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>244</v>
@@ -14882,42 +14905,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>205</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>205</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
fixed prnxt state accronym
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2060" uniqueCount="893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2060" uniqueCount="892">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -2841,9 +2841,6 @@
   </si>
   <si>
     <t xml:space="preserve">The multiplier being applied to interest cash flows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NPR</t>
   </si>
   <si>
     <t xml:space="preserve">The value at which principal is being repaid. This may be including or excluding of interest depending on the Contract Type</t>
@@ -14538,10 +14535,10 @@
         <v>542</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>849</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>850</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>301</v>
@@ -14558,7 +14555,7 @@
         <v>741</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>232</v>
@@ -14578,7 +14575,7 @@
         <v>746</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>301</v>
@@ -14595,7 +14592,7 @@
         <v>567</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>232</v>
@@ -14615,7 +14612,7 @@
         <v>502</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>232</v>
@@ -14678,16 +14675,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>855</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>856</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>857</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>858</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>232</v>
@@ -14698,16 +14695,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>859</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>860</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>861</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>862</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>232</v>
@@ -14718,22 +14715,22 @@
     </row>
     <row r="4" customFormat="false" ht="249" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>863</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>864</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>865</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>866</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>205</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14747,7 +14744,7 @@
         <v>476</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>244</v>
@@ -14758,16 +14755,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>869</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>870</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>871</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>872</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>301</v>
@@ -14775,19 +14772,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>872</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>873</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>874</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>875</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>876</v>
-      </c>
       <c r="E7" s="0" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14795,13 +14792,13 @@
         <v>247</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>249</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>244</v>
@@ -14888,16 +14885,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>878</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>879</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>880</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>881</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>882</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>244</v>
@@ -14905,42 +14902,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>882</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>883</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>884</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>885</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>886</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>205</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>887</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>888</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>889</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>890</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>891</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>205</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
added missing scaling multiplier terms
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,8 +17,8 @@
     <sheet name="ContractStructure" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Terms!$T$1:$T$115</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="Z_29585F7E_9463_4993_8067_5C2E42B28159_.wvu.FilterData" vbProcedure="false">Terms!$T$1:$T$115</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Terms!$T$1:$T$117</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="Z_29585F7E_9463_4993_8067_5C2E42B28159_.wvu.FilterData" vbProcedure="false">Terms!$T$1:$T$117</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2060" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="893">
   <si>
     <t xml:space="preserve">The ACTUS Dictionary</t>
   </si>
@@ -2020,13 +2020,40 @@
     <t xml:space="preserve">NN(7,1,)</t>
   </si>
   <si>
-    <t xml:space="preserve">scalingIndexAtStatusDate </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scaling Index At Status Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCIED</t>
+    <t xml:space="preserve">scalingIndexAtContractDealDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scaling Index At Contract Deal Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCCDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The value of the Scaling Index as per Contract Deal Date.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notionalScalingMultiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notional Scaling Multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The multiplier being applied to principal cash flows</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interestScalingMultiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interest Scaling Multiplier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The multiplier being applied to interest cash flows</t>
   </si>
   <si>
     <t xml:space="preserve">cycleAnchorDateOfScalingIndex</t>
@@ -2817,30 +2844,6 @@
   </si>
   <si>
     <t xml:space="preserve">The basis at which interest is being accrued. Potentially different from NVL.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notionalScalingMultiplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notional Scaling Multiplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NSC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The multiplier being applied to principal cash flows</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interestScalingMultiplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interest Scaling Multiplier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The multiplier being applied to interest cash flows</t>
   </si>
   <si>
     <t xml:space="preserve">The value at which principal is being repaid. This may be including or excluding of interest depending on the Contract Type</t>
@@ -3372,7 +3375,7 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -5270,9 +5273,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AA115"/>
+  <dimension ref="A1:AA117"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -9763,12 +9766,12 @@
       <c r="E78" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="F78" s="21" t="s">
-        <v>302</v>
-      </c>
+      <c r="F78" s="21"/>
       <c r="G78" s="22"/>
       <c r="H78" s="22"/>
-      <c r="I78" s="22"/>
+      <c r="I78" s="22" t="s">
+        <v>590</v>
+      </c>
       <c r="J78" s="22"/>
       <c r="K78" s="22"/>
       <c r="L78" s="22"/>
@@ -9800,45 +9803,45 @@
     </row>
     <row r="79" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="19" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B79" s="19" t="s">
         <v>474</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D79" s="19" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E79" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="F79" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="G79" s="22"/>
+        <v>301</v>
+      </c>
+      <c r="F79" s="21"/>
+      <c r="G79" s="22" t="n">
+        <v>1</v>
+      </c>
       <c r="H79" s="22"/>
-      <c r="I79" s="19" t="s">
-        <v>593</v>
+      <c r="I79" s="10" t="s">
+        <v>594</v>
       </c>
       <c r="J79" s="22"/>
       <c r="K79" s="22"/>
       <c r="L79" s="22"/>
       <c r="M79" s="19" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="N79" s="19" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="O79" s="19" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="P79" s="19" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="Q79" s="19" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="R79" s="22"/>
       <c r="S79" s="22"/>
@@ -9865,33 +9868,33 @@
         <v>597</v>
       </c>
       <c r="E80" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="F80" s="24" t="s">
-        <v>331</v>
-      </c>
-      <c r="G80" s="22"/>
+        <v>301</v>
+      </c>
+      <c r="F80" s="21"/>
+      <c r="G80" s="22" t="n">
+        <v>1</v>
+      </c>
       <c r="H80" s="22"/>
-      <c r="I80" s="19" t="s">
+      <c r="I80" s="10" t="s">
         <v>598</v>
       </c>
       <c r="J80" s="22"/>
       <c r="K80" s="22"/>
       <c r="L80" s="22"/>
       <c r="M80" s="19" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="N80" s="19" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="O80" s="19" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="P80" s="19" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="Q80" s="19" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="R80" s="22"/>
       <c r="S80" s="22"/>
@@ -9918,35 +9921,33 @@
         <v>601</v>
       </c>
       <c r="E81" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="F81" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="F81" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="G81" s="22"/>
+      <c r="H81" s="22"/>
+      <c r="I81" s="19" t="s">
         <v>602</v>
-      </c>
-      <c r="G81" s="20" t="s">
-        <v>603</v>
-      </c>
-      <c r="H81" s="21"/>
-      <c r="I81" s="19" t="s">
-        <v>604</v>
       </c>
       <c r="J81" s="22"/>
       <c r="K81" s="22"/>
       <c r="L81" s="22"/>
       <c r="M81" s="19" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="N81" s="19" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="O81" s="19" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="P81" s="19" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="Q81" s="19" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="R81" s="22"/>
       <c r="S81" s="22"/>
@@ -9961,226 +9962,232 @@
     </row>
     <row r="82" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="19" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="B82" s="19" t="s">
         <v>474</v>
       </c>
       <c r="C82" s="19" t="s">
+        <v>605</v>
+      </c>
+      <c r="D82" s="19" t="s">
+        <v>606</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="F82" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="G82" s="22"/>
+      <c r="H82" s="22"/>
+      <c r="I82" s="19" t="s">
         <v>607</v>
-      </c>
-      <c r="D82" s="19" t="s">
-        <v>608</v>
-      </c>
-      <c r="E82" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="F82" s="22"/>
-      <c r="G82" s="20"/>
-      <c r="H82" s="19" t="s">
-        <v>451</v>
-      </c>
-      <c r="I82" s="19" t="s">
-        <v>609</v>
       </c>
       <c r="J82" s="22"/>
       <c r="K82" s="22"/>
       <c r="L82" s="22"/>
       <c r="M82" s="19" t="s">
-        <v>209</v>
+        <v>603</v>
       </c>
       <c r="N82" s="19" t="s">
-        <v>209</v>
+        <v>603</v>
       </c>
       <c r="O82" s="19" t="s">
-        <v>209</v>
+        <v>603</v>
       </c>
       <c r="P82" s="19" t="s">
-        <v>209</v>
+        <v>603</v>
       </c>
       <c r="Q82" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="R82" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="S82" s="19" t="s">
-        <v>209</v>
-      </c>
+        <v>603</v>
+      </c>
+      <c r="R82" s="22"/>
+      <c r="S82" s="22"/>
       <c r="T82" s="22"/>
       <c r="U82" s="22"/>
-      <c r="V82" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="W82" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="X82" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="Y82" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="Z82" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="AA82" s="19" t="s">
-        <v>209</v>
-      </c>
+      <c r="V82" s="22"/>
+      <c r="W82" s="22"/>
+      <c r="X82" s="22"/>
+      <c r="Y82" s="22"/>
+      <c r="Z82" s="22"/>
+      <c r="AA82" s="22"/>
     </row>
     <row r="83" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="19" t="s">
+        <v>608</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>474</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>609</v>
+      </c>
+      <c r="D83" s="19" t="s">
         <v>610</v>
-      </c>
-      <c r="B83" s="19" t="s">
-        <v>611</v>
-      </c>
-      <c r="C83" s="19" t="s">
-        <v>612</v>
-      </c>
-      <c r="D83" s="19" t="s">
-        <v>613</v>
       </c>
       <c r="E83" s="19" t="s">
         <v>205</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>614</v>
-      </c>
-      <c r="G83" s="20"/>
+        <v>611</v>
+      </c>
+      <c r="G83" s="20" t="s">
+        <v>612</v>
+      </c>
       <c r="H83" s="21"/>
       <c r="I83" s="19" t="s">
-        <v>615</v>
-      </c>
-      <c r="J83" s="21"/>
-      <c r="K83" s="21"/>
-      <c r="L83" s="21"/>
-      <c r="M83" s="21"/>
-      <c r="N83" s="21"/>
-      <c r="O83" s="21"/>
-      <c r="P83" s="21"/>
-      <c r="Q83" s="21"/>
-      <c r="R83" s="21"/>
-      <c r="S83" s="21"/>
-      <c r="T83" s="21"/>
-      <c r="U83" s="21"/>
-      <c r="V83" s="21"/>
-      <c r="W83" s="21"/>
-      <c r="X83" s="21"/>
-      <c r="Y83" s="21"/>
-      <c r="Z83" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="AA83" s="21"/>
+        <v>613</v>
+      </c>
+      <c r="J83" s="22"/>
+      <c r="K83" s="22"/>
+      <c r="L83" s="22"/>
+      <c r="M83" s="19" t="s">
+        <v>614</v>
+      </c>
+      <c r="N83" s="19" t="s">
+        <v>614</v>
+      </c>
+      <c r="O83" s="19" t="s">
+        <v>614</v>
+      </c>
+      <c r="P83" s="19" t="s">
+        <v>614</v>
+      </c>
+      <c r="Q83" s="19" t="s">
+        <v>614</v>
+      </c>
+      <c r="R83" s="22"/>
+      <c r="S83" s="22"/>
+      <c r="T83" s="22"/>
+      <c r="U83" s="22"/>
+      <c r="V83" s="22"/>
+      <c r="W83" s="22"/>
+      <c r="X83" s="22"/>
+      <c r="Y83" s="22"/>
+      <c r="Z83" s="22"/>
+      <c r="AA83" s="22"/>
     </row>
     <row r="84" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="19" t="s">
+        <v>615</v>
+      </c>
+      <c r="B84" s="19" t="s">
+        <v>474</v>
+      </c>
+      <c r="C84" s="19" t="s">
         <v>616</v>
       </c>
-      <c r="B84" s="19" t="s">
-        <v>611</v>
-      </c>
-      <c r="C84" s="19" t="s">
+      <c r="D84" s="19" t="s">
         <v>617</v>
       </c>
-      <c r="D84" s="19" t="s">
+      <c r="E84" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="F84" s="22"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="19" t="s">
+        <v>451</v>
+      </c>
+      <c r="I84" s="19" t="s">
         <v>618</v>
-      </c>
-      <c r="E84" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="F84" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="G84" s="20"/>
-      <c r="H84" s="21"/>
-      <c r="I84" s="19" t="s">
-        <v>619</v>
       </c>
       <c r="J84" s="22"/>
       <c r="K84" s="22"/>
       <c r="L84" s="22"/>
       <c r="M84" s="19" t="s">
-        <v>620</v>
+        <v>209</v>
       </c>
       <c r="N84" s="19" t="s">
-        <v>620</v>
+        <v>209</v>
       </c>
       <c r="O84" s="19" t="s">
-        <v>620</v>
+        <v>209</v>
       </c>
       <c r="P84" s="19" t="s">
-        <v>620</v>
+        <v>209</v>
       </c>
       <c r="Q84" s="19" t="s">
-        <v>620</v>
-      </c>
-      <c r="R84" s="22"/>
-      <c r="S84" s="22"/>
+        <v>209</v>
+      </c>
+      <c r="R84" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="S84" s="19" t="s">
+        <v>209</v>
+      </c>
       <c r="T84" s="22"/>
       <c r="U84" s="22"/>
-      <c r="V84" s="22"/>
-      <c r="W84" s="22"/>
-      <c r="X84" s="22"/>
-      <c r="Y84" s="22"/>
+      <c r="V84" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="W84" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="X84" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y84" s="19" t="s">
+        <v>209</v>
+      </c>
       <c r="Z84" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="AA84" s="22"/>
+        <v>209</v>
+      </c>
+      <c r="AA84" s="19" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="19" t="s">
+        <v>619</v>
+      </c>
+      <c r="B85" s="19" t="s">
+        <v>620</v>
+      </c>
+      <c r="C85" s="19" t="s">
         <v>621</v>
       </c>
-      <c r="B85" s="19" t="s">
-        <v>611</v>
-      </c>
-      <c r="C85" s="19" t="s">
+      <c r="D85" s="19" t="s">
         <v>622</v>
       </c>
-      <c r="D85" s="19" t="s">
+      <c r="E85" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="F85" s="19" t="s">
         <v>623</v>
       </c>
-      <c r="E85" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="F85" s="22" t="s">
-        <v>302</v>
-      </c>
-      <c r="G85" s="22"/>
-      <c r="H85" s="19" t="s">
-        <v>337</v>
-      </c>
+      <c r="G85" s="20"/>
+      <c r="H85" s="21"/>
       <c r="I85" s="19" t="s">
         <v>624</v>
       </c>
-      <c r="J85" s="22"/>
-      <c r="K85" s="22"/>
-      <c r="L85" s="22"/>
-      <c r="M85" s="22"/>
-      <c r="N85" s="22"/>
-      <c r="O85" s="22"/>
-      <c r="P85" s="22"/>
-      <c r="Q85" s="22"/>
-      <c r="R85" s="22"/>
-      <c r="S85" s="22"/>
-      <c r="T85" s="22"/>
-      <c r="U85" s="22"/>
-      <c r="V85" s="22"/>
-      <c r="W85" s="22"/>
-      <c r="X85" s="22"/>
-      <c r="Y85" s="22"/>
+      <c r="J85" s="21"/>
+      <c r="K85" s="21"/>
+      <c r="L85" s="21"/>
+      <c r="M85" s="21"/>
+      <c r="N85" s="21"/>
+      <c r="O85" s="21"/>
+      <c r="P85" s="21"/>
+      <c r="Q85" s="21"/>
+      <c r="R85" s="21"/>
+      <c r="S85" s="21"/>
+      <c r="T85" s="21"/>
+      <c r="U85" s="21"/>
+      <c r="V85" s="21"/>
+      <c r="W85" s="21"/>
+      <c r="X85" s="21"/>
+      <c r="Y85" s="21"/>
       <c r="Z85" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="AA85" s="22"/>
+      <c r="AA85" s="21"/>
     </row>
     <row r="86" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="19" t="s">
         <v>625</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>611</v>
+        <v>620</v>
       </c>
       <c r="C86" s="19" t="s">
         <v>626</v>
@@ -10189,26 +10196,34 @@
         <v>627</v>
       </c>
       <c r="E86" s="19" t="s">
-        <v>301</v>
+        <v>232</v>
       </c>
       <c r="F86" s="22" t="s">
-        <v>302</v>
-      </c>
-      <c r="G86" s="22"/>
-      <c r="H86" s="19" t="s">
-        <v>337</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="G86" s="20"/>
+      <c r="H86" s="21"/>
       <c r="I86" s="19" t="s">
         <v>628</v>
       </c>
       <c r="J86" s="22"/>
       <c r="K86" s="22"/>
       <c r="L86" s="22"/>
-      <c r="M86" s="22"/>
-      <c r="N86" s="22"/>
-      <c r="O86" s="22"/>
-      <c r="P86" s="22"/>
-      <c r="Q86" s="22"/>
+      <c r="M86" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="N86" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="O86" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="P86" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q86" s="19" t="s">
+        <v>629</v>
+      </c>
       <c r="R86" s="22"/>
       <c r="S86" s="22"/>
       <c r="T86" s="22"/>
@@ -10218,31 +10233,33 @@
       <c r="X86" s="22"/>
       <c r="Y86" s="22"/>
       <c r="Z86" s="19" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="AA86" s="22"/>
     </row>
     <row r="87" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="19" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>611</v>
+        <v>620</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E87" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="F87" s="19" t="s">
-        <v>632</v>
+        <v>301</v>
+      </c>
+      <c r="F87" s="22" t="s">
+        <v>302</v>
       </c>
       <c r="G87" s="22"/>
-      <c r="H87" s="22"/>
+      <c r="H87" s="19" t="s">
+        <v>337</v>
+      </c>
       <c r="I87" s="19" t="s">
         <v>633</v>
       </c>
@@ -10272,7 +10289,7 @@
         <v>634</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>611</v>
+        <v>620</v>
       </c>
       <c r="C88" s="19" t="s">
         <v>635</v>
@@ -10281,34 +10298,26 @@
         <v>636</v>
       </c>
       <c r="E88" s="19" t="s">
-        <v>232</v>
+        <v>301</v>
       </c>
       <c r="F88" s="22" t="s">
-        <v>233</v>
-      </c>
-      <c r="G88" s="20"/>
-      <c r="H88" s="22"/>
+        <v>302</v>
+      </c>
+      <c r="G88" s="22"/>
+      <c r="H88" s="19" t="s">
+        <v>337</v>
+      </c>
       <c r="I88" s="19" t="s">
         <v>637</v>
       </c>
       <c r="J88" s="22"/>
       <c r="K88" s="22"/>
       <c r="L88" s="22"/>
-      <c r="M88" s="19" t="s">
-        <v>620</v>
-      </c>
-      <c r="N88" s="19" t="s">
-        <v>620</v>
-      </c>
-      <c r="O88" s="19" t="s">
-        <v>620</v>
-      </c>
-      <c r="P88" s="19" t="s">
-        <v>620</v>
-      </c>
-      <c r="Q88" s="19" t="s">
-        <v>620</v>
-      </c>
+      <c r="M88" s="22"/>
+      <c r="N88" s="22"/>
+      <c r="O88" s="22"/>
+      <c r="P88" s="22"/>
+      <c r="Q88" s="22"/>
       <c r="R88" s="22"/>
       <c r="S88" s="22"/>
       <c r="T88" s="22"/>
@@ -10327,7 +10336,7 @@
         <v>638</v>
       </c>
       <c r="B89" s="19" t="s">
-        <v>611</v>
+        <v>620</v>
       </c>
       <c r="C89" s="19" t="s">
         <v>639</v>
@@ -10336,34 +10345,24 @@
         <v>640</v>
       </c>
       <c r="E89" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="F89" s="24" t="s">
-        <v>331</v>
+        <v>205</v>
+      </c>
+      <c r="F89" s="19" t="s">
+        <v>641</v>
       </c>
       <c r="G89" s="22"/>
       <c r="H89" s="22"/>
       <c r="I89" s="19" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="J89" s="22"/>
       <c r="K89" s="22"/>
       <c r="L89" s="22"/>
-      <c r="M89" s="19" t="s">
-        <v>620</v>
-      </c>
-      <c r="N89" s="19" t="s">
-        <v>620</v>
-      </c>
-      <c r="O89" s="19" t="s">
-        <v>620</v>
-      </c>
-      <c r="P89" s="19" t="s">
-        <v>620</v>
-      </c>
-      <c r="Q89" s="19" t="s">
-        <v>620</v>
-      </c>
+      <c r="M89" s="22"/>
+      <c r="N89" s="22"/>
+      <c r="O89" s="22"/>
+      <c r="P89" s="22"/>
+      <c r="Q89" s="22"/>
       <c r="R89" s="22"/>
       <c r="S89" s="22"/>
       <c r="T89" s="22"/>
@@ -10373,53 +10372,51 @@
       <c r="X89" s="22"/>
       <c r="Y89" s="22"/>
       <c r="Z89" s="19" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="AA89" s="22"/>
     </row>
     <row r="90" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="19" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="B90" s="19" t="s">
-        <v>611</v>
+        <v>620</v>
       </c>
       <c r="C90" s="19" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D90" s="19" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="E90" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="F90" s="20" t="s">
-        <v>645</v>
-      </c>
-      <c r="G90" s="20" t="s">
-        <v>646</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="F90" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="G90" s="20"/>
       <c r="H90" s="22"/>
       <c r="I90" s="19" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="J90" s="22"/>
       <c r="K90" s="22"/>
       <c r="L90" s="22"/>
       <c r="M90" s="19" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="N90" s="19" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="O90" s="19" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="P90" s="19" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="Q90" s="19" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="R90" s="22"/>
       <c r="S90" s="22"/>
@@ -10429,54 +10426,52 @@
       <c r="W90" s="22"/>
       <c r="X90" s="22"/>
       <c r="Y90" s="22"/>
-      <c r="Z90" s="22"/>
+      <c r="Z90" s="19" t="s">
+        <v>209</v>
+      </c>
       <c r="AA90" s="22"/>
     </row>
     <row r="91" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="19" t="s">
+        <v>647</v>
+      </c>
+      <c r="B91" s="19" t="s">
+        <v>620</v>
+      </c>
+      <c r="C91" s="19" t="s">
         <v>648</v>
       </c>
-      <c r="B91" s="19" t="s">
-        <v>611</v>
-      </c>
-      <c r="C91" s="19" t="s">
+      <c r="D91" s="19" t="s">
         <v>649</v>
       </c>
-      <c r="D91" s="19" t="s">
+      <c r="E91" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="F91" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="G91" s="22"/>
+      <c r="H91" s="22"/>
+      <c r="I91" s="19" t="s">
         <v>650</v>
-      </c>
-      <c r="E91" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="F91" s="22" t="s">
-        <v>302</v>
-      </c>
-      <c r="G91" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="H91" s="19" t="s">
-        <v>337</v>
-      </c>
-      <c r="I91" s="19" t="s">
-        <v>651</v>
       </c>
       <c r="J91" s="22"/>
       <c r="K91" s="22"/>
       <c r="L91" s="22"/>
       <c r="M91" s="19" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="N91" s="19" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="O91" s="19" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="P91" s="19" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="Q91" s="19" t="s">
-        <v>620</v>
+        <v>629</v>
       </c>
       <c r="R91" s="22"/>
       <c r="S91" s="22"/>
@@ -10486,52 +10481,54 @@
       <c r="W91" s="22"/>
       <c r="X91" s="22"/>
       <c r="Y91" s="22"/>
-      <c r="Z91" s="22"/>
+      <c r="Z91" s="19" t="s">
+        <v>209</v>
+      </c>
       <c r="AA91" s="22"/>
     </row>
     <row r="92" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="19" t="s">
+        <v>651</v>
+      </c>
+      <c r="B92" s="19" t="s">
+        <v>620</v>
+      </c>
+      <c r="C92" s="19" t="s">
         <v>652</v>
       </c>
-      <c r="B92" s="19" t="s">
-        <v>611</v>
-      </c>
-      <c r="C92" s="19" t="s">
+      <c r="D92" s="19" t="s">
         <v>653</v>
-      </c>
-      <c r="D92" s="19" t="s">
-        <v>654</v>
       </c>
       <c r="E92" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="F92" s="21" t="s">
+      <c r="F92" s="20" t="s">
+        <v>654</v>
+      </c>
+      <c r="G92" s="20" t="s">
         <v>655</v>
-      </c>
-      <c r="G92" s="20" t="s">
-        <v>656</v>
       </c>
       <c r="H92" s="22"/>
       <c r="I92" s="19" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="J92" s="22"/>
       <c r="K92" s="22"/>
       <c r="L92" s="22"/>
       <c r="M92" s="19" t="s">
-        <v>658</v>
+        <v>629</v>
       </c>
       <c r="N92" s="19" t="s">
-        <v>658</v>
+        <v>629</v>
       </c>
       <c r="O92" s="19" t="s">
-        <v>658</v>
+        <v>629</v>
       </c>
       <c r="P92" s="19" t="s">
-        <v>658</v>
+        <v>629</v>
       </c>
       <c r="Q92" s="19" t="s">
-        <v>658</v>
+        <v>629</v>
       </c>
       <c r="R92" s="22"/>
       <c r="S92" s="22"/>
@@ -10546,144 +10543,156 @@
     </row>
     <row r="93" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="19" t="s">
+        <v>657</v>
+      </c>
+      <c r="B93" s="19" t="s">
+        <v>620</v>
+      </c>
+      <c r="C93" s="19" t="s">
+        <v>658</v>
+      </c>
+      <c r="D93" s="19" t="s">
         <v>659</v>
-      </c>
-      <c r="B93" s="19" t="s">
-        <v>611</v>
-      </c>
-      <c r="C93" s="19" t="s">
-        <v>660</v>
-      </c>
-      <c r="D93" s="19" t="s">
-        <v>661</v>
       </c>
       <c r="E93" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="F93" s="21" t="s">
+      <c r="F93" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="G93" s="20" t="s">
-        <v>662</v>
-      </c>
-      <c r="H93" s="21"/>
+      <c r="G93" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" s="19" t="s">
+        <v>337</v>
+      </c>
       <c r="I93" s="19" t="s">
-        <v>663</v>
-      </c>
-      <c r="J93" s="21"/>
-      <c r="K93" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="L93" s="21"/>
-      <c r="M93" s="21"/>
-      <c r="N93" s="21"/>
-      <c r="O93" s="21"/>
-      <c r="P93" s="21"/>
-      <c r="Q93" s="21"/>
-      <c r="R93" s="21"/>
-      <c r="S93" s="21"/>
-      <c r="T93" s="21"/>
-      <c r="U93" s="21"/>
-      <c r="V93" s="21"/>
-      <c r="W93" s="21"/>
-      <c r="X93" s="21"/>
-      <c r="Y93" s="21"/>
-      <c r="Z93" s="21"/>
-      <c r="AA93" s="21"/>
+        <v>660</v>
+      </c>
+      <c r="J93" s="22"/>
+      <c r="K93" s="22"/>
+      <c r="L93" s="22"/>
+      <c r="M93" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="N93" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="O93" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="P93" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="Q93" s="19" t="s">
+        <v>629</v>
+      </c>
+      <c r="R93" s="22"/>
+      <c r="S93" s="22"/>
+      <c r="T93" s="22"/>
+      <c r="U93" s="22"/>
+      <c r="V93" s="22"/>
+      <c r="W93" s="22"/>
+      <c r="X93" s="22"/>
+      <c r="Y93" s="22"/>
+      <c r="Z93" s="22"/>
+      <c r="AA93" s="22"/>
     </row>
     <row r="94" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="19" t="s">
+        <v>661</v>
+      </c>
+      <c r="B94" s="19" t="s">
+        <v>620</v>
+      </c>
+      <c r="C94" s="19" t="s">
+        <v>662</v>
+      </c>
+      <c r="D94" s="19" t="s">
+        <v>663</v>
+      </c>
+      <c r="E94" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="F94" s="21" t="s">
         <v>664</v>
       </c>
-      <c r="B94" s="19" t="s">
+      <c r="G94" s="20" t="s">
         <v>665</v>
       </c>
-      <c r="C94" s="19" t="s">
+      <c r="H94" s="22"/>
+      <c r="I94" s="19" t="s">
         <v>666</v>
       </c>
-      <c r="D94" s="19" t="s">
+      <c r="J94" s="22"/>
+      <c r="K94" s="22"/>
+      <c r="L94" s="22"/>
+      <c r="M94" s="19" t="s">
         <v>667</v>
       </c>
-      <c r="E94" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="F94" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="G94" s="20"/>
-      <c r="H94" s="19"/>
-      <c r="I94" s="19" t="s">
-        <v>668</v>
-      </c>
-      <c r="J94" s="19"/>
-      <c r="K94" s="19" t="s">
-        <v>669</v>
-      </c>
-      <c r="L94" s="19" t="s">
-        <v>669</v>
-      </c>
-      <c r="M94" s="19" t="s">
-        <v>669</v>
-      </c>
       <c r="N94" s="19" t="s">
-        <v>669</v>
-      </c>
-      <c r="O94" s="21"/>
+        <v>667</v>
+      </c>
+      <c r="O94" s="19" t="s">
+        <v>667</v>
+      </c>
       <c r="P94" s="19" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="Q94" s="19" t="s">
-        <v>671</v>
-      </c>
-      <c r="R94" s="19"/>
-      <c r="S94" s="19"/>
-      <c r="T94" s="19"/>
-      <c r="U94" s="19"/>
-      <c r="V94" s="19" t="s">
-        <v>671</v>
-      </c>
-      <c r="W94" s="21"/>
-      <c r="X94" s="21"/>
-      <c r="Y94" s="21"/>
-      <c r="Z94" s="21"/>
-      <c r="AA94" s="21"/>
+        <v>667</v>
+      </c>
+      <c r="R94" s="22"/>
+      <c r="S94" s="22"/>
+      <c r="T94" s="22"/>
+      <c r="U94" s="22"/>
+      <c r="V94" s="22"/>
+      <c r="W94" s="22"/>
+      <c r="X94" s="22"/>
+      <c r="Y94" s="22"/>
+      <c r="Z94" s="22"/>
+      <c r="AA94" s="22"/>
     </row>
     <row r="95" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="19" t="s">
+        <v>668</v>
+      </c>
+      <c r="B95" s="19" t="s">
+        <v>620</v>
+      </c>
+      <c r="C95" s="19" t="s">
+        <v>669</v>
+      </c>
+      <c r="D95" s="19" t="s">
+        <v>670</v>
+      </c>
+      <c r="E95" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="F95" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="G95" s="20" t="s">
+        <v>671</v>
+      </c>
+      <c r="H95" s="21"/>
+      <c r="I95" s="19" t="s">
         <v>672</v>
       </c>
-      <c r="B95" s="19" t="s">
-        <v>665</v>
-      </c>
-      <c r="C95" s="19" t="s">
-        <v>673</v>
-      </c>
-      <c r="D95" s="19" t="s">
-        <v>674</v>
-      </c>
-      <c r="E95" s="19" t="s">
-        <v>381</v>
-      </c>
-      <c r="F95" s="21"/>
-      <c r="G95" s="22"/>
-      <c r="H95" s="19"/>
-      <c r="I95" s="19" t="s">
-        <v>675</v>
-      </c>
-      <c r="J95" s="19"/>
-      <c r="K95" s="21"/>
+      <c r="J95" s="21"/>
+      <c r="K95" s="19" t="s">
+        <v>209</v>
+      </c>
       <c r="L95" s="21"/>
       <c r="M95" s="21"/>
       <c r="N95" s="21"/>
-      <c r="O95" s="19" t="s">
-        <v>669</v>
-      </c>
+      <c r="O95" s="21"/>
       <c r="P95" s="21"/>
       <c r="Q95" s="21"/>
-      <c r="R95" s="19"/>
-      <c r="S95" s="19"/>
-      <c r="T95" s="19"/>
-      <c r="U95" s="19"/>
+      <c r="R95" s="21"/>
+      <c r="S95" s="21"/>
+      <c r="T95" s="21"/>
+      <c r="U95" s="21"/>
       <c r="V95" s="21"/>
       <c r="W95" s="21"/>
       <c r="X95" s="21"/>
@@ -10693,54 +10702,54 @@
     </row>
     <row r="96" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="19" t="s">
+        <v>673</v>
+      </c>
+      <c r="B96" s="19" t="s">
+        <v>674</v>
+      </c>
+      <c r="C96" s="19" t="s">
+        <v>675</v>
+      </c>
+      <c r="D96" s="19" t="s">
         <v>676</v>
       </c>
-      <c r="B96" s="19" t="s">
-        <v>665</v>
-      </c>
-      <c r="C96" s="19" t="s">
-        <v>677</v>
-      </c>
-      <c r="D96" s="19" t="s">
-        <v>678</v>
-      </c>
       <c r="E96" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="F96" s="24" t="s">
-        <v>331</v>
+        <v>232</v>
+      </c>
+      <c r="F96" s="21" t="s">
+        <v>233</v>
       </c>
       <c r="G96" s="20"/>
       <c r="H96" s="19"/>
       <c r="I96" s="19" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="J96" s="19"/>
       <c r="K96" s="19" t="s">
-        <v>669</v>
+        <v>678</v>
       </c>
       <c r="L96" s="19" t="s">
-        <v>669</v>
+        <v>678</v>
       </c>
       <c r="M96" s="19" t="s">
-        <v>669</v>
+        <v>678</v>
       </c>
       <c r="N96" s="19" t="s">
-        <v>669</v>
+        <v>678</v>
       </c>
       <c r="O96" s="21"/>
       <c r="P96" s="19" t="s">
-        <v>670</v>
+        <v>679</v>
       </c>
       <c r="Q96" s="19" t="s">
-        <v>671</v>
+        <v>680</v>
       </c>
       <c r="R96" s="19"/>
       <c r="S96" s="19"/>
       <c r="T96" s="19"/>
       <c r="U96" s="19"/>
       <c r="V96" s="19" t="s">
-        <v>671</v>
+        <v>680</v>
       </c>
       <c r="W96" s="21"/>
       <c r="X96" s="21"/>
@@ -10750,25 +10759,25 @@
     </row>
     <row r="97" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="19" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="C97" s="19" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="D97" s="19" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="E97" s="19" t="s">
-        <v>391</v>
-      </c>
-      <c r="F97" s="19"/>
+        <v>381</v>
+      </c>
+      <c r="F97" s="21"/>
       <c r="G97" s="22"/>
       <c r="H97" s="19"/>
       <c r="I97" s="19" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="J97" s="19"/>
       <c r="K97" s="21"/>
@@ -10776,7 +10785,7 @@
       <c r="M97" s="21"/>
       <c r="N97" s="21"/>
       <c r="O97" s="19" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
       <c r="P97" s="21"/>
       <c r="Q97" s="21"/>
@@ -10796,7 +10805,7 @@
         <v>685</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="C98" s="19" t="s">
         <v>686</v>
@@ -10805,42 +10814,42 @@
         <v>687</v>
       </c>
       <c r="E98" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="F98" s="21"/>
-      <c r="G98" s="20" t="n">
-        <v>0</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="F98" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="G98" s="20"/>
       <c r="H98" s="19"/>
       <c r="I98" s="19" t="s">
         <v>688</v>
       </c>
       <c r="J98" s="19"/>
       <c r="K98" s="19" t="s">
-        <v>689</v>
+        <v>678</v>
       </c>
       <c r="L98" s="19" t="s">
-        <v>689</v>
+        <v>678</v>
       </c>
       <c r="M98" s="19" t="s">
-        <v>689</v>
+        <v>678</v>
       </c>
       <c r="N98" s="19" t="s">
-        <v>689</v>
+        <v>678</v>
       </c>
       <c r="O98" s="21"/>
       <c r="P98" s="19" t="s">
-        <v>689</v>
+        <v>679</v>
       </c>
       <c r="Q98" s="19" t="s">
-        <v>228</v>
+        <v>680</v>
       </c>
       <c r="R98" s="19"/>
       <c r="S98" s="19"/>
       <c r="T98" s="19"/>
       <c r="U98" s="19"/>
       <c r="V98" s="19" t="s">
-        <v>228</v>
+        <v>680</v>
       </c>
       <c r="W98" s="21"/>
       <c r="X98" s="21"/>
@@ -10850,25 +10859,25 @@
     </row>
     <row r="99" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="B99" s="19" t="s">
+        <v>674</v>
+      </c>
+      <c r="C99" s="19" t="s">
         <v>690</v>
       </c>
-      <c r="B99" s="19" t="s">
-        <v>665</v>
-      </c>
-      <c r="C99" s="19" t="s">
+      <c r="D99" s="19" t="s">
         <v>691</v>
       </c>
-      <c r="D99" s="19" t="s">
-        <v>692</v>
-      </c>
       <c r="E99" s="19" t="s">
-        <v>548</v>
-      </c>
-      <c r="F99" s="21"/>
+        <v>391</v>
+      </c>
+      <c r="F99" s="19"/>
       <c r="G99" s="22"/>
       <c r="H99" s="19"/>
       <c r="I99" s="19" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="J99" s="19"/>
       <c r="K99" s="21"/>
@@ -10876,7 +10885,7 @@
       <c r="M99" s="21"/>
       <c r="N99" s="21"/>
       <c r="O99" s="19" t="s">
-        <v>689</v>
+        <v>693</v>
       </c>
       <c r="P99" s="21"/>
       <c r="Q99" s="21"/>
@@ -10896,7 +10905,7 @@
         <v>694</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="C100" s="19" t="s">
         <v>695</v>
@@ -10905,31 +10914,43 @@
         <v>696</v>
       </c>
       <c r="E100" s="19" t="s">
-        <v>317</v>
-      </c>
-      <c r="F100" s="19" t="s">
-        <v>697</v>
-      </c>
-      <c r="G100" s="22"/>
+        <v>301</v>
+      </c>
+      <c r="F100" s="21"/>
+      <c r="G100" s="20" t="n">
+        <v>0</v>
+      </c>
       <c r="H100" s="19"/>
       <c r="I100" s="19" t="s">
+        <v>697</v>
+      </c>
+      <c r="J100" s="19"/>
+      <c r="K100" s="19" t="s">
         <v>698</v>
       </c>
-      <c r="J100" s="19"/>
-      <c r="K100" s="21"/>
-      <c r="L100" s="21"/>
-      <c r="M100" s="21"/>
-      <c r="N100" s="21"/>
-      <c r="O100" s="19" t="s">
-        <v>689</v>
-      </c>
-      <c r="P100" s="21"/>
-      <c r="Q100" s="21"/>
+      <c r="L100" s="19" t="s">
+        <v>698</v>
+      </c>
+      <c r="M100" s="19" t="s">
+        <v>698</v>
+      </c>
+      <c r="N100" s="19" t="s">
+        <v>698</v>
+      </c>
+      <c r="O100" s="21"/>
+      <c r="P100" s="19" t="s">
+        <v>698</v>
+      </c>
+      <c r="Q100" s="19" t="s">
+        <v>228</v>
+      </c>
       <c r="R100" s="19"/>
       <c r="S100" s="19"/>
       <c r="T100" s="19"/>
       <c r="U100" s="19"/>
-      <c r="V100" s="21"/>
+      <c r="V100" s="19" t="s">
+        <v>228</v>
+      </c>
       <c r="W100" s="21"/>
       <c r="X100" s="21"/>
       <c r="Y100" s="21"/>
@@ -10941,7 +10962,7 @@
         <v>699</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="C101" s="19" t="s">
         <v>700</v>
@@ -10950,43 +10971,29 @@
         <v>701</v>
       </c>
       <c r="E101" s="19" t="s">
-        <v>244</v>
-      </c>
-      <c r="F101" s="19"/>
-      <c r="G101" s="20"/>
+        <v>548</v>
+      </c>
+      <c r="F101" s="21"/>
+      <c r="G101" s="22"/>
       <c r="H101" s="19"/>
       <c r="I101" s="19" t="s">
         <v>702</v>
       </c>
       <c r="J101" s="19"/>
-      <c r="K101" s="19" t="s">
-        <v>689</v>
-      </c>
-      <c r="L101" s="19" t="s">
-        <v>689</v>
-      </c>
-      <c r="M101" s="19" t="s">
-        <v>689</v>
-      </c>
-      <c r="N101" s="19" t="s">
-        <v>689</v>
-      </c>
+      <c r="K101" s="21"/>
+      <c r="L101" s="21"/>
+      <c r="M101" s="21"/>
+      <c r="N101" s="21"/>
       <c r="O101" s="19" t="s">
-        <v>689</v>
-      </c>
-      <c r="P101" s="19" t="s">
-        <v>689</v>
-      </c>
-      <c r="Q101" s="19" t="s">
-        <v>228</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="P101" s="21"/>
+      <c r="Q101" s="21"/>
       <c r="R101" s="19"/>
       <c r="S101" s="19"/>
       <c r="T101" s="19"/>
       <c r="U101" s="19"/>
-      <c r="V101" s="19" t="s">
-        <v>228</v>
-      </c>
+      <c r="V101" s="21"/>
       <c r="W101" s="21"/>
       <c r="X101" s="21"/>
       <c r="Y101" s="21"/>
@@ -10998,7 +11005,7 @@
         <v>703</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="C102" s="19" t="s">
         <v>704</v>
@@ -11007,32 +11014,26 @@
         <v>705</v>
       </c>
       <c r="E102" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="F102" s="21"/>
-      <c r="G102" s="20"/>
+        <v>317</v>
+      </c>
+      <c r="F102" s="19" t="s">
+        <v>706</v>
+      </c>
+      <c r="G102" s="22"/>
       <c r="H102" s="19"/>
       <c r="I102" s="19" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="J102" s="19"/>
-      <c r="K102" s="19"/>
+      <c r="K102" s="21"/>
       <c r="L102" s="21"/>
-      <c r="M102" s="19" t="s">
-        <v>684</v>
-      </c>
-      <c r="N102" s="19" t="s">
-        <v>684</v>
-      </c>
+      <c r="M102" s="21"/>
+      <c r="N102" s="21"/>
       <c r="O102" s="19" t="s">
-        <v>684</v>
-      </c>
-      <c r="P102" s="19" t="s">
-        <v>684</v>
-      </c>
-      <c r="Q102" s="19" t="s">
-        <v>684</v>
-      </c>
+        <v>698</v>
+      </c>
+      <c r="P102" s="21"/>
+      <c r="Q102" s="21"/>
       <c r="R102" s="19"/>
       <c r="S102" s="19"/>
       <c r="T102" s="19"/>
@@ -11042,104 +11043,104 @@
       <c r="X102" s="21"/>
       <c r="Y102" s="21"/>
       <c r="Z102" s="21"/>
-      <c r="AA102" s="19" t="s">
-        <v>594</v>
-      </c>
+      <c r="AA102" s="21"/>
     </row>
     <row r="103" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="19" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="C103" s="19" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="D103" s="19" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="E103" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="F103" s="21"/>
+        <v>244</v>
+      </c>
+      <c r="F103" s="19"/>
       <c r="G103" s="20"/>
       <c r="H103" s="19"/>
       <c r="I103" s="19" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="J103" s="19"/>
-      <c r="K103" s="19"/>
-      <c r="L103" s="21"/>
+      <c r="K103" s="19" t="s">
+        <v>698</v>
+      </c>
+      <c r="L103" s="19" t="s">
+        <v>698</v>
+      </c>
       <c r="M103" s="19" t="s">
-        <v>684</v>
+        <v>698</v>
       </c>
       <c r="N103" s="19" t="s">
-        <v>684</v>
+        <v>698</v>
       </c>
       <c r="O103" s="19" t="s">
-        <v>684</v>
+        <v>698</v>
       </c>
       <c r="P103" s="19" t="s">
-        <v>684</v>
+        <v>698</v>
       </c>
       <c r="Q103" s="19" t="s">
-        <v>684</v>
+        <v>228</v>
       </c>
       <c r="R103" s="19"/>
       <c r="S103" s="19"/>
       <c r="T103" s="19"/>
       <c r="U103" s="19"/>
-      <c r="V103" s="21"/>
+      <c r="V103" s="19" t="s">
+        <v>228</v>
+      </c>
       <c r="W103" s="21"/>
       <c r="X103" s="21"/>
       <c r="Y103" s="21"/>
       <c r="Z103" s="21"/>
-      <c r="AA103" s="19" t="s">
-        <v>594</v>
-      </c>
+      <c r="AA103" s="21"/>
     </row>
     <row r="104" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="19" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="C104" s="19" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="D104" s="19" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E104" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="F104" s="21" t="s">
-        <v>302</v>
-      </c>
+      <c r="F104" s="21"/>
       <c r="G104" s="20"/>
       <c r="H104" s="19"/>
       <c r="I104" s="19" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="J104" s="19"/>
       <c r="K104" s="19"/>
       <c r="L104" s="21"/>
       <c r="M104" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="N104" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="O104" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="P104" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="Q104" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="R104" s="19"/>
       <c r="S104" s="19"/>
@@ -11150,49 +11151,49 @@
       <c r="X104" s="21"/>
       <c r="Y104" s="21"/>
       <c r="Z104" s="21"/>
-      <c r="AA104" s="19"/>
+      <c r="AA104" s="19" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="19" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="C105" s="19" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="D105" s="19" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="E105" s="19" t="s">
         <v>301</v>
       </c>
-      <c r="F105" s="21" t="s">
-        <v>302</v>
-      </c>
+      <c r="F105" s="21"/>
       <c r="G105" s="20"/>
       <c r="H105" s="19"/>
       <c r="I105" s="19" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="J105" s="19"/>
       <c r="K105" s="19"/>
       <c r="L105" s="21"/>
       <c r="M105" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="N105" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="O105" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="P105" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="Q105" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="R105" s="19"/>
       <c r="S105" s="19"/>
@@ -11203,55 +11204,57 @@
       <c r="X105" s="21"/>
       <c r="Y105" s="21"/>
       <c r="Z105" s="21"/>
-      <c r="AA105" s="19"/>
+      <c r="AA105" s="19" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="19" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="C106" s="19" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="D106" s="19" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="E106" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="F106" s="19" t="s">
-        <v>722</v>
-      </c>
-      <c r="G106" s="20" t="s">
-        <v>723</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="F106" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="G106" s="20"/>
       <c r="H106" s="19"/>
       <c r="I106" s="19" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="J106" s="19"/>
       <c r="K106" s="19"/>
       <c r="L106" s="21"/>
       <c r="M106" s="19" t="s">
-        <v>725</v>
+        <v>693</v>
       </c>
       <c r="N106" s="19" t="s">
-        <v>725</v>
+        <v>693</v>
       </c>
       <c r="O106" s="19" t="s">
-        <v>725</v>
-      </c>
-      <c r="P106" s="21"/>
-      <c r="Q106" s="21"/>
+        <v>693</v>
+      </c>
+      <c r="P106" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="Q106" s="19" t="s">
+        <v>693</v>
+      </c>
       <c r="R106" s="19"/>
       <c r="S106" s="19"/>
       <c r="T106" s="19"/>
       <c r="U106" s="19"/>
-      <c r="V106" s="19" t="s">
-        <v>725</v>
-      </c>
+      <c r="V106" s="21"/>
       <c r="W106" s="21"/>
       <c r="X106" s="21"/>
       <c r="Y106" s="21"/>
@@ -11260,57 +11263,51 @@
     </row>
     <row r="107" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="19" t="s">
+        <v>724</v>
+      </c>
+      <c r="B107" s="19" t="s">
+        <v>674</v>
+      </c>
+      <c r="C107" s="19" t="s">
+        <v>725</v>
+      </c>
+      <c r="D107" s="19" t="s">
         <v>726</v>
       </c>
-      <c r="B107" s="19" t="s">
-        <v>665</v>
-      </c>
-      <c r="C107" s="19" t="s">
-        <v>727</v>
-      </c>
-      <c r="D107" s="19" t="s">
-        <v>728</v>
-      </c>
       <c r="E107" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="F107" s="24" t="s">
-        <v>286</v>
-      </c>
-      <c r="G107" s="20" t="s">
-        <v>287</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="F107" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="G107" s="20"/>
       <c r="H107" s="19"/>
       <c r="I107" s="19" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="J107" s="19"/>
       <c r="K107" s="19"/>
-      <c r="L107" s="19" t="s">
-        <v>684</v>
-      </c>
+      <c r="L107" s="21"/>
       <c r="M107" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="N107" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="O107" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="P107" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="Q107" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="R107" s="19"/>
       <c r="S107" s="19"/>
       <c r="T107" s="19"/>
       <c r="U107" s="19"/>
-      <c r="V107" s="19" t="s">
-        <v>684</v>
-      </c>
+      <c r="V107" s="21"/>
       <c r="W107" s="21"/>
       <c r="X107" s="21"/>
       <c r="Y107" s="21"/>
@@ -11319,52 +11316,50 @@
     </row>
     <row r="108" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="19" t="s">
+        <v>728</v>
+      </c>
+      <c r="B108" s="19" t="s">
+        <v>674</v>
+      </c>
+      <c r="C108" s="19" t="s">
+        <v>729</v>
+      </c>
+      <c r="D108" s="19" t="s">
         <v>730</v>
       </c>
-      <c r="B108" s="19" t="s">
-        <v>665</v>
-      </c>
-      <c r="C108" s="19" t="s">
+      <c r="E108" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="F108" s="19" t="s">
         <v>731</v>
       </c>
-      <c r="D108" s="19" t="s">
+      <c r="G108" s="20" t="s">
         <v>732</v>
       </c>
-      <c r="E108" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="F108" s="21"/>
-      <c r="G108" s="20"/>
       <c r="H108" s="19"/>
       <c r="I108" s="19" t="s">
         <v>733</v>
       </c>
       <c r="J108" s="19"/>
       <c r="K108" s="19"/>
-      <c r="L108" s="19" t="s">
-        <v>684</v>
-      </c>
+      <c r="L108" s="21"/>
       <c r="M108" s="19" t="s">
-        <v>684</v>
+        <v>734</v>
       </c>
       <c r="N108" s="19" t="s">
-        <v>684</v>
+        <v>734</v>
       </c>
       <c r="O108" s="19" t="s">
-        <v>684</v>
-      </c>
-      <c r="P108" s="19" t="s">
-        <v>684</v>
-      </c>
-      <c r="Q108" s="19" t="s">
-        <v>684</v>
-      </c>
+        <v>734</v>
+      </c>
+      <c r="P108" s="21"/>
+      <c r="Q108" s="21"/>
       <c r="R108" s="19"/>
       <c r="S108" s="19"/>
       <c r="T108" s="19"/>
       <c r="U108" s="19"/>
       <c r="V108" s="19" t="s">
-        <v>684</v>
+        <v>734</v>
       </c>
       <c r="W108" s="21"/>
       <c r="X108" s="21"/>
@@ -11374,54 +11369,56 @@
     </row>
     <row r="109" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="19" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>665</v>
+        <v>674</v>
       </c>
       <c r="C109" s="19" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="D109" s="19" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="E109" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="F109" s="21"/>
-      <c r="G109" s="20" t="n">
-        <v>1</v>
+        <v>285</v>
+      </c>
+      <c r="F109" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="G109" s="20" t="s">
+        <v>287</v>
       </c>
       <c r="H109" s="19"/>
       <c r="I109" s="19" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="J109" s="19"/>
       <c r="K109" s="19"/>
       <c r="L109" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="M109" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="N109" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="O109" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="P109" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="Q109" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="R109" s="19"/>
       <c r="S109" s="19"/>
       <c r="T109" s="19"/>
       <c r="U109" s="19"/>
       <c r="V109" s="19" t="s">
-        <v>684</v>
+        <v>693</v>
       </c>
       <c r="W109" s="21"/>
       <c r="X109" s="21"/>
@@ -11431,10 +11428,10 @@
     </row>
     <row r="110" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="19" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>739</v>
+        <v>674</v>
       </c>
       <c r="C110" s="19" t="s">
         <v>740</v>
@@ -11443,11 +11440,9 @@
         <v>741</v>
       </c>
       <c r="E110" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="F110" s="21" t="s">
-        <v>233</v>
-      </c>
+        <v>301</v>
+      </c>
+      <c r="F110" s="21"/>
       <c r="G110" s="20"/>
       <c r="H110" s="19"/>
       <c r="I110" s="19" t="s">
@@ -11455,111 +11450,117 @@
       </c>
       <c r="J110" s="19"/>
       <c r="K110" s="19"/>
-      <c r="L110" s="19"/>
-      <c r="M110" s="19"/>
-      <c r="N110" s="19"/>
-      <c r="O110" s="19"/>
-      <c r="P110" s="19"/>
-      <c r="Q110" s="19"/>
+      <c r="L110" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="M110" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="N110" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="O110" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="P110" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="Q110" s="19" t="s">
+        <v>693</v>
+      </c>
       <c r="R110" s="19"/>
       <c r="S110" s="19"/>
-      <c r="T110" s="19" t="s">
-        <v>743</v>
-      </c>
-      <c r="U110" s="19" t="s">
-        <v>743</v>
-      </c>
-      <c r="V110" s="21"/>
+      <c r="T110" s="19"/>
+      <c r="U110" s="19"/>
+      <c r="V110" s="19" t="s">
+        <v>693</v>
+      </c>
       <c r="W110" s="21"/>
-      <c r="X110" s="19" t="s">
-        <v>743</v>
-      </c>
-      <c r="Y110" s="19" t="s">
-        <v>743</v>
-      </c>
-      <c r="Z110" s="19" t="s">
-        <v>743</v>
-      </c>
+      <c r="X110" s="21"/>
+      <c r="Y110" s="21"/>
+      <c r="Z110" s="21"/>
       <c r="AA110" s="19"/>
     </row>
     <row r="111" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="19" t="s">
+        <v>743</v>
+      </c>
+      <c r="B111" s="19" t="s">
+        <v>674</v>
+      </c>
+      <c r="C111" s="19" t="s">
         <v>744</v>
       </c>
-      <c r="B111" s="19" t="s">
-        <v>739</v>
-      </c>
-      <c r="C111" s="19" t="s">
+      <c r="D111" s="19" t="s">
         <v>745</v>
-      </c>
-      <c r="D111" s="19" t="s">
-        <v>746</v>
       </c>
       <c r="E111" s="19" t="s">
         <v>301</v>
       </c>
       <c r="F111" s="21"/>
-      <c r="G111" s="20"/>
-      <c r="H111" s="19" t="s">
-        <v>337</v>
-      </c>
+      <c r="G111" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="H111" s="19"/>
       <c r="I111" s="19" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="J111" s="19"/>
       <c r="K111" s="19"/>
-      <c r="L111" s="19"/>
-      <c r="M111" s="19"/>
-      <c r="N111" s="19"/>
-      <c r="O111" s="19"/>
-      <c r="P111" s="19"/>
-      <c r="Q111" s="19"/>
+      <c r="L111" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="M111" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="N111" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="O111" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="P111" s="19" t="s">
+        <v>693</v>
+      </c>
+      <c r="Q111" s="19" t="s">
+        <v>693</v>
+      </c>
       <c r="R111" s="19"/>
       <c r="S111" s="19"/>
-      <c r="T111" s="19" t="s">
-        <v>748</v>
-      </c>
-      <c r="U111" s="19" t="s">
-        <v>748</v>
-      </c>
-      <c r="V111" s="21"/>
+      <c r="T111" s="19"/>
+      <c r="U111" s="19"/>
+      <c r="V111" s="19" t="s">
+        <v>693</v>
+      </c>
       <c r="W111" s="21"/>
-      <c r="X111" s="19" t="s">
-        <v>748</v>
-      </c>
-      <c r="Y111" s="19" t="s">
-        <v>748</v>
-      </c>
-      <c r="Z111" s="19" t="s">
-        <v>748</v>
-      </c>
+      <c r="X111" s="21"/>
+      <c r="Y111" s="21"/>
+      <c r="Z111" s="21"/>
       <c r="AA111" s="19"/>
     </row>
     <row r="112" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="19" t="s">
+        <v>747</v>
+      </c>
+      <c r="B112" s="19" t="s">
+        <v>748</v>
+      </c>
+      <c r="C112" s="19" t="s">
         <v>749</v>
       </c>
-      <c r="B112" s="19" t="s">
-        <v>739</v>
-      </c>
-      <c r="C112" s="19" t="s">
+      <c r="D112" s="19" t="s">
         <v>750</v>
       </c>
-      <c r="D112" s="19" t="s">
-        <v>751</v>
-      </c>
       <c r="E112" s="19" t="s">
-        <v>285</v>
+        <v>232</v>
       </c>
       <c r="F112" s="21" t="s">
-        <v>286</v>
-      </c>
-      <c r="G112" s="20" t="s">
-        <v>287</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="G112" s="20"/>
       <c r="H112" s="19"/>
       <c r="I112" s="19" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="J112" s="19"/>
       <c r="K112" s="19"/>
@@ -11572,21 +11573,21 @@
       <c r="R112" s="19"/>
       <c r="S112" s="19"/>
       <c r="T112" s="19" t="s">
-        <v>209</v>
+        <v>752</v>
       </c>
       <c r="U112" s="19" t="s">
-        <v>209</v>
+        <v>752</v>
       </c>
       <c r="V112" s="21"/>
       <c r="W112" s="21"/>
       <c r="X112" s="19" t="s">
-        <v>209</v>
+        <v>752</v>
       </c>
       <c r="Y112" s="19" t="s">
-        <v>209</v>
+        <v>752</v>
       </c>
       <c r="Z112" s="19" t="s">
-        <v>209</v>
+        <v>752</v>
       </c>
       <c r="AA112" s="19"/>
     </row>
@@ -11595,7 +11596,7 @@
         <v>753</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>739</v>
+        <v>748</v>
       </c>
       <c r="C113" s="19" t="s">
         <v>754</v>
@@ -11604,17 +11605,15 @@
         <v>755</v>
       </c>
       <c r="E113" s="19" t="s">
-        <v>205</v>
-      </c>
-      <c r="F113" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="F113" s="21"/>
+      <c r="G113" s="20"/>
+      <c r="H113" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="I113" s="19" t="s">
         <v>756</v>
-      </c>
-      <c r="G113" s="20" t="s">
-        <v>757</v>
-      </c>
-      <c r="H113" s="19"/>
-      <c r="I113" s="19" t="s">
-        <v>758</v>
       </c>
       <c r="J113" s="19"/>
       <c r="K113" s="19"/>
@@ -11626,46 +11625,50 @@
       <c r="Q113" s="19"/>
       <c r="R113" s="19"/>
       <c r="S113" s="19"/>
-      <c r="T113" s="19"/>
-      <c r="U113" s="19"/>
-      <c r="V113" s="19" t="s">
-        <v>272</v>
-      </c>
-      <c r="W113" s="19" t="s">
-        <v>272</v>
-      </c>
+      <c r="T113" s="19" t="s">
+        <v>757</v>
+      </c>
+      <c r="U113" s="19" t="s">
+        <v>757</v>
+      </c>
+      <c r="V113" s="21"/>
+      <c r="W113" s="21"/>
       <c r="X113" s="19" t="s">
-        <v>272</v>
+        <v>757</v>
       </c>
       <c r="Y113" s="19" t="s">
-        <v>272</v>
+        <v>757</v>
       </c>
       <c r="Z113" s="19" t="s">
-        <v>272</v>
+        <v>757</v>
       </c>
       <c r="AA113" s="19"/>
     </row>
     <row r="114" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="19" t="s">
+        <v>758</v>
+      </c>
+      <c r="B114" s="19" t="s">
+        <v>748</v>
+      </c>
+      <c r="C114" s="19" t="s">
         <v>759</v>
       </c>
-      <c r="B114" s="19" t="s">
-        <v>739</v>
-      </c>
-      <c r="C114" s="19" t="s">
+      <c r="D114" s="19" t="s">
         <v>760</v>
       </c>
-      <c r="D114" s="19" t="s">
-        <v>761</v>
-      </c>
       <c r="E114" s="19" t="s">
-        <v>301</v>
-      </c>
-      <c r="F114" s="19"/>
-      <c r="G114" s="20"/>
+        <v>285</v>
+      </c>
+      <c r="F114" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="G114" s="20" t="s">
+        <v>287</v>
+      </c>
       <c r="H114" s="19"/>
       <c r="I114" s="19" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="J114" s="19"/>
       <c r="K114" s="19"/>
@@ -11677,92 +11680,198 @@
       <c r="Q114" s="19"/>
       <c r="R114" s="19"/>
       <c r="S114" s="19"/>
-      <c r="T114" s="19"/>
-      <c r="U114" s="19"/>
-      <c r="V114" s="19"/>
-      <c r="W114" s="19"/>
-      <c r="X114" s="19"/>
+      <c r="T114" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="U114" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="V114" s="21"/>
+      <c r="W114" s="21"/>
+      <c r="X114" s="19" t="s">
+        <v>209</v>
+      </c>
       <c r="Y114" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="Z114" s="19"/>
+        <v>209</v>
+      </c>
+      <c r="Z114" s="19" t="s">
+        <v>209</v>
+      </c>
       <c r="AA114" s="19"/>
     </row>
     <row r="115" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="19" t="s">
+        <v>762</v>
+      </c>
+      <c r="B115" s="19" t="s">
+        <v>748</v>
+      </c>
+      <c r="C115" s="19" t="s">
         <v>763</v>
       </c>
-      <c r="B115" s="19" t="s">
-        <v>739</v>
-      </c>
-      <c r="C115" s="19" t="s">
+      <c r="D115" s="19" t="s">
         <v>764</v>
       </c>
-      <c r="D115" s="19" t="s">
+      <c r="E115" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="F115" s="19" t="s">
         <v>765</v>
       </c>
-      <c r="E115" s="19" t="s">
-        <v>244</v>
-      </c>
-      <c r="F115" s="19" t="s">
-        <v>477</v>
-      </c>
-      <c r="G115" s="20"/>
+      <c r="G115" s="20" t="s">
+        <v>766</v>
+      </c>
       <c r="H115" s="19"/>
       <c r="I115" s="19" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="J115" s="19"/>
-      <c r="K115" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="L115" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="M115" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="N115" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="O115" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="P115" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="Q115" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="R115" s="19" t="s">
-        <v>209</v>
-      </c>
+      <c r="K115" s="19"/>
+      <c r="L115" s="19"/>
+      <c r="M115" s="19"/>
+      <c r="N115" s="19"/>
+      <c r="O115" s="19"/>
+      <c r="P115" s="19"/>
+      <c r="Q115" s="19"/>
+      <c r="R115" s="19"/>
       <c r="S115" s="19"/>
-      <c r="T115" s="19" t="s">
-        <v>209</v>
-      </c>
+      <c r="T115" s="19"/>
       <c r="U115" s="19"/>
       <c r="V115" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="W115" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="X115" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y115" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z115" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA115" s="19"/>
+    </row>
+    <row r="116" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A116" s="19" t="s">
+        <v>768</v>
+      </c>
+      <c r="B116" s="19" t="s">
+        <v>748</v>
+      </c>
+      <c r="C116" s="19" t="s">
+        <v>769</v>
+      </c>
+      <c r="D116" s="19" t="s">
+        <v>770</v>
+      </c>
+      <c r="E116" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="F116" s="19"/>
+      <c r="G116" s="20"/>
+      <c r="H116" s="19"/>
+      <c r="I116" s="19" t="s">
+        <v>771</v>
+      </c>
+      <c r="J116" s="19"/>
+      <c r="K116" s="19"/>
+      <c r="L116" s="19"/>
+      <c r="M116" s="19"/>
+      <c r="N116" s="19"/>
+      <c r="O116" s="19"/>
+      <c r="P116" s="19"/>
+      <c r="Q116" s="19"/>
+      <c r="R116" s="19"/>
+      <c r="S116" s="19"/>
+      <c r="T116" s="19"/>
+      <c r="U116" s="19"/>
+      <c r="V116" s="19"/>
+      <c r="W116" s="19"/>
+      <c r="X116" s="19"/>
+      <c r="Y116" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z116" s="19"/>
+      <c r="AA116" s="19"/>
+    </row>
+    <row r="117" customFormat="false" ht="102.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A117" s="19" t="s">
+        <v>772</v>
+      </c>
+      <c r="B117" s="19" t="s">
+        <v>748</v>
+      </c>
+      <c r="C117" s="19" t="s">
+        <v>773</v>
+      </c>
+      <c r="D117" s="19" t="s">
+        <v>774</v>
+      </c>
+      <c r="E117" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="F117" s="19" t="s">
+        <v>477</v>
+      </c>
+      <c r="G117" s="20"/>
+      <c r="H117" s="19"/>
+      <c r="I117" s="19" t="s">
+        <v>775</v>
+      </c>
+      <c r="J117" s="19"/>
+      <c r="K117" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="W115" s="19" t="s">
+      <c r="L117" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="X115" s="19" t="s">
+      <c r="M117" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="Y115" s="19" t="s">
+      <c r="N117" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="Z115" s="19" t="s">
+      <c r="O117" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="AA115" s="19" t="s">
+      <c r="P117" s="19" t="s">
         <v>209</v>
       </c>
+      <c r="Q117" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="R117" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="S117" s="19"/>
+      <c r="T117" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="U117" s="19"/>
+      <c r="V117" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="W117" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="X117" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y117" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z117" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="AA117" s="19" t="s">
+        <v>209</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="T1:T115"/>
+  <autoFilter ref="T1:T117"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -11828,7 +11937,7 @@
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10"/>
       <c r="B2" s="30" t="s">
-        <v>767</v>
+        <v>776</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -11886,7 +11995,7 @@
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="30"/>
       <c r="B4" s="30" t="s">
-        <v>768</v>
+        <v>777</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -11944,10 +12053,10 @@
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="30"/>
       <c r="B6" s="30" t="s">
-        <v>769</v>
+        <v>778</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>770</v>
+        <v>779</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="30"/>
@@ -11977,7 +12086,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="30" t="s">
-        <v>771</v>
+        <v>780</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -12034,10 +12143,10 @@
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="30"/>
       <c r="B9" s="30" t="s">
-        <v>772</v>
+        <v>781</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>773</v>
+        <v>782</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="30"/>
@@ -12067,11 +12176,11 @@
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="30" t="s">
-        <v>774</v>
+        <v>783</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="30" t="s">
-        <v>775</v>
+        <v>784</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -12126,12 +12235,12 @@
     <row r="12" customFormat="false" ht="118.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="10"/>
       <c r="B12" s="30" t="s">
-        <v>776</v>
+        <v>785</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="21" t="s">
-        <v>777</v>
+        <v>786</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
@@ -12186,14 +12295,14 @@
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
       <c r="B14" s="30" t="s">
-        <v>778</v>
+        <v>787</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>779</v>
+        <v>788</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="21" t="s">
-        <v>780</v>
+        <v>789</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
@@ -12250,10 +12359,10 @@
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
       <c r="D16" s="30" t="s">
-        <v>781</v>
+        <v>790</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>782</v>
+        <v>791</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
@@ -12282,10 +12391,10 @@
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="30" t="s">
-        <v>783</v>
+        <v>792</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>784</v>
+        <v>793</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -12314,10 +12423,10 @@
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
       <c r="D18" s="30" t="s">
-        <v>785</v>
+        <v>794</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>786</v>
+        <v>795</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
@@ -12373,11 +12482,11 @@
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="30" t="s">
-        <v>787</v>
+        <v>796</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="21" t="s">
-        <v>788</v>
+        <v>797</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
@@ -12434,10 +12543,10 @@
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
       <c r="D22" s="30" t="s">
-        <v>781</v>
+        <v>790</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>789</v>
+        <v>798</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
@@ -12466,10 +12575,10 @@
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
       <c r="D23" s="30" t="s">
-        <v>790</v>
+        <v>799</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>791</v>
+        <v>800</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
@@ -12525,11 +12634,11 @@
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="30" t="s">
-        <v>792</v>
+        <v>801</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="21" t="s">
-        <v>793</v>
+        <v>802</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
@@ -12586,10 +12695,10 @@
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="31" t="s">
-        <v>794</v>
+        <v>803</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>795</v>
+        <v>804</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
@@ -12618,10 +12727,10 @@
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="31" t="s">
-        <v>796</v>
+        <v>805</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>797</v>
+        <v>806</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
@@ -12650,10 +12759,10 @@
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
       <c r="D29" s="31" t="s">
-        <v>798</v>
+        <v>807</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>799</v>
+        <v>808</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
@@ -12682,10 +12791,10 @@
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="31" t="s">
-        <v>800</v>
+        <v>809</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>801</v>
+        <v>810</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
@@ -12714,10 +12823,10 @@
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
       <c r="D31" s="31" t="s">
-        <v>802</v>
+        <v>811</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>803</v>
+        <v>812</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
@@ -12773,11 +12882,11 @@
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="30" t="s">
-        <v>804</v>
+        <v>813</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="21" t="s">
-        <v>805</v>
+        <v>814</v>
       </c>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
@@ -12834,10 +12943,10 @@
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
       <c r="D35" s="30" t="s">
-        <v>781</v>
+        <v>790</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>806</v>
+        <v>815</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
@@ -12866,10 +12975,10 @@
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="30" t="s">
-        <v>807</v>
+        <v>816</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>808</v>
+        <v>817</v>
       </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
@@ -12898,10 +13007,10 @@
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
       <c r="D37" s="30" t="s">
-        <v>809</v>
+        <v>818</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>810</v>
+        <v>819</v>
       </c>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
@@ -12930,10 +13039,10 @@
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
       <c r="D38" s="30" t="s">
-        <v>811</v>
+        <v>820</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>812</v>
+        <v>821</v>
       </c>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
@@ -12962,10 +13071,10 @@
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
       <c r="D39" s="30" t="s">
-        <v>813</v>
+        <v>822</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>814</v>
+        <v>823</v>
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
@@ -13021,11 +13130,11 @@
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10" t="s">
-        <v>815</v>
+        <v>824</v>
       </c>
       <c r="D41" s="10"/>
       <c r="E41" s="21" t="s">
-        <v>816</v>
+        <v>825</v>
       </c>
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
@@ -13082,10 +13191,10 @@
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
       <c r="D43" s="30" t="s">
-        <v>781</v>
+        <v>790</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>817</v>
+        <v>826</v>
       </c>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
@@ -13114,10 +13223,10 @@
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
       <c r="D44" s="31" t="s">
-        <v>818</v>
+        <v>827</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>819</v>
+        <v>828</v>
       </c>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
@@ -13146,10 +13255,10 @@
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
       <c r="D45" s="30" t="s">
-        <v>820</v>
+        <v>829</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>821</v>
+        <v>830</v>
       </c>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
@@ -13204,14 +13313,14 @@
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="30"/>
       <c r="B47" s="30" t="s">
-        <v>822</v>
+        <v>831</v>
       </c>
       <c r="C47" s="30" t="s">
-        <v>823</v>
+        <v>832</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="21" t="s">
-        <v>824</v>
+        <v>833</v>
       </c>
       <c r="F47" s="30"/>
       <c r="G47" s="30"/>
@@ -13241,7 +13350,7 @@
       <c r="C48" s="30"/>
       <c r="D48" s="30"/>
       <c r="E48" s="21" t="s">
-        <v>825</v>
+        <v>834</v>
       </c>
       <c r="F48" s="30"/>
       <c r="G48" s="30"/>
@@ -13271,7 +13380,7 @@
       <c r="C49" s="30"/>
       <c r="D49" s="30"/>
       <c r="E49" s="21" t="s">
-        <v>826</v>
+        <v>835</v>
       </c>
       <c r="F49" s="30"/>
       <c r="G49" s="30"/>
@@ -14265,7 +14374,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14308,7 +14417,7 @@
         <v>231</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>827</v>
+        <v>836</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>232</v>
@@ -14328,7 +14437,7 @@
         <v>268</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>828</v>
+        <v>837</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>205</v>
@@ -14348,7 +14457,7 @@
         <v>280</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>829</v>
+        <v>838</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>232</v>
@@ -14368,7 +14477,7 @@
         <v>427</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>830</v>
+        <v>839</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>301</v>
@@ -14385,7 +14494,7 @@
         <v>508</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>831</v>
+        <v>840</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>301</v>
@@ -14402,7 +14511,7 @@
         <v>395</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>832</v>
+        <v>841</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>301</v>
@@ -14419,7 +14528,7 @@
         <v>399</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>832</v>
+        <v>841</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>301</v>
@@ -14436,7 +14545,7 @@
         <v>408</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>833</v>
+        <v>842</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>301</v>
@@ -14444,16 +14553,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>834</v>
+        <v>843</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>835</v>
+        <v>844</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>836</v>
+        <v>845</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>837</v>
+        <v>846</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>301</v>
@@ -14470,7 +14579,7 @@
         <v>368</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>838</v>
+        <v>847</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>301</v>
@@ -14484,10 +14593,10 @@
         <v>431</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>839</v>
+        <v>848</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>840</v>
+        <v>849</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>301</v>
@@ -14495,16 +14604,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>841</v>
+        <v>591</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>842</v>
+        <v>592</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>843</v>
+        <v>593</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>844</v>
+        <v>594</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>301</v>
@@ -14512,16 +14621,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>845</v>
+        <v>595</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>846</v>
+        <v>596</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>847</v>
+        <v>597</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>848</v>
+        <v>598</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>301</v>
@@ -14538,7 +14647,7 @@
         <v>543</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>301</v>
@@ -14546,16 +14655,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>738</v>
+        <v>747</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>740</v>
+        <v>749</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>741</v>
+        <v>750</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>232</v>
@@ -14566,16 +14675,16 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>744</v>
+        <v>753</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>745</v>
+        <v>754</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>746</v>
+        <v>755</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>301</v>
@@ -14592,7 +14701,7 @@
         <v>567</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>232</v>
@@ -14612,7 +14721,7 @@
         <v>502</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="E19" s="0" t="s">
         <v>232</v>
@@ -14675,16 +14784,16 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>232</v>
@@ -14695,16 +14804,16 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>232</v>
@@ -14715,22 +14824,22 @@
     </row>
     <row r="4" customFormat="false" ht="249" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>205</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14744,7 +14853,7 @@
         <v>476</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>244</v>
@@ -14755,16 +14864,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>301</v>
@@ -14772,19 +14881,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>875</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>876</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>874</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>875</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14792,13 +14901,13 @@
         <v>247</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>249</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>244</v>
@@ -14885,16 +14994,16 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>244</v>
@@ -14902,42 +15011,42 @@
     </row>
     <row r="3" customFormat="false" ht="375" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>205</v>
       </c>
       <c r="F3" s="35" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="209.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>205</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Spreadsheet entries for terms for Single boundary BCRSW now corrected , check and create-dictionary.R script run
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisnparr/git/actus-dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08F6B44-040C-2749-89AE-0979F2C0CA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57960695-F83F-DE43-B44B-8DB07118EC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33800" yWindow="500" windowWidth="33600" windowHeight="21000" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35660" yWindow="500" windowWidth="33600" windowHeight="19640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="956">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="956">
   <si>
     <t>The ACTUS Dictionary</t>
   </si>
@@ -3095,9 +3095,6 @@
     <t>BLAF2</t>
   </si>
   <si>
-    <t>Boundary monitoring starts on this date</t>
-  </si>
-  <si>
     <t>Boundary monitoring ends on this date</t>
   </si>
   <si>
@@ -3110,31 +3107,6 @@
     <t>Boundary value in a barrier options contract, when reached, triggers the boundary effect specified e.g. Knock-In or Knock-out</t>
   </si>
   <si>
-    <t>Boundary direction refers to the movement of the underlying asset's price. The direction/trend in which the underlying asset's price is expected to move concerning the boundary value can be set as "INCR" (increasing) or "DECR" (decreasing).
-Eg: The boundary direction set to INCR suggests that the ExternalReferenceIndex could increase and arrive at the boundary value during the monitoring period and Viz-a-viz.</t>
-  </si>
-  <si>
-    <t>This term refers to the impact or changes in the contract when the underlying asset's price crosses a specified boundary value. The boundary effect specifies how the option contract will be adjusted or triggered in response to this event.
-KnockINFirstLeg:
-This term indicates that if the underlying asset's price crosses the boundary value, it triggers the activation of the contract within the first leg. 
-KnockINSecondLeg:
-Similar to KnockINFirstLeg, this term suggests that the crossing of the boundary value triggers the activation of the contract within the second leg.
-KnockOUTCurrentLeg:
-This term implies that if the underlying asset's price crosses the boundary value, it deactivates the contract on the active leg. In other words, the option associated with the current leg is terminated or knocked out.</t>
-  </si>
-  <si>
-    <t>On a given Boundary Monitoring Date, this condition specifies 
-First Leg Active (FIL):
-If this condition is set to FIL on a given Boundary Monitoring Date, it indicates that the first leg of the option structure is active.
-Second Leg Active (SEL):
-If this condition is set to SEL on a given Boundary Monitoring Date, it implies that the second leg of the option structure is active.
-Neither First Leg nor Second Leg Active (Null):
-If the condition is set to Null on a given Boundary Monitoring Date, it suggests that neither the first leg nor the second leg is active. In this case, the option structure does not trigger based on the specified criteria or market conditions, and both legs remain inactive.</t>
-  </si>
-  <si>
-    <t>The frequency with which boundary monitoring events occur. It defines how often the system checks or evaluates the conditions related to boundary values. For example, if the cycle is set to a day, the monitoring events might occur daily.</t>
-  </si>
-  <si>
     <t>A barrier option is a derivative contract that is activated (knocked in) or extinguished (knocked out) when the asset price reaches a barrier. The underlying asset may be a stock, index, or exchange-traded fund.Two boundary switches can be controlled.</t>
   </si>
   <si>
@@ -3189,22 +3161,36 @@
     <t>How do we express the direcion? Our assumption is, that the CNTRL of the child contracts must be set correctly</t>
   </si>
   <si>
-    <t xml:space="preserve">option: 0, identifier: fromBelow, name: From Below, acronym: INCR, description: Boundary action if observed market object value greater than or equal to boundary value at a monitor time.
-option: 1  identifier: fromAbove, name: From Above, acronym: DECR, description: Boundary action if observed market object value less than or equal to boundary value at a monitor time.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">option: 0, identifier: firstLeg, name: First Leg, acronym: FIL, description: the first leg is active when boundary controlled switch contract starts.
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">option: 0, identifier: fromBelow, name: From Below, acronym: INCR, description: Boundary effect is trigerred if the observed underlying asset value is greater than or equal to the boundary value at a monitor time.
+option: 1,  identifier: fromAbove, name: From Above, acronym: DECR, description: Boundary action if observed market object value less than or equal to boundary value at a monitor time.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boundary direction specifies the direction of motion in the underlying asset's price which will be considered a valid crossing of the boundary and trigger the boundary effect changing which, if any, of the boundary legs is  active.  </t>
+  </si>
+  <si>
+    <t>option: 0, identifier: knockINFirstLeg, name: KnockIN First Leg, acronym: INFIL, description: effect of boundary crossing is to knock IN the first leg making this the active contract; monitoring of the boundary stops.
+option: 1, identifier: knockINSecondLeg, name: KnockIN Second Leg, acronym: INSEL, description: effect of boundary crossing is to knock IN the Second Leg making this the active contract; monitoring of the boundary stops.
+option: 2, identifier: knockOUTCurrentLeg, name: KnockOUT Current Leg, acronym: OUT, description: effect of boundary crossing is to knockOUT any active contract so there is no active contract after the boundary crossing; monitoring of the boundary stops.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifies which leg - if any - is the active contract  in effect when the boundary controlled switch contract starts.  </t>
+  </si>
+  <si>
+    <t>The first Boundary monitoring event occurs on this date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">option: 0, identifier: firstLeg, name: First Leg, acronym: FIL, description: the first leg is active when the boundary controlled switch contract is initialized.
 option: 1, identifier: secondLeg, name: Second Leg, acronym: SEL, description: the second leg is active when the boundary controlled switch contract starts.
-option: 2, identifier: Null, name: Null, acronym: Null, description: there is nnactive subcontract when the boundary controlled switch starts subcontract when the boundary controlled switch starts. </t>
-  </si>
-  <si>
-    <t>option: 0, identifier: knockINFirstLeg, name: KnockIN First Leg, acronym: INFIL, description: effect of boundary crossing is to knock IN the first leg making this the active contract; monitoring of the boundary stops.
-option: 1, identifier: knockINSecondLeg, name: KnockIN Second Leg, acronym: INSEL, description: effect of boundary crossing os to knock IN the Second Leg making this the active contract; monitoring of the boundary stops.
-option: 2, identifier: knockOUTCurrentLeg, name: KnockOUT Current Leg, acronym:
-OUT, description: effect of boundary crossing is to knockOUT any active contractso there is no active contract after the boundary crossing; monitoring of the boundary stops.</t>
-  </si>
-  <si>
-    <t>Boolean</t>
+option: 2, identifier: Null, name: Null, acronym: Null, description: there is no active subcontract when the boundary controlled switch contract starts. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The frequency with which boundary monitoring events occur. It defines how often the system checks to test whether the  market value of the underlying asset has crossed the boundary in the specified direction triggerring  a boundary crossing event. </t>
+  </si>
+  <si>
+    <t>This term specifies which leg - if any-  becomes the active subcontract  when the underlying asset's price crosses the specified boundary value in the specified direction triggerring a boundary crossing event.</t>
   </si>
 </sst>
 </file>
@@ -3480,7 +3466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3631,6 +3617,12 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3644,12 +3636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5941,10 +5928,10 @@
         <v>122</v>
       </c>
       <c r="F34" s="44" t="s">
-        <v>934</v>
+        <v>929</v>
       </c>
       <c r="G34" s="44" t="s">
-        <v>935</v>
+        <v>930</v>
       </c>
       <c r="H34" s="45" t="s">
         <v>103</v>
@@ -5961,11 +5948,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC132"/>
+  <dimension ref="A1:AC131"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I120" sqref="I120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6078,7 +6065,7 @@
         <v>205</v>
       </c>
       <c r="AB1" s="50" t="s">
-        <v>936</v>
+        <v>931</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6634,10 +6621,10 @@
         <v>239</v>
       </c>
       <c r="AB8" s="51" t="s">
-        <v>937</v>
+        <v>932</v>
       </c>
       <c r="AC8" s="52" t="s">
-        <v>938</v>
+        <v>933</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6921,10 +6908,10 @@
         <v>239</v>
       </c>
       <c r="AB12" s="51" t="s">
-        <v>937</v>
+        <v>932</v>
       </c>
       <c r="AC12" s="52" t="s">
-        <v>938</v>
+        <v>933</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7001,8 +6988,8 @@
       <c r="AA13" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB13" s="59" t="s">
-        <v>939</v>
+      <c r="AB13" s="63" t="s">
+        <v>934</v>
       </c>
       <c r="AC13" s="52"/>
     </row>
@@ -7076,7 +7063,7 @@
       <c r="AA14" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB14" s="60"/>
+      <c r="AB14" s="64"/>
     </row>
     <row r="15" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
@@ -7150,7 +7137,7 @@
       <c r="AA15" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB15" s="60"/>
+      <c r="AB15" s="64"/>
     </row>
     <row r="16" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
@@ -7210,7 +7197,7 @@
       <c r="Y16" s="23"/>
       <c r="Z16" s="23"/>
       <c r="AA16" s="23"/>
-      <c r="AB16" s="60"/>
+      <c r="AB16" s="64"/>
     </row>
     <row r="17" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
@@ -7284,7 +7271,7 @@
       <c r="AA17" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB17" s="60"/>
+      <c r="AB17" s="64"/>
     </row>
     <row r="18" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
@@ -7358,7 +7345,7 @@
       <c r="AA18" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB18" s="60"/>
+      <c r="AB18" s="64"/>
     </row>
     <row r="19" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
@@ -7432,7 +7419,7 @@
       <c r="AA19" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB19" s="60"/>
+      <c r="AB19" s="64"/>
     </row>
     <row r="20" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
@@ -9699,10 +9686,10 @@
       <c r="Z62" s="23"/>
       <c r="AA62" s="23"/>
       <c r="AB62" s="53" t="s">
-        <v>941</v>
+        <v>936</v>
       </c>
       <c r="AC62" s="52" t="s">
-        <v>940</v>
+        <v>935</v>
       </c>
     </row>
     <row r="63" spans="1:29" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -10294,10 +10281,10 @@
         <v>573</v>
       </c>
       <c r="AB73" s="53" t="s">
-        <v>942</v>
-      </c>
-      <c r="AC73" s="61" t="s">
-        <v>944</v>
+        <v>937</v>
+      </c>
+      <c r="AC73" s="65" t="s">
+        <v>939</v>
       </c>
     </row>
     <row r="74" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10373,9 +10360,9 @@
         <v>578</v>
       </c>
       <c r="AB74" s="53" t="s">
-        <v>943</v>
-      </c>
-      <c r="AC74" s="62"/>
+        <v>938</v>
+      </c>
+      <c r="AC74" s="66"/>
     </row>
     <row r="75" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
@@ -12672,17 +12659,17 @@
         <v>305</v>
       </c>
       <c r="F118" s="34"/>
-      <c r="H118" s="58" t="s">
-        <v>951</v>
+      <c r="H118" s="67" t="s">
+        <v>946</v>
       </c>
       <c r="I118" s="49" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="AB118" s="53" t="s">
-        <v>945</v>
+        <v>940</v>
       </c>
       <c r="AC118" s="57" t="s">
-        <v>946</v>
+        <v>941</v>
       </c>
     </row>
     <row r="119" spans="1:29" ht="148" customHeight="1" x14ac:dyDescent="0.2">
@@ -12702,17 +12689,17 @@
         <v>209</v>
       </c>
       <c r="F119" s="49" t="s">
-        <v>952</v>
-      </c>
-      <c r="H119" s="58"/>
+        <v>948</v>
+      </c>
+      <c r="H119" s="62"/>
       <c r="I119" s="49" t="s">
-        <v>930</v>
+        <v>949</v>
       </c>
       <c r="AB119" s="53" t="s">
-        <v>948</v>
+        <v>943</v>
       </c>
       <c r="AC119" s="56" t="s">
-        <v>947</v>
+        <v>942</v>
       </c>
     </row>
     <row r="120" spans="1:29" ht="243" customHeight="1" x14ac:dyDescent="0.2">
@@ -12732,14 +12719,14 @@
         <v>209</v>
       </c>
       <c r="F120" s="49" t="s">
-        <v>954</v>
-      </c>
-      <c r="H120" s="58"/>
+        <v>950</v>
+      </c>
+      <c r="H120" s="62"/>
       <c r="I120" s="49" t="s">
-        <v>931</v>
+        <v>955</v>
       </c>
       <c r="AC120" s="55" t="s">
-        <v>949</v>
+        <v>944</v>
       </c>
     </row>
     <row r="121" spans="1:29" ht="186" customHeight="1" x14ac:dyDescent="0.2">
@@ -12762,11 +12749,11 @@
         <v>953</v>
       </c>
       <c r="G121" t="s">
-        <v>950</v>
-      </c>
-      <c r="H121" s="58"/>
+        <v>945</v>
+      </c>
+      <c r="H121" s="62"/>
       <c r="I121" s="49" t="s">
-        <v>932</v>
+        <v>951</v>
       </c>
       <c r="AB121" s="53" t="s">
         <v>213</v>
@@ -12791,9 +12778,9 @@
       <c r="F122" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="H122" s="58"/>
+      <c r="H122" s="62"/>
       <c r="I122" s="49" t="s">
-        <v>925</v>
+        <v>952</v>
       </c>
       <c r="AB122" s="53" t="s">
         <v>232</v>
@@ -12818,77 +12805,64 @@
       <c r="F123" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="H123" s="58"/>
+      <c r="H123" s="62"/>
       <c r="I123" s="49" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="AB123" s="53" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="124" spans="1:29" ht="48" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:29" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="34" t="s">
         <v>792</v>
       </c>
       <c r="B124" s="34" t="s">
         <v>922</v>
       </c>
-      <c r="C124" s="48" t="s">
+      <c r="C124" s="34" t="s">
         <v>793</v>
       </c>
       <c r="D124" s="34" t="s">
         <v>921</v>
       </c>
-      <c r="E124" s="35" t="s">
-        <v>334</v>
-      </c>
-      <c r="F124" s="36" t="s">
-        <v>335</v>
-      </c>
-      <c r="H124" s="58"/>
+      <c r="E124" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="F124" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="G124" s="34"/>
+      <c r="H124" s="34"/>
       <c r="I124" s="49" t="s">
-        <v>933</v>
-      </c>
-      <c r="AB124" s="53" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A125" s="34"/>
-      <c r="B125" s="34"/>
-      <c r="C125" s="34"/>
-      <c r="D125" s="34"/>
-      <c r="E125" s="34"/>
-      <c r="F125" s="34"/>
-      <c r="G125" s="34"/>
-      <c r="H125" s="34"/>
-      <c r="I125" s="49"/>
+        <v>954</v>
+      </c>
+    </row>
+    <row r="126" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="F126" s="36"/>
     </row>
     <row r="127" spans="1:29" x14ac:dyDescent="0.2">
       <c r="F127" s="36"/>
     </row>
     <row r="128" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="D128" s="30"/>
       <c r="F128" s="36"/>
     </row>
-    <row r="129" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D129" s="30"/>
+    <row r="129" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F129" s="36"/>
     </row>
-    <row r="130" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="F130" s="36"/>
-    </row>
-    <row r="131" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F130" s="37"/>
+      <c r="G130" s="30"/>
+    </row>
+    <row r="131" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F131" s="37"/>
       <c r="G131" s="30"/>
-    </row>
-    <row r="132" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="F132" s="37"/>
-      <c r="G132" s="30"/>
     </row>
   </sheetData>
   <autoFilter ref="T1:T117" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <mergeCells count="3">
-    <mergeCell ref="H118:H124"/>
+    <mergeCell ref="H118:H123"/>
     <mergeCell ref="AB13:AB19"/>
     <mergeCell ref="AC73:AC74"/>
   </mergeCells>
@@ -15374,7 +15348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -15408,414 +15382,414 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="58" t="s">
         <v>233</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="58" t="s">
         <v>234</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="58" t="s">
         <v>235</v>
       </c>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="58" t="s">
         <v>854</v>
       </c>
-      <c r="E2" s="63" t="s">
+      <c r="E2" s="58" t="s">
         <v>236</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="59" t="s">
         <v>237</v>
       </c>
-      <c r="G2" s="64"/>
+      <c r="G2" s="59"/>
     </row>
     <row r="3" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="58" t="s">
         <v>270</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="58" t="s">
         <v>271</v>
       </c>
-      <c r="C3" s="63" t="s">
+      <c r="C3" s="58" t="s">
         <v>272</v>
       </c>
-      <c r="D3" s="63" t="s">
+      <c r="D3" s="58" t="s">
         <v>855</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="E3" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="60" t="s">
         <v>273</v>
       </c>
-      <c r="G3" s="64"/>
+      <c r="G3" s="59"/>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="58" t="s">
         <v>282</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="58" t="s">
         <v>283</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="58" t="s">
         <v>284</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="58" t="s">
         <v>856</v>
       </c>
-      <c r="E4" s="63" t="s">
+      <c r="E4" s="58" t="s">
         <v>236</v>
       </c>
-      <c r="F4" s="64" t="s">
+      <c r="F4" s="59" t="s">
         <v>237</v>
       </c>
-      <c r="G4" s="64"/>
+      <c r="G4" s="59"/>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="58" t="s">
         <v>508</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="58" t="s">
         <v>478</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="58" t="s">
         <v>431</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="58" t="s">
         <v>857</v>
       </c>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="F5" s="64"/>
-      <c r="G5" s="64"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="58" t="s">
         <v>510</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="58" t="s">
         <v>511</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="58" t="s">
         <v>512</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="58" t="s">
         <v>858</v>
       </c>
-      <c r="E6" s="63" t="s">
+      <c r="E6" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="58" t="s">
         <v>397</v>
       </c>
-      <c r="B7" s="63" t="s">
+      <c r="B7" s="58" t="s">
         <v>398</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="58" t="s">
         <v>399</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="58" t="s">
         <v>859</v>
       </c>
-      <c r="E7" s="63" t="s">
+      <c r="E7" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="63" t="s">
+      <c r="A8" s="58" t="s">
         <v>401</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="B8" s="58" t="s">
         <v>402</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="58" t="s">
         <v>403</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="58" t="s">
         <v>859</v>
       </c>
-      <c r="E8" s="63" t="s">
+      <c r="E8" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="58" t="s">
         <v>410</v>
       </c>
-      <c r="B9" s="63" t="s">
+      <c r="B9" s="58" t="s">
         <v>411</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="58" t="s">
         <v>412</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="58" t="s">
         <v>860</v>
       </c>
-      <c r="E9" s="63" t="s">
+      <c r="E9" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
     </row>
     <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="63" t="s">
+      <c r="A10" s="58" t="s">
         <v>861</v>
       </c>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="58" t="s">
         <v>862</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="58" t="s">
         <v>863</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="58" t="s">
         <v>864</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
     </row>
     <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="58" t="s">
         <v>370</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="58" t="s">
         <v>371</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="58" t="s">
         <v>372</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="58" t="s">
         <v>865</v>
       </c>
-      <c r="E11" s="63" t="s">
+      <c r="E11" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="F11" s="64"/>
-      <c r="G11" s="64"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
     </row>
     <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="58" t="s">
         <v>434</v>
       </c>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="58" t="s">
         <v>435</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="58" t="s">
         <v>866</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="58" t="s">
         <v>867</v>
       </c>
-      <c r="E12" s="63" t="s">
+      <c r="E12" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
     </row>
     <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="58" t="s">
         <v>595</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="58" t="s">
         <v>596</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="58" t="s">
         <v>597</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="58" t="s">
         <v>598</v>
       </c>
-      <c r="E13" s="63" t="s">
+      <c r="E13" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
     </row>
     <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="63" t="s">
+      <c r="A14" s="58" t="s">
         <v>599</v>
       </c>
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="58" t="s">
         <v>600</v>
       </c>
-      <c r="C14" s="63" t="s">
+      <c r="C14" s="58" t="s">
         <v>601</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="58" t="s">
         <v>602</v>
       </c>
-      <c r="E14" s="63" t="s">
+      <c r="E14" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
     </row>
     <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="63" t="s">
+      <c r="A15" s="58" t="s">
         <v>545</v>
       </c>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="58" t="s">
         <v>546</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="58" t="s">
         <v>547</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="58" t="s">
         <v>868</v>
       </c>
-      <c r="E15" s="63" t="s">
+      <c r="E15" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="63" t="s">
+      <c r="A16" s="58" t="s">
         <v>751</v>
       </c>
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="58" t="s">
         <v>753</v>
       </c>
-      <c r="C16" s="63" t="s">
+      <c r="C16" s="58" t="s">
         <v>754</v>
       </c>
-      <c r="D16" s="63" t="s">
+      <c r="D16" s="58" t="s">
         <v>869</v>
       </c>
-      <c r="E16" s="63" t="s">
+      <c r="E16" s="58" t="s">
         <v>236</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="59" t="s">
         <v>237</v>
       </c>
-      <c r="G16" s="64"/>
+      <c r="G16" s="59"/>
     </row>
     <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="63" t="s">
+      <c r="A17" s="58" t="s">
         <v>757</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="58" t="s">
         <v>758</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="58" t="s">
         <v>759</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="58" t="s">
         <v>870</v>
       </c>
-      <c r="E17" s="63" t="s">
+      <c r="E17" s="58" t="s">
         <v>305</v>
       </c>
-      <c r="F17" s="64"/>
-      <c r="G17" s="64"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="63" t="s">
+      <c r="A18" s="58" t="s">
         <v>569</v>
       </c>
-      <c r="B18" s="63" t="s">
+      <c r="B18" s="58" t="s">
         <v>570</v>
       </c>
-      <c r="C18" s="63" t="s">
+      <c r="C18" s="58" t="s">
         <v>571</v>
       </c>
-      <c r="D18" s="63" t="s">
+      <c r="D18" s="58" t="s">
         <v>871</v>
       </c>
-      <c r="E18" s="63" t="s">
+      <c r="E18" s="58" t="s">
         <v>236</v>
       </c>
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="59" t="s">
         <v>237</v>
       </c>
-      <c r="G18" s="64"/>
+      <c r="G18" s="59"/>
     </row>
     <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="64" t="s">
+      <c r="A19" s="59" t="s">
         <v>504</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="59" t="s">
         <v>505</v>
       </c>
-      <c r="C19" s="64" t="s">
+      <c r="C19" s="59" t="s">
         <v>506</v>
       </c>
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="59" t="s">
         <v>872</v>
       </c>
-      <c r="E19" s="64" t="s">
+      <c r="E19" s="59" t="s">
         <v>236</v>
       </c>
-      <c r="F19" s="64" t="s">
+      <c r="F19" s="59" t="s">
         <v>237</v>
       </c>
-      <c r="G19" s="64"/>
+      <c r="G19" s="59"/>
     </row>
     <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="64"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
+      <c r="A20" s="59"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
     </row>
     <row r="21" spans="1:7" s="34" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="61" t="s">
         <v>873</v>
       </c>
-      <c r="B21" s="66" t="s">
+      <c r="B21" s="61" t="s">
         <v>874</v>
       </c>
-      <c r="C21" s="66" t="s">
+      <c r="C21" s="61" t="s">
         <v>923</v>
       </c>
-      <c r="D21" s="66" t="s">
+      <c r="D21" s="61" t="s">
+        <v>926</v>
+      </c>
+      <c r="E21" s="61" t="s">
+        <v>947</v>
+      </c>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+    </row>
+    <row r="22" spans="1:7" s="34" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="61" t="s">
+        <v>875</v>
+      </c>
+      <c r="B22" s="61" t="s">
+        <v>876</v>
+      </c>
+      <c r="C22" s="61" t="s">
+        <v>924</v>
+      </c>
+      <c r="D22" s="61" t="s">
         <v>927</v>
       </c>
-      <c r="E21" s="66" t="s">
-        <v>955</v>
-      </c>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-    </row>
-    <row r="22" spans="1:7" s="34" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="66" t="s">
-        <v>875</v>
-      </c>
-      <c r="B22" s="66" t="s">
-        <v>876</v>
-      </c>
-      <c r="C22" s="66" t="s">
-        <v>924</v>
-      </c>
-      <c r="D22" s="66" t="s">
-        <v>928</v>
-      </c>
-      <c r="E22" s="66" t="s">
-        <v>955</v>
-      </c>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
+      <c r="E22" s="61" t="s">
+        <v>947</v>
+      </c>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="64"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="64"/>
-      <c r="G23" s="64"/>
+      <c r="A23" s="59"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
TAxonomy for BCRSW updated: single BCRSW only ( at this time ) defined and implemented. Changes to description Terms minor corrections; states BoundaryCrossedFlag added. descriptions of BoundaryLeg(X=1,2)ActiveFlag corrected Events: new event types for BCRSW:  BoundaryMonitoring event  and Boundary event
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisnparr/git/actus-dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57960695-F83F-DE43-B44B-8DB07118EC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A535EE-27B5-5244-926F-DED00A1A2725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35660" yWindow="500" windowWidth="33600" windowHeight="19640" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35660" yWindow="500" windowWidth="33600" windowHeight="19640" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="956">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2184" uniqueCount="959">
   <si>
     <t>The ACTUS Dictionary</t>
   </si>
@@ -2958,7 +2958,228 @@
     <t>The type of the event. Different types have their own business logic in terms of payoff and state transition functions</t>
   </si>
   <si>
-    <t>option: 0, identifier: monitoring, name: Monitoring, acronym: AD, description: Monitoring of contract. Evaluates all contract states, sequence: 22
+    <t>The currency in which the event payoff is scheduled</t>
+  </si>
+  <si>
+    <t>payoff</t>
+  </si>
+  <si>
+    <t>Payoff</t>
+  </si>
+  <si>
+    <t>PYO</t>
+  </si>
+  <si>
+    <t>The event payoff (if any). Is zero if no payoff needs be settled for the event</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>EVS</t>
+  </si>
+  <si>
+    <t>The post-event state. Results from applying the event’s state transition function to the pre-event state</t>
+  </si>
+  <si>
+    <t>Contract ID</t>
+  </si>
+  <si>
+    <t>The Contract ID of the contract which created the event.</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>OBJ</t>
+  </si>
+  <si>
+    <t>The referencing object</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Reference Type</t>
+  </si>
+  <si>
+    <t>RTP</t>
+  </si>
+  <si>
+    <t>The type of the referencing object</t>
+  </si>
+  <si>
+    <t>option: 0, identifier: contract, name: Contract, acronym: CNT, description: The reference represents an actual contract
+option: 1, identifier: contractIdentifier, name: Contract Identifier, acronym: CID, description: The reference represents an identifier of an actual contract
+option: 2, identifier: marketObjectIdentifier, name: Market Object Identifier, acronym: MOC, description: The reference represents the identifier of a market object
+option: 3, identifier: legalEntityIdentifier, name: Legal Entity Identifier, acronym: EID, description: The reference represents the identifier of a legal entity
+option: 4, identifier: contractStructure, name: Contract Structure, acronym: CST, description: The reference represents a ContractStructure</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>Reference Role</t>
+  </si>
+  <si>
+    <t>RRL</t>
+  </si>
+  <si>
+    <t>The role of the referencing object</t>
+  </si>
+  <si>
+    <t>option: 0, identifier: underlying, name: Underlying, acronym: UDL, description: The reference represents a simple underlyer contract
+option: 1, identifier: firstLeg, name: First Leg, acronym: FIL, description: The reference represents the first leg contract
+option: 2, identifier: secondLeg, name: Second Leg, acronym: SEL, description: The reference represents the second leg contract
+option: 3, identifier: coveredContract, name: Covered Contract, acronym: COVE, description: The reference represents a contract that is covered under the parent contract
+option: 4, identifier: coveringContract, name: Covering Contract, acronym: COVI, description: The reference represents a contract that covers for covering contracts under the parent contract Contract</t>
+  </si>
+  <si>
+    <t>BV</t>
+  </si>
+  <si>
+    <t>BDR</t>
+  </si>
+  <si>
+    <t>BEF</t>
+  </si>
+  <si>
+    <t>BLIA</t>
+  </si>
+  <si>
+    <t>BMANX</t>
+  </si>
+  <si>
+    <t>BMED</t>
+  </si>
+  <si>
+    <t>BMCL</t>
+  </si>
+  <si>
+    <t>Barrier</t>
+  </si>
+  <si>
+    <t>BLAF1</t>
+  </si>
+  <si>
+    <t>BLAF2</t>
+  </si>
+  <si>
+    <t>Boundary monitoring ends on this date</t>
+  </si>
+  <si>
+    <t>Boundary value in a barrier options contract, when reached, triggers the boundary effect specified e.g. Knock-In or Knock-out</t>
+  </si>
+  <si>
+    <t>BoundaryControlledSwitch</t>
+  </si>
+  <si>
+    <t>NN?</t>
+  </si>
+  <si>
+    <t>dbd with Francis under the new contractStructure</t>
+  </si>
+  <si>
+    <t>This entire group is under discussion with respect to the new conractStructure</t>
+  </si>
+  <si>
+    <t>Tbd with Francis</t>
+  </si>
+  <si>
+    <t>x?</t>
+  </si>
+  <si>
+    <t>x(1,0,1)</t>
+  </si>
+  <si>
+    <t>NN(1,1,1)</t>
+  </si>
+  <si>
+    <t>The parent child relationship needs to be discussed</t>
+  </si>
+  <si>
+    <t>NN(2,???</t>
+  </si>
+  <si>
+    <t>tbd is this a third attribute or the same as Boundary 1 Value? Also needs a new conditionality saying it has to be set in case where it exists.</t>
+  </si>
+  <si>
+    <t>We do not see the attributes on the code level</t>
+  </si>
+  <si>
+    <t>NN(3,???</t>
+  </si>
+  <si>
+    <t>Is there for example no knockOutFirst leg? What is "current" leg.</t>
+  </si>
+  <si>
+    <t>How do we express the direcion? Our assumption is, that the CNTRL of the child contracts must be set correctly</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">option: 0, identifier: fromBelow, name: From Below, acronym: INCR, description: Boundary effect is trigerred if the observed underlying asset value is greater than or equal to the boundary value at a monitor time.
+option: 1,  identifier: fromAbove, name: From Above, acronym: DECR, description: Boundary action if observed market object value less than or equal to boundary value at a monitor time.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boundary direction specifies the direction of motion in the underlying asset's price which will be considered a valid crossing of the boundary and trigger the boundary effect changing which, if any, of the boundary legs is  active.  </t>
+  </si>
+  <si>
+    <t>option: 0, identifier: knockINFirstLeg, name: KnockIN First Leg, acronym: INFIL, description: effect of boundary crossing is to knock IN the first leg making this the active contract; monitoring of the boundary stops.
+option: 1, identifier: knockINSecondLeg, name: KnockIN Second Leg, acronym: INSEL, description: effect of boundary crossing is to knock IN the Second Leg making this the active contract; monitoring of the boundary stops.
+option: 2, identifier: knockOUTCurrentLeg, name: KnockOUT Current Leg, acronym: OUT, description: effect of boundary crossing is to knockOUT any active contract so there is no active contract after the boundary crossing; monitoring of the boundary stops.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specifies which leg - if any - is the active contract  in effect when the boundary controlled switch contract starts.  </t>
+  </si>
+  <si>
+    <t>The first Boundary monitoring event occurs on this date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">option: 0, identifier: firstLeg, name: First Leg, acronym: FIL, description: the first leg is active when the boundary controlled switch contract is initialized.
+option: 1, identifier: secondLeg, name: Second Leg, acronym: SEL, description: the second leg is active when the boundary controlled switch contract starts.
+option: 2, identifier: Null, name: Null, acronym: Null, description: there is no active subcontract when the boundary controlled switch contract starts. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The frequency with which boundary monitoring events occur. It defines how often the system checks to test whether the  market value of the underlying asset has crossed the boundary in the specified direction triggerring  a boundary crossing event. </t>
+  </si>
+  <si>
+    <t>This term specifies which leg - if any-  becomes the active subcontract  when the underlying asset's price crosses the specified boundary value in the specified direction triggerring a boundary crossing event.</t>
+  </si>
+  <si>
+    <t>A boundary controlled switch is a derivative contract with subcontract legs which can be activated (knocked in) or extinguished (knocked out) when the underlying asset price reaches a specified value.  The underlying asset may be a stock, index, or exchange-traded fund. Boundary controlled switch contracts with a single boundary are currently defined.</t>
+  </si>
+  <si>
+    <t>boundaryCrossedFlag</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TRUE value indicates that boundaryLeg1 is currently active and generating cashflow events. </t>
+  </si>
+  <si>
+    <t>TRUE value indicates that boundaryLeg2 is currently active and generating cashflow events.</t>
+  </si>
+  <si>
+    <t>Boundary Crossed Flag</t>
+  </si>
+  <si>
+    <t>BCF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE value indicates that a boundary crossing event has already occurred; boundary monitoring is no longer in effect. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knock-in and Knock-out barrier options with a single boundary. Bonus contracts with payout when underlying asset price remains above or below a specified level for specified period. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">option: 0, identifier: monitoring, name: Monitoring, acronym: AD, description: Monitoring of contract. Evaluates all contract states, sequence: 22
 option: 1, identifier: initialExchange, name: Initial Exchange, acronym: IED, description: Scheduled date of initial exchange of e.g. principal value in fixed income products, sequence: 1
 Option: 2, identifier: feePayment, name: Fee Payment, acronym: FP, description: Scheduled fee payments, sequence: 2
 option: 3, identifier: principalRedemption, name: Principal Redemption, acronym: PR, description: Scheduled principal redemption payment, sequence: 3
@@ -2979,218 +3200,19 @@
 option: 18, identifier: interestCalculationBaseFixing, name: Interest Calculation Base Fixing, acronym: IPCB, description: Scheduled fixing of the interest calculation base, sequence: 18
 option: 19, identifier: maturity, name: Maturity, acronym: MD, description: Maturity of a contract, sequence: 19
 option: 20, identifier: exercise, name: Exercise, acronym: XD, description: Exercise of a contractual feature such as an optionality, sequence: 20
-option: 21, identifier: settlement, name: Settlement, acronym: STD, description: Settlement of an exercised contractual claim, sequence: 21</t>
-  </si>
-  <si>
-    <t>The currency in which the event payoff is scheduled</t>
-  </si>
-  <si>
-    <t>payoff</t>
-  </si>
-  <si>
-    <t>Payoff</t>
-  </si>
-  <si>
-    <t>PYO</t>
-  </si>
-  <si>
-    <t>The event payoff (if any). Is zero if no payoff needs be settled for the event</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>EVS</t>
-  </si>
-  <si>
-    <t>The post-event state. Results from applying the event’s state transition function to the pre-event state</t>
-  </si>
-  <si>
-    <t>Contract ID</t>
-  </si>
-  <si>
-    <t>The Contract ID of the contract which created the event.</t>
-  </si>
-  <si>
-    <t>object</t>
-  </si>
-  <si>
-    <t>Object</t>
-  </si>
-  <si>
-    <t>OBJ</t>
-  </si>
-  <si>
-    <t>The referencing object</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>Reference Type</t>
-  </si>
-  <si>
-    <t>RTP</t>
-  </si>
-  <si>
-    <t>The type of the referencing object</t>
-  </si>
-  <si>
-    <t>option: 0, identifier: contract, name: Contract, acronym: CNT, description: The reference represents an actual contract
-option: 1, identifier: contractIdentifier, name: Contract Identifier, acronym: CID, description: The reference represents an identifier of an actual contract
-option: 2, identifier: marketObjectIdentifier, name: Market Object Identifier, acronym: MOC, description: The reference represents the identifier of a market object
-option: 3, identifier: legalEntityIdentifier, name: Legal Entity Identifier, acronym: EID, description: The reference represents the identifier of a legal entity
-option: 4, identifier: contractStructure, name: Contract Structure, acronym: CST, description: The reference represents a ContractStructure</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>Reference Role</t>
-  </si>
-  <si>
-    <t>RRL</t>
-  </si>
-  <si>
-    <t>The role of the referencing object</t>
-  </si>
-  <si>
-    <t>option: 0, identifier: underlying, name: Underlying, acronym: UDL, description: The reference represents a simple underlyer contract
-option: 1, identifier: firstLeg, name: First Leg, acronym: FIL, description: The reference represents the first leg contract
-option: 2, identifier: secondLeg, name: Second Leg, acronym: SEL, description: The reference represents the second leg contract
-option: 3, identifier: coveredContract, name: Covered Contract, acronym: COVE, description: The reference represents a contract that is covered under the parent contract
-option: 4, identifier: coveringContract, name: Covering Contract, acronym: COVI, description: The reference represents a contract that covers for covering contracts under the parent contract Contract</t>
-  </si>
-  <si>
-    <t>BV</t>
-  </si>
-  <si>
-    <t>BDR</t>
-  </si>
-  <si>
-    <t>BEF</t>
-  </si>
-  <si>
-    <t>BLIA</t>
-  </si>
-  <si>
-    <t>BMANX</t>
-  </si>
-  <si>
-    <t>BMED</t>
-  </si>
-  <si>
-    <t>BMCL</t>
-  </si>
-  <si>
-    <t>Barrier</t>
-  </si>
-  <si>
-    <t>BLAF1</t>
-  </si>
-  <si>
-    <t>BLAF2</t>
-  </si>
-  <si>
-    <t>Boundary monitoring ends on this date</t>
-  </si>
-  <si>
-    <t>A boolean state variable boundaryMonitoringFlag with values {TRUE, FALSE} denotes whether boundary monitoring is currently active on the Leg1of BRCSW contract</t>
-  </si>
-  <si>
-    <t>A boolean state variable boundaryMonitoringFlag with values {TRUE, FALSE} denotes whether boundary monitoring is currently active on the Leg1of BRCSW contract.</t>
-  </si>
-  <si>
-    <t>Boundary value in a barrier options contract, when reached, triggers the boundary effect specified e.g. Knock-In or Knock-out</t>
-  </si>
-  <si>
-    <t>A barrier option is a derivative contract that is activated (knocked in) or extinguished (knocked out) when the asset price reaches a barrier. The underlying asset may be a stock, index, or exchange-traded fund.Two boundary switches can be controlled.</t>
-  </si>
-  <si>
-    <t>Knock-in and Knock-out options with maximum two boundaries</t>
-  </si>
-  <si>
-    <t>BoundaryControlledSwitch</t>
-  </si>
-  <si>
-    <t>NN?</t>
-  </si>
-  <si>
-    <t>dbd with Francis under the new contractStructure</t>
-  </si>
-  <si>
-    <t>This entire group is under discussion with respect to the new conractStructure</t>
-  </si>
-  <si>
-    <t>Tbd with Francis</t>
-  </si>
-  <si>
-    <t>x?</t>
-  </si>
-  <si>
-    <t>x(1,0,1)</t>
-  </si>
-  <si>
-    <t>NN(1,1,1)</t>
-  </si>
-  <si>
-    <t>The parent child relationship needs to be discussed</t>
-  </si>
-  <si>
-    <t>NN(2,???</t>
-  </si>
-  <si>
-    <t>tbd is this a third attribute or the same as Boundary 1 Value? Also needs a new conditionality saying it has to be set in case where it exists.</t>
-  </si>
-  <si>
-    <t>We do not see the attributes on the code level</t>
-  </si>
-  <si>
-    <t>NN(3,???</t>
-  </si>
-  <si>
-    <t>Is there for example no knockOutFirst leg? What is "current" leg.</t>
-  </si>
-  <si>
-    <t>Neither first nor second leg activ</t>
-  </si>
-  <si>
-    <t>How do we express the direcion? Our assumption is, that the CNTRL of the child contracts must be set correctly</t>
-  </si>
-  <si>
-    <t>Boolean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">option: 0, identifier: fromBelow, name: From Below, acronym: INCR, description: Boundary effect is trigerred if the observed underlying asset value is greater than or equal to the boundary value at a monitor time.
-option: 1,  identifier: fromAbove, name: From Above, acronym: DECR, description: Boundary action if observed market object value less than or equal to boundary value at a monitor time.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boundary direction specifies the direction of motion in the underlying asset's price which will be considered a valid crossing of the boundary and trigger the boundary effect changing which, if any, of the boundary legs is  active.  </t>
-  </si>
-  <si>
-    <t>option: 0, identifier: knockINFirstLeg, name: KnockIN First Leg, acronym: INFIL, description: effect of boundary crossing is to knock IN the first leg making this the active contract; monitoring of the boundary stops.
-option: 1, identifier: knockINSecondLeg, name: KnockIN Second Leg, acronym: INSEL, description: effect of boundary crossing is to knock IN the Second Leg making this the active contract; monitoring of the boundary stops.
-option: 2, identifier: knockOUTCurrentLeg, name: KnockOUT Current Leg, acronym: OUT, description: effect of boundary crossing is to knockOUT any active contract so there is no active contract after the boundary crossing; monitoring of the boundary stops.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specifies which leg - if any - is the active contract  in effect when the boundary controlled switch contract starts.  </t>
-  </si>
-  <si>
-    <t>The first Boundary monitoring event occurs on this date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">option: 0, identifier: firstLeg, name: First Leg, acronym: FIL, description: the first leg is active when the boundary controlled switch contract is initialized.
-option: 1, identifier: secondLeg, name: Second Leg, acronym: SEL, description: the second leg is active when the boundary controlled switch contract starts.
-option: 2, identifier: Null, name: Null, acronym: Null, description: there is no active subcontract when the boundary controlled switch contract starts. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The frequency with which boundary monitoring events occur. It defines how often the system checks to test whether the  market value of the underlying asset has crossed the boundary in the specified direction triggerring  a boundary crossing event. </t>
-  </si>
-  <si>
-    <t>This term specifies which leg - if any-  becomes the active subcontract  when the underlying asset's price crosses the specified boundary value in the specified direction triggerring a boundary crossing event.</t>
+option: 21, identifier: settlement, name: Settlement, acronym: STD, description: Settlement of an exercised contractual claim, sequence: 21
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFD43C40"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">option: 22, identifier: boundaryMonitor, name: Boundary Monitor, acronym: BDM, description: Compare asset price with boundary value, sequence: 22 
+option: 23, identifier: boundary, name: Boundary, acronym: BDC, description: Underlying asset price crossed boundary, sequence 23 </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -3201,7 +3223,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3379,6 +3401,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD43C40"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFD43C40"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -3466,7 +3500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3623,6 +3657,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3636,7 +3671,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3710,6 +3745,10 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFD43C40"/>
+      <color rgb="FFD25714"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -4449,8 +4488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA34"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5911,7 +5950,7 @@
       <c r="Z33" s="11"/>
       <c r="AA33" s="11"/>
     </row>
-    <row r="34" spans="1:27" s="46" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" s="46" customFormat="1" ht="122" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="43" t="s">
         <v>189</v>
       </c>
@@ -5928,10 +5967,10 @@
         <v>122</v>
       </c>
       <c r="F34" s="44" t="s">
-        <v>929</v>
+        <v>950</v>
       </c>
       <c r="G34" s="44" t="s">
-        <v>930</v>
+        <v>957</v>
       </c>
       <c r="H34" s="45" t="s">
         <v>103</v>
@@ -5950,9 +5989,9 @@
   </sheetPr>
   <dimension ref="A1:AC131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I120" sqref="I120"/>
+      <selection pane="bottomLeft" activeCell="G121" sqref="G121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6065,7 +6104,7 @@
         <v>205</v>
       </c>
       <c r="AB1" s="50" t="s">
-        <v>931</v>
+        <v>926</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6621,10 +6660,10 @@
         <v>239</v>
       </c>
       <c r="AB8" s="51" t="s">
-        <v>932</v>
+        <v>927</v>
       </c>
       <c r="AC8" s="52" t="s">
-        <v>933</v>
+        <v>928</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6908,10 +6947,10 @@
         <v>239</v>
       </c>
       <c r="AB12" s="51" t="s">
-        <v>932</v>
+        <v>927</v>
       </c>
       <c r="AC12" s="52" t="s">
-        <v>933</v>
+        <v>928</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6988,8 +7027,8 @@
       <c r="AA13" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB13" s="63" t="s">
-        <v>934</v>
+      <c r="AB13" s="64" t="s">
+        <v>929</v>
       </c>
       <c r="AC13" s="52"/>
     </row>
@@ -7063,7 +7102,7 @@
       <c r="AA14" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB14" s="64"/>
+      <c r="AB14" s="65"/>
     </row>
     <row r="15" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
@@ -7137,7 +7176,7 @@
       <c r="AA15" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB15" s="64"/>
+      <c r="AB15" s="65"/>
     </row>
     <row r="16" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
@@ -7197,7 +7236,7 @@
       <c r="Y16" s="23"/>
       <c r="Z16" s="23"/>
       <c r="AA16" s="23"/>
-      <c r="AB16" s="64"/>
+      <c r="AB16" s="65"/>
     </row>
     <row r="17" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
@@ -7271,7 +7310,7 @@
       <c r="AA17" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB17" s="64"/>
+      <c r="AB17" s="65"/>
     </row>
     <row r="18" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
@@ -7345,7 +7384,7 @@
       <c r="AA18" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB18" s="64"/>
+      <c r="AB18" s="65"/>
     </row>
     <row r="19" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
@@ -7419,7 +7458,7 @@
       <c r="AA19" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB19" s="64"/>
+      <c r="AB19" s="65"/>
     </row>
     <row r="20" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
@@ -9686,10 +9725,10 @@
       <c r="Z62" s="23"/>
       <c r="AA62" s="23"/>
       <c r="AB62" s="53" t="s">
-        <v>936</v>
+        <v>931</v>
       </c>
       <c r="AC62" s="52" t="s">
-        <v>935</v>
+        <v>930</v>
       </c>
     </row>
     <row r="63" spans="1:29" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -10281,10 +10320,10 @@
         <v>573</v>
       </c>
       <c r="AB73" s="53" t="s">
-        <v>937</v>
-      </c>
-      <c r="AC73" s="65" t="s">
-        <v>939</v>
+        <v>932</v>
+      </c>
+      <c r="AC73" s="66" t="s">
+        <v>934</v>
       </c>
     </row>
     <row r="74" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10360,9 +10399,9 @@
         <v>578</v>
       </c>
       <c r="AB74" s="53" t="s">
-        <v>938</v>
-      </c>
-      <c r="AC74" s="66"/>
+        <v>933</v>
+      </c>
+      <c r="AC74" s="67"/>
     </row>
     <row r="75" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
@@ -12647,29 +12686,29 @@
         <v>780</v>
       </c>
       <c r="B118" s="34" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C118" s="48" t="s">
         <v>781</v>
       </c>
       <c r="D118" s="34" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E118" s="35" t="s">
         <v>305</v>
       </c>
       <c r="F118" s="34"/>
-      <c r="H118" s="67" t="s">
-        <v>946</v>
+      <c r="H118" s="62" t="s">
+        <v>940</v>
       </c>
       <c r="I118" s="49" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="AB118" s="53" t="s">
-        <v>940</v>
+        <v>935</v>
       </c>
       <c r="AC118" s="57" t="s">
-        <v>941</v>
+        <v>936</v>
       </c>
     </row>
     <row r="119" spans="1:29" ht="148" customHeight="1" x14ac:dyDescent="0.2">
@@ -12677,29 +12716,29 @@
         <v>782</v>
       </c>
       <c r="B119" s="34" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C119" s="48" t="s">
         <v>783</v>
       </c>
       <c r="D119" s="34" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E119" s="34" t="s">
         <v>209</v>
       </c>
       <c r="F119" s="49" t="s">
-        <v>948</v>
-      </c>
-      <c r="H119" s="62"/>
+        <v>942</v>
+      </c>
+      <c r="H119" s="63"/>
       <c r="I119" s="49" t="s">
-        <v>949</v>
+        <v>943</v>
       </c>
       <c r="AB119" s="53" t="s">
-        <v>943</v>
+        <v>938</v>
       </c>
       <c r="AC119" s="56" t="s">
-        <v>942</v>
+        <v>937</v>
       </c>
     </row>
     <row r="120" spans="1:29" ht="243" customHeight="1" x14ac:dyDescent="0.2">
@@ -12707,26 +12746,26 @@
         <v>784</v>
       </c>
       <c r="B120" s="34" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C120" s="48" t="s">
         <v>785</v>
       </c>
       <c r="D120" s="34" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E120" s="34" t="s">
         <v>209</v>
       </c>
       <c r="F120" s="49" t="s">
-        <v>950</v>
-      </c>
-      <c r="H120" s="62"/>
+        <v>944</v>
+      </c>
+      <c r="H120" s="63"/>
       <c r="I120" s="49" t="s">
-        <v>955</v>
+        <v>949</v>
       </c>
       <c r="AC120" s="55" t="s">
-        <v>944</v>
+        <v>939</v>
       </c>
     </row>
     <row r="121" spans="1:29" ht="186" customHeight="1" x14ac:dyDescent="0.2">
@@ -12734,26 +12773,23 @@
         <v>786</v>
       </c>
       <c r="B121" s="34" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C121" s="48" t="s">
         <v>787</v>
       </c>
       <c r="D121" s="34" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E121" s="34" t="s">
         <v>209</v>
       </c>
       <c r="F121" s="49" t="s">
-        <v>953</v>
-      </c>
-      <c r="G121" t="s">
+        <v>947</v>
+      </c>
+      <c r="H121" s="63"/>
+      <c r="I121" s="49" t="s">
         <v>945</v>
-      </c>
-      <c r="H121" s="62"/>
-      <c r="I121" s="49" t="s">
-        <v>951</v>
       </c>
       <c r="AB121" s="53" t="s">
         <v>213</v>
@@ -12764,13 +12800,13 @@
         <v>788</v>
       </c>
       <c r="B122" s="34" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C122" s="48" t="s">
         <v>789</v>
       </c>
       <c r="D122" s="34" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="E122" s="35" t="s">
         <v>236</v>
@@ -12778,9 +12814,9 @@
       <c r="F122" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="H122" s="62"/>
+      <c r="H122" s="63"/>
       <c r="I122" s="49" t="s">
-        <v>952</v>
+        <v>946</v>
       </c>
       <c r="AB122" s="53" t="s">
         <v>232</v>
@@ -12791,13 +12827,13 @@
         <v>790</v>
       </c>
       <c r="B123" s="34" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C123" s="48" t="s">
         <v>791</v>
       </c>
       <c r="D123" s="34" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="E123" s="35" t="s">
         <v>236</v>
@@ -12805,9 +12841,9 @@
       <c r="F123" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="H123" s="62"/>
+      <c r="H123" s="63"/>
       <c r="I123" s="49" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="AB123" s="53" t="s">
         <v>232</v>
@@ -12818,13 +12854,13 @@
         <v>792</v>
       </c>
       <c r="B124" s="34" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C124" s="34" t="s">
         <v>793</v>
       </c>
       <c r="D124" s="34" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="E124" s="34" t="s">
         <v>289</v>
@@ -12835,7 +12871,7 @@
       <c r="G124" s="34"/>
       <c r="H124" s="34"/>
       <c r="I124" s="49" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
     </row>
     <row r="126" spans="1:29" x14ac:dyDescent="0.2">
@@ -15349,7 +15385,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15752,13 +15788,13 @@
         <v>874</v>
       </c>
       <c r="C21" s="61" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>926</v>
+        <v>952</v>
       </c>
       <c r="E21" s="61" t="s">
-        <v>947</v>
+        <v>941</v>
       </c>
       <c r="F21" s="61"/>
       <c r="G21" s="61"/>
@@ -15771,23 +15807,33 @@
         <v>876</v>
       </c>
       <c r="C22" s="61" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>927</v>
+        <v>953</v>
       </c>
       <c r="E22" s="61" t="s">
-        <v>947</v>
+        <v>941</v>
       </c>
       <c r="F22" s="61"/>
       <c r="G22" s="61"/>
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="59"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
+      <c r="A23" s="68" t="s">
+        <v>951</v>
+      </c>
+      <c r="B23" s="68" t="s">
+        <v>954</v>
+      </c>
+      <c r="C23" s="68" t="s">
+        <v>955</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>956</v>
+      </c>
+      <c r="E23" s="59" t="s">
+        <v>941</v>
+      </c>
       <c r="F23" s="59"/>
       <c r="G23" s="59"/>
     </row>
@@ -15801,8 +15847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15893,7 +15939,7 @@
         <v>209</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>889</v>
+        <v>958</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -15907,7 +15953,7 @@
         <v>480</v>
       </c>
       <c r="D5" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E5" t="s">
         <v>248</v>
@@ -15918,16 +15964,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>890</v>
+      </c>
+      <c r="B6" t="s">
         <v>891</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>892</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>893</v>
-      </c>
-      <c r="D6" t="s">
-        <v>894</v>
       </c>
       <c r="E6" t="s">
         <v>305</v>
@@ -15935,19 +15981,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>894</v>
+      </c>
+      <c r="B7" t="s">
         <v>895</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>896</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>897</v>
       </c>
-      <c r="D7" t="s">
-        <v>898</v>
-      </c>
       <c r="E7" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -15955,13 +16001,13 @@
         <v>251</v>
       </c>
       <c r="B8" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C8" t="s">
         <v>253</v>
       </c>
       <c r="D8" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E8" t="s">
         <v>248</v>
@@ -16010,16 +16056,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>900</v>
+      </c>
+      <c r="B2" t="s">
         <v>901</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>902</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>903</v>
-      </c>
-      <c r="D2" t="s">
-        <v>904</v>
       </c>
       <c r="E2" t="s">
         <v>248</v>
@@ -16027,42 +16073,42 @@
     </row>
     <row r="3" spans="1:6" ht="399" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>904</v>
+      </c>
+      <c r="B3" t="s">
         <v>905</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>906</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>907</v>
-      </c>
-      <c r="D3" t="s">
-        <v>908</v>
       </c>
       <c r="E3" t="s">
         <v>209</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="385" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>909</v>
+      </c>
+      <c r="B4" t="s">
         <v>910</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>911</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>912</v>
-      </c>
-      <c r="D4" t="s">
-        <v>913</v>
       </c>
       <c r="E4" t="s">
         <v>209</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Explicitly include changes to actus-dictionary-event.json  dropped from last commit and push
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisnparr/git/actus-dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A535EE-27B5-5244-926F-DED00A1A2725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832F291B-460C-9942-903E-DD3870278AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35660" yWindow="500" windowWidth="33600" windowHeight="19640" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3657,6 +3657,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3671,7 +3672,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7027,7 +7027,7 @@
       <c r="AA13" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB13" s="64" t="s">
+      <c r="AB13" s="65" t="s">
         <v>929</v>
       </c>
       <c r="AC13" s="52"/>
@@ -7102,7 +7102,7 @@
       <c r="AA14" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB14" s="65"/>
+      <c r="AB14" s="66"/>
     </row>
     <row r="15" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
@@ -7176,7 +7176,7 @@
       <c r="AA15" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB15" s="65"/>
+      <c r="AB15" s="66"/>
     </row>
     <row r="16" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
@@ -7236,7 +7236,7 @@
       <c r="Y16" s="23"/>
       <c r="Z16" s="23"/>
       <c r="AA16" s="23"/>
-      <c r="AB16" s="65"/>
+      <c r="AB16" s="66"/>
     </row>
     <row r="17" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
@@ -7310,7 +7310,7 @@
       <c r="AA17" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB17" s="65"/>
+      <c r="AB17" s="66"/>
     </row>
     <row r="18" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
@@ -7384,7 +7384,7 @@
       <c r="AA18" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB18" s="65"/>
+      <c r="AB18" s="66"/>
     </row>
     <row r="19" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
@@ -7458,7 +7458,7 @@
       <c r="AA19" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="AB19" s="65"/>
+      <c r="AB19" s="66"/>
     </row>
     <row r="20" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
@@ -10322,7 +10322,7 @@
       <c r="AB73" s="53" t="s">
         <v>932</v>
       </c>
-      <c r="AC73" s="66" t="s">
+      <c r="AC73" s="67" t="s">
         <v>934</v>
       </c>
     </row>
@@ -10401,7 +10401,7 @@
       <c r="AB74" s="53" t="s">
         <v>933</v>
       </c>
-      <c r="AC74" s="67"/>
+      <c r="AC74" s="68"/>
     </row>
     <row r="75" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
@@ -12698,7 +12698,7 @@
         <v>305</v>
       </c>
       <c r="F118" s="34"/>
-      <c r="H118" s="62" t="s">
+      <c r="H118" s="63" t="s">
         <v>940</v>
       </c>
       <c r="I118" s="49" t="s">
@@ -12730,7 +12730,7 @@
       <c r="F119" s="49" t="s">
         <v>942</v>
       </c>
-      <c r="H119" s="63"/>
+      <c r="H119" s="64"/>
       <c r="I119" s="49" t="s">
         <v>943</v>
       </c>
@@ -12760,7 +12760,7 @@
       <c r="F120" s="49" t="s">
         <v>944</v>
       </c>
-      <c r="H120" s="63"/>
+      <c r="H120" s="64"/>
       <c r="I120" s="49" t="s">
         <v>949</v>
       </c>
@@ -12787,7 +12787,7 @@
       <c r="F121" s="49" t="s">
         <v>947</v>
       </c>
-      <c r="H121" s="63"/>
+      <c r="H121" s="64"/>
       <c r="I121" s="49" t="s">
         <v>945</v>
       </c>
@@ -12814,7 +12814,7 @@
       <c r="F122" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="H122" s="63"/>
+      <c r="H122" s="64"/>
       <c r="I122" s="49" t="s">
         <v>946</v>
       </c>
@@ -12841,7 +12841,7 @@
       <c r="F123" s="36" t="s">
         <v>237</v>
       </c>
-      <c r="H123" s="63"/>
+      <c r="H123" s="64"/>
       <c r="I123" s="49" t="s">
         <v>924</v>
       </c>
@@ -15819,16 +15819,16 @@
       <c r="G22" s="61"/>
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="68" t="s">
+      <c r="A23" s="62" t="s">
         <v>951</v>
       </c>
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="62" t="s">
         <v>954</v>
       </c>
-      <c r="C23" s="68" t="s">
+      <c r="C23" s="62" t="s">
         <v>955</v>
       </c>
-      <c r="D23" s="68" t="s">
+      <c r="D23" s="62" t="s">
         <v>956</v>
       </c>
       <c r="E23" s="59" t="s">

</xml_diff>

<commit_message>
Make sure actus-dictionary.xlsx with no hidden columns is saved
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisnparr/git/actus-dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832F291B-460C-9942-903E-DD3870278AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891AA6C8-DD33-8941-ABF3-3CDBC6E56C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35660" yWindow="500" windowWidth="33600" windowHeight="19640" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13420" yWindow="500" windowWidth="27480" windowHeight="19040" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -2182,9 +2182,6 @@
   </si>
   <si>
     <t>Option Strike 2</t>
-  </si>
-  <si>
-    <t>OPS2</t>
   </si>
   <si>
     <t>Put price in case of call/put.</t>
@@ -3213,6 +3210,9 @@
       <t xml:space="preserve">option: 22, identifier: boundaryMonitor, name: Boundary Monitor, acronym: BDM, description: Compare asset price with boundary value, sequence: 22 
 option: 23, identifier: boundary, name: Boundary, acronym: BDC, description: Underlying asset price crossed boundary, sequence 23 </t>
     </r>
+  </si>
+  <si>
+    <t>sss</t>
   </si>
 </sst>
 </file>
@@ -5967,10 +5967,10 @@
         <v>122</v>
       </c>
       <c r="F34" s="44" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="G34" s="44" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="H34" s="45" t="s">
         <v>103</v>
@@ -5991,7 +5991,7 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G121" sqref="G121"/>
+      <selection pane="bottomLeft" activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6104,7 +6104,7 @@
         <v>205</v>
       </c>
       <c r="AB1" s="50" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6660,10 +6660,10 @@
         <v>239</v>
       </c>
       <c r="AB8" s="51" t="s">
+        <v>926</v>
+      </c>
+      <c r="AC8" s="52" t="s">
         <v>927</v>
-      </c>
-      <c r="AC8" s="52" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6947,10 +6947,10 @@
         <v>239</v>
       </c>
       <c r="AB12" s="51" t="s">
+        <v>926</v>
+      </c>
+      <c r="AC12" s="52" t="s">
         <v>927</v>
-      </c>
-      <c r="AC12" s="52" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7028,7 +7028,7 @@
         <v>276</v>
       </c>
       <c r="AB13" s="65" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="AC13" s="52"/>
     </row>
@@ -9725,10 +9725,10 @@
       <c r="Z62" s="23"/>
       <c r="AA62" s="23"/>
       <c r="AB62" s="53" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="AC62" s="52" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="63" spans="1:29" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -10320,10 +10320,10 @@
         <v>573</v>
       </c>
       <c r="AB73" s="53" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="AC73" s="67" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="74" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10399,7 +10399,7 @@
         <v>578</v>
       </c>
       <c r="AB74" s="53" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="AC74" s="68"/>
     </row>
@@ -11100,7 +11100,7 @@
         <v>639</v>
       </c>
       <c r="D88" s="20" t="s">
-        <v>640</v>
+        <v>958</v>
       </c>
       <c r="E88" s="20" t="s">
         <v>305</v>
@@ -11113,7 +11113,7 @@
         <v>341</v>
       </c>
       <c r="I88" s="20" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="J88" s="23"/>
       <c r="K88" s="23"/>
@@ -11138,27 +11138,27 @@
     </row>
     <row r="89" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="20" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B89" s="20" t="s">
         <v>624</v>
       </c>
       <c r="C89" s="20" t="s">
+        <v>642</v>
+      </c>
+      <c r="D89" s="20" t="s">
         <v>643</v>
-      </c>
-      <c r="D89" s="20" t="s">
-        <v>644</v>
       </c>
       <c r="E89" s="20" t="s">
         <v>209</v>
       </c>
       <c r="F89" s="20" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G89" s="23"/>
       <c r="H89" s="23"/>
       <c r="I89" s="20" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="J89" s="23"/>
       <c r="K89" s="23"/>
@@ -11183,16 +11183,16 @@
     </row>
     <row r="90" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="20" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B90" s="20" t="s">
         <v>624</v>
       </c>
       <c r="C90" s="20" t="s">
+        <v>647</v>
+      </c>
+      <c r="D90" s="20" t="s">
         <v>648</v>
-      </c>
-      <c r="D90" s="20" t="s">
-        <v>649</v>
       </c>
       <c r="E90" s="20" t="s">
         <v>236</v>
@@ -11203,7 +11203,7 @@
       <c r="G90" s="21"/>
       <c r="H90" s="23"/>
       <c r="I90" s="20" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J90" s="23"/>
       <c r="K90" s="23"/>
@@ -11238,16 +11238,16 @@
     </row>
     <row r="91" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="20" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B91" s="20" t="s">
         <v>624</v>
       </c>
       <c r="C91" s="20" t="s">
+        <v>651</v>
+      </c>
+      <c r="D91" s="20" t="s">
         <v>652</v>
-      </c>
-      <c r="D91" s="20" t="s">
-        <v>653</v>
       </c>
       <c r="E91" s="20" t="s">
         <v>334</v>
@@ -11258,7 +11258,7 @@
       <c r="G91" s="23"/>
       <c r="H91" s="23"/>
       <c r="I91" s="20" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="J91" s="23"/>
       <c r="K91" s="23"/>
@@ -11293,29 +11293,29 @@
     </row>
     <row r="92" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="20" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B92" s="20" t="s">
         <v>624</v>
       </c>
       <c r="C92" s="20" t="s">
+        <v>655</v>
+      </c>
+      <c r="D92" s="20" t="s">
         <v>656</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>657</v>
       </c>
       <c r="E92" s="20" t="s">
         <v>209</v>
       </c>
       <c r="F92" s="21" t="s">
+        <v>657</v>
+      </c>
+      <c r="G92" s="21" t="s">
         <v>658</v>
-      </c>
-      <c r="G92" s="21" t="s">
-        <v>659</v>
       </c>
       <c r="H92" s="23"/>
       <c r="I92" s="20" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J92" s="23"/>
       <c r="K92" s="23"/>
@@ -11348,16 +11348,16 @@
     </row>
     <row r="93" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="20" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B93" s="20" t="s">
         <v>624</v>
       </c>
       <c r="C93" s="20" t="s">
+        <v>661</v>
+      </c>
+      <c r="D93" s="20" t="s">
         <v>662</v>
-      </c>
-      <c r="D93" s="20" t="s">
-        <v>663</v>
       </c>
       <c r="E93" s="20" t="s">
         <v>305</v>
@@ -11372,7 +11372,7 @@
         <v>341</v>
       </c>
       <c r="I93" s="20" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J93" s="23"/>
       <c r="K93" s="23"/>
@@ -11405,47 +11405,47 @@
     </row>
     <row r="94" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="20" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B94" s="20" t="s">
         <v>624</v>
       </c>
       <c r="C94" s="20" t="s">
+        <v>665</v>
+      </c>
+      <c r="D94" s="20" t="s">
         <v>666</v>
-      </c>
-      <c r="D94" s="20" t="s">
-        <v>667</v>
       </c>
       <c r="E94" s="20" t="s">
         <v>209</v>
       </c>
       <c r="F94" s="22" t="s">
+        <v>667</v>
+      </c>
+      <c r="G94" s="21" t="s">
         <v>668</v>
-      </c>
-      <c r="G94" s="21" t="s">
-        <v>669</v>
       </c>
       <c r="H94" s="23"/>
       <c r="I94" s="20" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="J94" s="23"/>
       <c r="K94" s="23"/>
       <c r="L94" s="23"/>
       <c r="M94" s="20" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N94" s="20" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="O94" s="20" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="P94" s="20" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="Q94" s="20" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="R94" s="23"/>
       <c r="S94" s="23"/>
@@ -11460,16 +11460,16 @@
     </row>
     <row r="95" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="20" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B95" s="20" t="s">
         <v>624</v>
       </c>
       <c r="C95" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="D95" s="20" t="s">
         <v>673</v>
-      </c>
-      <c r="D95" s="20" t="s">
-        <v>674</v>
       </c>
       <c r="E95" s="20" t="s">
         <v>305</v>
@@ -11478,11 +11478,11 @@
         <v>306</v>
       </c>
       <c r="G95" s="21" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="H95" s="22"/>
       <c r="I95" s="20" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="J95" s="22"/>
       <c r="K95" s="20" t="s">
@@ -11507,16 +11507,16 @@
     </row>
     <row r="96" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="20" t="s">
+        <v>676</v>
+      </c>
+      <c r="B96" s="20" t="s">
         <v>677</v>
       </c>
-      <c r="B96" s="20" t="s">
+      <c r="C96" s="20" t="s">
         <v>678</v>
       </c>
-      <c r="C96" s="20" t="s">
+      <c r="D96" s="20" t="s">
         <v>679</v>
-      </c>
-      <c r="D96" s="20" t="s">
-        <v>680</v>
       </c>
       <c r="E96" s="20" t="s">
         <v>236</v>
@@ -11527,34 +11527,34 @@
       <c r="G96" s="21"/>
       <c r="H96" s="20"/>
       <c r="I96" s="20" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="J96" s="20"/>
       <c r="K96" s="20" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="L96" s="20" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="M96" s="20" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N96" s="20" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="O96" s="22"/>
       <c r="P96" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="Q96" s="20" t="s">
         <v>683</v>
-      </c>
-      <c r="Q96" s="20" t="s">
-        <v>684</v>
       </c>
       <c r="R96" s="20"/>
       <c r="S96" s="20"/>
       <c r="T96" s="20"/>
       <c r="U96" s="20"/>
       <c r="V96" s="20" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="W96" s="22"/>
       <c r="X96" s="22"/>
@@ -11564,16 +11564,16 @@
     </row>
     <row r="97" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="B97" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C97" s="20" t="s">
         <v>685</v>
       </c>
-      <c r="B97" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C97" s="20" t="s">
+      <c r="D97" s="20" t="s">
         <v>686</v>
-      </c>
-      <c r="D97" s="20" t="s">
-        <v>687</v>
       </c>
       <c r="E97" s="20" t="s">
         <v>385</v>
@@ -11582,7 +11582,7 @@
       <c r="G97" s="23"/>
       <c r="H97" s="20"/>
       <c r="I97" s="20" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="J97" s="20"/>
       <c r="K97" s="22"/>
@@ -11590,7 +11590,7 @@
       <c r="M97" s="22"/>
       <c r="N97" s="22"/>
       <c r="O97" s="20" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="P97" s="22"/>
       <c r="Q97" s="22"/>
@@ -11607,16 +11607,16 @@
     </row>
     <row r="98" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="20" t="s">
+        <v>688</v>
+      </c>
+      <c r="B98" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C98" s="20" t="s">
         <v>689</v>
       </c>
-      <c r="B98" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C98" s="20" t="s">
+      <c r="D98" s="20" t="s">
         <v>690</v>
-      </c>
-      <c r="D98" s="20" t="s">
-        <v>691</v>
       </c>
       <c r="E98" s="20" t="s">
         <v>334</v>
@@ -11627,34 +11627,34 @@
       <c r="G98" s="21"/>
       <c r="H98" s="20"/>
       <c r="I98" s="20" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="J98" s="20"/>
       <c r="K98" s="20" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="L98" s="20" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="M98" s="20" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="N98" s="20" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="O98" s="22"/>
       <c r="P98" s="20" t="s">
+        <v>682</v>
+      </c>
+      <c r="Q98" s="20" t="s">
         <v>683</v>
-      </c>
-      <c r="Q98" s="20" t="s">
-        <v>684</v>
       </c>
       <c r="R98" s="20"/>
       <c r="S98" s="20"/>
       <c r="T98" s="20"/>
       <c r="U98" s="20"/>
       <c r="V98" s="20" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="W98" s="22"/>
       <c r="X98" s="22"/>
@@ -11664,16 +11664,16 @@
     </row>
     <row r="99" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="20" t="s">
+        <v>692</v>
+      </c>
+      <c r="B99" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C99" s="20" t="s">
         <v>693</v>
       </c>
-      <c r="B99" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C99" s="20" t="s">
+      <c r="D99" s="20" t="s">
         <v>694</v>
-      </c>
-      <c r="D99" s="20" t="s">
-        <v>695</v>
       </c>
       <c r="E99" s="20" t="s">
         <v>395</v>
@@ -11682,7 +11682,7 @@
       <c r="G99" s="23"/>
       <c r="H99" s="20"/>
       <c r="I99" s="20" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="J99" s="20"/>
       <c r="K99" s="22"/>
@@ -11690,7 +11690,7 @@
       <c r="M99" s="22"/>
       <c r="N99" s="22"/>
       <c r="O99" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="P99" s="22"/>
       <c r="Q99" s="22"/>
@@ -11707,16 +11707,16 @@
     </row>
     <row r="100" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="20" t="s">
+        <v>697</v>
+      </c>
+      <c r="B100" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C100" s="20" t="s">
         <v>698</v>
       </c>
-      <c r="B100" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C100" s="20" t="s">
+      <c r="D100" s="20" t="s">
         <v>699</v>
-      </c>
-      <c r="D100" s="20" t="s">
-        <v>700</v>
       </c>
       <c r="E100" s="20" t="s">
         <v>305</v>
@@ -11727,24 +11727,24 @@
       </c>
       <c r="H100" s="20"/>
       <c r="I100" s="20" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="J100" s="20"/>
       <c r="K100" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="L100" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="M100" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="N100" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="O100" s="22"/>
       <c r="P100" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="Q100" s="20" t="s">
         <v>232</v>
@@ -11764,16 +11764,16 @@
     </row>
     <row r="101" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="20" t="s">
+        <v>702</v>
+      </c>
+      <c r="B101" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C101" s="20" t="s">
         <v>703</v>
       </c>
-      <c r="B101" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C101" s="20" t="s">
+      <c r="D101" s="20" t="s">
         <v>704</v>
-      </c>
-      <c r="D101" s="20" t="s">
-        <v>705</v>
       </c>
       <c r="E101" s="20" t="s">
         <v>552</v>
@@ -11782,7 +11782,7 @@
       <c r="G101" s="23"/>
       <c r="H101" s="20"/>
       <c r="I101" s="20" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="J101" s="20"/>
       <c r="K101" s="22"/>
@@ -11790,7 +11790,7 @@
       <c r="M101" s="22"/>
       <c r="N101" s="22"/>
       <c r="O101" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="P101" s="22"/>
       <c r="Q101" s="22"/>
@@ -11807,27 +11807,27 @@
     </row>
     <row r="102" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="20" t="s">
+        <v>706</v>
+      </c>
+      <c r="B102" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C102" s="20" t="s">
         <v>707</v>
       </c>
-      <c r="B102" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C102" s="20" t="s">
+      <c r="D102" s="20" t="s">
         <v>708</v>
-      </c>
-      <c r="D102" s="20" t="s">
-        <v>709</v>
       </c>
       <c r="E102" s="20" t="s">
         <v>321</v>
       </c>
       <c r="F102" s="20" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="G102" s="23"/>
       <c r="H102" s="20"/>
       <c r="I102" s="20" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="J102" s="20"/>
       <c r="K102" s="22"/>
@@ -11835,7 +11835,7 @@
       <c r="M102" s="22"/>
       <c r="N102" s="22"/>
       <c r="O102" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="P102" s="22"/>
       <c r="Q102" s="22"/>
@@ -11852,16 +11852,16 @@
     </row>
     <row r="103" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="20" t="s">
+        <v>711</v>
+      </c>
+      <c r="B103" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C103" s="20" t="s">
         <v>712</v>
       </c>
-      <c r="B103" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C103" s="20" t="s">
+      <c r="D103" s="20" t="s">
         <v>713</v>
-      </c>
-      <c r="D103" s="20" t="s">
-        <v>714</v>
       </c>
       <c r="E103" s="20" t="s">
         <v>248</v>
@@ -11870,26 +11870,26 @@
       <c r="G103" s="21"/>
       <c r="H103" s="20"/>
       <c r="I103" s="20" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="J103" s="20"/>
       <c r="K103" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="L103" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="M103" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="N103" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="O103" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="P103" s="20" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="Q103" s="20" t="s">
         <v>232</v>
@@ -11909,16 +11909,16 @@
     </row>
     <row r="104" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="20" t="s">
+        <v>715</v>
+      </c>
+      <c r="B104" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C104" s="20" t="s">
         <v>716</v>
       </c>
-      <c r="B104" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C104" s="20" t="s">
+      <c r="D104" s="20" t="s">
         <v>717</v>
-      </c>
-      <c r="D104" s="20" t="s">
-        <v>718</v>
       </c>
       <c r="E104" s="20" t="s">
         <v>305</v>
@@ -11927,25 +11927,25 @@
       <c r="G104" s="21"/>
       <c r="H104" s="20"/>
       <c r="I104" s="20" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="J104" s="20"/>
       <c r="K104" s="20"/>
       <c r="L104" s="22"/>
       <c r="M104" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N104" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="O104" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="P104" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="Q104" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="R104" s="20"/>
       <c r="S104" s="20"/>
@@ -11962,16 +11962,16 @@
     </row>
     <row r="105" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="20" t="s">
+        <v>719</v>
+      </c>
+      <c r="B105" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C105" s="20" t="s">
         <v>720</v>
       </c>
-      <c r="B105" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C105" s="20" t="s">
+      <c r="D105" s="20" t="s">
         <v>721</v>
-      </c>
-      <c r="D105" s="20" t="s">
-        <v>722</v>
       </c>
       <c r="E105" s="20" t="s">
         <v>305</v>
@@ -11980,25 +11980,25 @@
       <c r="G105" s="21"/>
       <c r="H105" s="20"/>
       <c r="I105" s="20" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="J105" s="20"/>
       <c r="K105" s="20"/>
       <c r="L105" s="22"/>
       <c r="M105" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N105" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="O105" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="P105" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="Q105" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="R105" s="20"/>
       <c r="S105" s="20"/>
@@ -12015,16 +12015,16 @@
     </row>
     <row r="106" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="20" t="s">
+        <v>723</v>
+      </c>
+      <c r="B106" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C106" s="20" t="s">
         <v>724</v>
       </c>
-      <c r="B106" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C106" s="20" t="s">
+      <c r="D106" s="20" t="s">
         <v>725</v>
-      </c>
-      <c r="D106" s="20" t="s">
-        <v>726</v>
       </c>
       <c r="E106" s="20" t="s">
         <v>305</v>
@@ -12035,25 +12035,25 @@
       <c r="G106" s="21"/>
       <c r="H106" s="20"/>
       <c r="I106" s="20" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J106" s="20"/>
       <c r="K106" s="20"/>
       <c r="L106" s="22"/>
       <c r="M106" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N106" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="O106" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="P106" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="Q106" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="R106" s="20"/>
       <c r="S106" s="20"/>
@@ -12068,16 +12068,16 @@
     </row>
     <row r="107" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="20" t="s">
+        <v>727</v>
+      </c>
+      <c r="B107" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C107" s="20" t="s">
         <v>728</v>
       </c>
-      <c r="B107" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C107" s="20" t="s">
+      <c r="D107" s="20" t="s">
         <v>729</v>
-      </c>
-      <c r="D107" s="20" t="s">
-        <v>730</v>
       </c>
       <c r="E107" s="20" t="s">
         <v>305</v>
@@ -12088,25 +12088,25 @@
       <c r="G107" s="21"/>
       <c r="H107" s="20"/>
       <c r="I107" s="20" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="J107" s="20"/>
       <c r="K107" s="20"/>
       <c r="L107" s="22"/>
       <c r="M107" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N107" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="O107" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="P107" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="Q107" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="R107" s="20"/>
       <c r="S107" s="20"/>
@@ -12121,41 +12121,41 @@
     </row>
     <row r="108" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="20" t="s">
+        <v>731</v>
+      </c>
+      <c r="B108" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C108" s="20" t="s">
         <v>732</v>
       </c>
-      <c r="B108" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C108" s="20" t="s">
+      <c r="D108" s="20" t="s">
         <v>733</v>
-      </c>
-      <c r="D108" s="20" t="s">
-        <v>734</v>
       </c>
       <c r="E108" s="20" t="s">
         <v>209</v>
       </c>
       <c r="F108" s="20" t="s">
+        <v>734</v>
+      </c>
+      <c r="G108" s="21" t="s">
         <v>735</v>
-      </c>
-      <c r="G108" s="21" t="s">
-        <v>736</v>
       </c>
       <c r="H108" s="20"/>
       <c r="I108" s="20" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="J108" s="20"/>
       <c r="K108" s="20"/>
       <c r="L108" s="22"/>
       <c r="M108" s="20" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="N108" s="20" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="O108" s="20" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="P108" s="22"/>
       <c r="Q108" s="22"/>
@@ -12164,7 +12164,7 @@
       <c r="T108" s="20"/>
       <c r="U108" s="20"/>
       <c r="V108" s="20" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="W108" s="22"/>
       <c r="X108" s="22"/>
@@ -12174,16 +12174,16 @@
     </row>
     <row r="109" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="20" t="s">
+        <v>738</v>
+      </c>
+      <c r="B109" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C109" s="20" t="s">
         <v>739</v>
       </c>
-      <c r="B109" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C109" s="20" t="s">
+      <c r="D109" s="20" t="s">
         <v>740</v>
-      </c>
-      <c r="D109" s="20" t="s">
-        <v>741</v>
       </c>
       <c r="E109" s="20" t="s">
         <v>289</v>
@@ -12196,34 +12196,34 @@
       </c>
       <c r="H109" s="20"/>
       <c r="I109" s="20" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="J109" s="20"/>
       <c r="K109" s="20"/>
       <c r="L109" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="M109" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N109" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="O109" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="P109" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="Q109" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="R109" s="20"/>
       <c r="S109" s="20"/>
       <c r="T109" s="20"/>
       <c r="U109" s="20"/>
       <c r="V109" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="W109" s="22"/>
       <c r="X109" s="22"/>
@@ -12233,16 +12233,16 @@
     </row>
     <row r="110" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="20" t="s">
+        <v>742</v>
+      </c>
+      <c r="B110" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C110" s="20" t="s">
         <v>743</v>
       </c>
-      <c r="B110" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C110" s="20" t="s">
+      <c r="D110" s="20" t="s">
         <v>744</v>
-      </c>
-      <c r="D110" s="20" t="s">
-        <v>745</v>
       </c>
       <c r="E110" s="20" t="s">
         <v>305</v>
@@ -12251,34 +12251,34 @@
       <c r="G110" s="21"/>
       <c r="H110" s="20"/>
       <c r="I110" s="20" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="J110" s="20"/>
       <c r="K110" s="20"/>
       <c r="L110" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="M110" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N110" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="O110" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="P110" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="Q110" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="R110" s="20"/>
       <c r="S110" s="20"/>
       <c r="T110" s="20"/>
       <c r="U110" s="20"/>
       <c r="V110" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="W110" s="22"/>
       <c r="X110" s="22"/>
@@ -12288,16 +12288,16 @@
     </row>
     <row r="111" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="B111" s="20" t="s">
+        <v>677</v>
+      </c>
+      <c r="C111" s="20" t="s">
         <v>747</v>
       </c>
-      <c r="B111" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="C111" s="20" t="s">
+      <c r="D111" s="20" t="s">
         <v>748</v>
-      </c>
-      <c r="D111" s="20" t="s">
-        <v>749</v>
       </c>
       <c r="E111" s="20" t="s">
         <v>305</v>
@@ -12308,34 +12308,34 @@
       </c>
       <c r="H111" s="20"/>
       <c r="I111" s="20" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="J111" s="20"/>
       <c r="K111" s="20"/>
       <c r="L111" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="M111" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N111" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="O111" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="P111" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="Q111" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="R111" s="20"/>
       <c r="S111" s="20"/>
       <c r="T111" s="20"/>
       <c r="U111" s="20"/>
       <c r="V111" s="20" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="W111" s="22"/>
       <c r="X111" s="22"/>
@@ -12345,16 +12345,16 @@
     </row>
     <row r="112" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="20" t="s">
+        <v>750</v>
+      </c>
+      <c r="B112" s="20" t="s">
         <v>751</v>
       </c>
-      <c r="B112" s="20" t="s">
+      <c r="C112" s="20" t="s">
         <v>752</v>
       </c>
-      <c r="C112" s="20" t="s">
+      <c r="D112" s="20" t="s">
         <v>753</v>
-      </c>
-      <c r="D112" s="20" t="s">
-        <v>754</v>
       </c>
       <c r="E112" s="20" t="s">
         <v>236</v>
@@ -12365,7 +12365,7 @@
       <c r="G112" s="21"/>
       <c r="H112" s="20"/>
       <c r="I112" s="20" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="J112" s="20"/>
       <c r="K112" s="20"/>
@@ -12378,36 +12378,36 @@
       <c r="R112" s="20"/>
       <c r="S112" s="20"/>
       <c r="T112" s="20" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="U112" s="20" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="V112" s="22"/>
       <c r="W112" s="22"/>
       <c r="X112" s="20" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="Y112" s="20" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="Z112" s="20" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="AA112" s="20"/>
     </row>
     <row r="113" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="20" t="s">
+        <v>756</v>
+      </c>
+      <c r="B113" s="20" t="s">
+        <v>751</v>
+      </c>
+      <c r="C113" s="20" t="s">
         <v>757</v>
       </c>
-      <c r="B113" s="20" t="s">
-        <v>752</v>
-      </c>
-      <c r="C113" s="20" t="s">
+      <c r="D113" s="20" t="s">
         <v>758</v>
-      </c>
-      <c r="D113" s="20" t="s">
-        <v>759</v>
       </c>
       <c r="E113" s="20" t="s">
         <v>305</v>
@@ -12418,7 +12418,7 @@
         <v>341</v>
       </c>
       <c r="I113" s="20" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="J113" s="20"/>
       <c r="K113" s="20"/>
@@ -12431,36 +12431,36 @@
       <c r="R113" s="20"/>
       <c r="S113" s="20"/>
       <c r="T113" s="20" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="U113" s="20" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="V113" s="22"/>
       <c r="W113" s="22"/>
       <c r="X113" s="20" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="Y113" s="20" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="Z113" s="20" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="AA113" s="20"/>
     </row>
     <row r="114" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="20" t="s">
+        <v>761</v>
+      </c>
+      <c r="B114" s="20" t="s">
+        <v>751</v>
+      </c>
+      <c r="C114" s="20" t="s">
         <v>762</v>
       </c>
-      <c r="B114" s="20" t="s">
-        <v>752</v>
-      </c>
-      <c r="C114" s="20" t="s">
+      <c r="D114" s="20" t="s">
         <v>763</v>
-      </c>
-      <c r="D114" s="20" t="s">
-        <v>764</v>
       </c>
       <c r="E114" s="20" t="s">
         <v>289</v>
@@ -12473,7 +12473,7 @@
       </c>
       <c r="H114" s="20"/>
       <c r="I114" s="20" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="J114" s="20"/>
       <c r="K114" s="20"/>
@@ -12509,29 +12509,29 @@
     </row>
     <row r="115" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="20" t="s">
+        <v>765</v>
+      </c>
+      <c r="B115" s="20" t="s">
+        <v>751</v>
+      </c>
+      <c r="C115" s="20" t="s">
         <v>766</v>
       </c>
-      <c r="B115" s="20" t="s">
-        <v>752</v>
-      </c>
-      <c r="C115" s="20" t="s">
+      <c r="D115" s="20" t="s">
         <v>767</v>
-      </c>
-      <c r="D115" s="20" t="s">
-        <v>768</v>
       </c>
       <c r="E115" s="20" t="s">
         <v>209</v>
       </c>
       <c r="F115" s="20" t="s">
+        <v>768</v>
+      </c>
+      <c r="G115" s="21" t="s">
         <v>769</v>
-      </c>
-      <c r="G115" s="21" t="s">
-        <v>770</v>
       </c>
       <c r="H115" s="20"/>
       <c r="I115" s="20" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="J115" s="20"/>
       <c r="K115" s="20"/>
@@ -12567,16 +12567,16 @@
     </row>
     <row r="116" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="20" t="s">
+        <v>771</v>
+      </c>
+      <c r="B116" s="20" t="s">
+        <v>751</v>
+      </c>
+      <c r="C116" s="20" t="s">
         <v>772</v>
       </c>
-      <c r="B116" s="20" t="s">
-        <v>752</v>
-      </c>
-      <c r="C116" s="20" t="s">
+      <c r="D116" s="20" t="s">
         <v>773</v>
-      </c>
-      <c r="D116" s="20" t="s">
-        <v>774</v>
       </c>
       <c r="E116" s="20" t="s">
         <v>305</v>
@@ -12585,7 +12585,7 @@
       <c r="G116" s="21"/>
       <c r="H116" s="20"/>
       <c r="I116" s="20" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="J116" s="20"/>
       <c r="K116" s="20"/>
@@ -12610,16 +12610,16 @@
     </row>
     <row r="117" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="20" t="s">
+        <v>775</v>
+      </c>
+      <c r="B117" s="20" t="s">
+        <v>751</v>
+      </c>
+      <c r="C117" s="20" t="s">
         <v>776</v>
       </c>
-      <c r="B117" s="20" t="s">
-        <v>752</v>
-      </c>
-      <c r="C117" s="20" t="s">
+      <c r="D117" s="20" t="s">
         <v>777</v>
-      </c>
-      <c r="D117" s="20" t="s">
-        <v>778</v>
       </c>
       <c r="E117" s="20" t="s">
         <v>248</v>
@@ -12630,7 +12630,7 @@
       <c r="G117" s="21"/>
       <c r="H117" s="20"/>
       <c r="I117" s="20" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="J117" s="20"/>
       <c r="K117" s="20" t="s">
@@ -12683,113 +12683,113 @@
     </row>
     <row r="118" spans="1:29" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="34" t="s">
+        <v>779</v>
+      </c>
+      <c r="B118" s="34" t="s">
+        <v>920</v>
+      </c>
+      <c r="C118" s="48" t="s">
         <v>780</v>
       </c>
-      <c r="B118" s="34" t="s">
-        <v>921</v>
-      </c>
-      <c r="C118" s="48" t="s">
-        <v>781</v>
-      </c>
       <c r="D118" s="34" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="E118" s="35" t="s">
         <v>305</v>
       </c>
       <c r="F118" s="34"/>
       <c r="H118" s="63" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="I118" s="49" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="AB118" s="53" t="s">
+        <v>934</v>
+      </c>
+      <c r="AC118" s="57" t="s">
         <v>935</v>
-      </c>
-      <c r="AC118" s="57" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="119" spans="1:29" ht="148" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="34" t="s">
+        <v>781</v>
+      </c>
+      <c r="B119" s="34" t="s">
+        <v>920</v>
+      </c>
+      <c r="C119" s="48" t="s">
         <v>782</v>
       </c>
-      <c r="B119" s="34" t="s">
-        <v>921</v>
-      </c>
-      <c r="C119" s="48" t="s">
-        <v>783</v>
-      </c>
       <c r="D119" s="34" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E119" s="34" t="s">
         <v>209</v>
       </c>
       <c r="F119" s="49" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="H119" s="64"/>
       <c r="I119" s="49" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="AB119" s="53" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="AC119" s="56" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="120" spans="1:29" ht="243" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="34" t="s">
+        <v>783</v>
+      </c>
+      <c r="B120" s="34" t="s">
+        <v>920</v>
+      </c>
+      <c r="C120" s="48" t="s">
         <v>784</v>
       </c>
-      <c r="B120" s="34" t="s">
-        <v>921</v>
-      </c>
-      <c r="C120" s="48" t="s">
-        <v>785</v>
-      </c>
       <c r="D120" s="34" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="E120" s="34" t="s">
         <v>209</v>
       </c>
       <c r="F120" s="49" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="H120" s="64"/>
       <c r="I120" s="49" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="AC120" s="55" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="121" spans="1:29" ht="186" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="34" t="s">
+        <v>785</v>
+      </c>
+      <c r="B121" s="34" t="s">
+        <v>920</v>
+      </c>
+      <c r="C121" s="48" t="s">
         <v>786</v>
       </c>
-      <c r="B121" s="34" t="s">
-        <v>921</v>
-      </c>
-      <c r="C121" s="48" t="s">
-        <v>787</v>
-      </c>
       <c r="D121" s="34" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="E121" s="34" t="s">
         <v>209</v>
       </c>
       <c r="F121" s="49" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="H121" s="64"/>
       <c r="I121" s="49" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="AB121" s="53" t="s">
         <v>213</v>
@@ -12797,16 +12797,16 @@
     </row>
     <row r="122" spans="1:29" ht="28" x14ac:dyDescent="0.2">
       <c r="A122" s="34" t="s">
+        <v>787</v>
+      </c>
+      <c r="B122" s="34" t="s">
+        <v>920</v>
+      </c>
+      <c r="C122" s="48" t="s">
         <v>788</v>
       </c>
-      <c r="B122" s="34" t="s">
-        <v>921</v>
-      </c>
-      <c r="C122" s="48" t="s">
-        <v>789</v>
-      </c>
       <c r="D122" s="34" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E122" s="35" t="s">
         <v>236</v>
@@ -12816,7 +12816,7 @@
       </c>
       <c r="H122" s="64"/>
       <c r="I122" s="49" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="AB122" s="53" t="s">
         <v>232</v>
@@ -12824,16 +12824,16 @@
     </row>
     <row r="123" spans="1:29" ht="28" x14ac:dyDescent="0.2">
       <c r="A123" s="34" t="s">
+        <v>789</v>
+      </c>
+      <c r="B123" s="34" t="s">
+        <v>920</v>
+      </c>
+      <c r="C123" s="48" t="s">
         <v>790</v>
       </c>
-      <c r="B123" s="34" t="s">
-        <v>921</v>
-      </c>
-      <c r="C123" s="48" t="s">
-        <v>791</v>
-      </c>
       <c r="D123" s="34" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="E123" s="35" t="s">
         <v>236</v>
@@ -12843,7 +12843,7 @@
       </c>
       <c r="H123" s="64"/>
       <c r="I123" s="49" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="AB123" s="53" t="s">
         <v>232</v>
@@ -12851,16 +12851,16 @@
     </row>
     <row r="124" spans="1:29" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="34" t="s">
+        <v>791</v>
+      </c>
+      <c r="B124" s="34" t="s">
+        <v>920</v>
+      </c>
+      <c r="C124" s="34" t="s">
         <v>792</v>
       </c>
-      <c r="B124" s="34" t="s">
-        <v>921</v>
-      </c>
-      <c r="C124" s="34" t="s">
-        <v>793</v>
-      </c>
       <c r="D124" s="34" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="E124" s="34" t="s">
         <v>289</v>
@@ -12871,7 +12871,7 @@
       <c r="G124" s="34"/>
       <c r="H124" s="34"/>
       <c r="I124" s="49" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="126" spans="1:29" x14ac:dyDescent="0.2">
@@ -12911,7 +12911,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12956,7 +12958,7 @@
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="B2" s="27" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
@@ -13014,7 +13016,7 @@
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27"/>
       <c r="B4" s="27" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -13072,10 +13074,10 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="27"/>
       <c r="B6" s="27" t="s">
+        <v>795</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>796</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>797</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="27"/>
@@ -13105,7 +13107,7 @@
       <c r="A7" s="11"/>
       <c r="B7" s="11"/>
       <c r="C7" s="27" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
@@ -13162,10 +13164,10 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="27"/>
       <c r="B9" s="27" t="s">
+        <v>798</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>799</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>800</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="27"/>
@@ -13195,11 +13197,11 @@
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
       <c r="C10" s="27" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="27" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
@@ -13254,12 +13256,12 @@
     <row r="12" spans="1:26" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="27" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="22" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
@@ -13314,14 +13316,14 @@
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="27" t="s">
+        <v>804</v>
+      </c>
+      <c r="C14" s="27" t="s">
         <v>805</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>806</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="22" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
@@ -13378,10 +13380,10 @@
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="27" t="s">
+        <v>807</v>
+      </c>
+      <c r="E16" s="22" t="s">
         <v>808</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>809</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
@@ -13410,10 +13412,10 @@
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="27" t="s">
+        <v>809</v>
+      </c>
+      <c r="E17" s="22" t="s">
         <v>810</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>811</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="11"/>
@@ -13442,10 +13444,10 @@
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="27" t="s">
+        <v>811</v>
+      </c>
+      <c r="E18" s="22" t="s">
         <v>812</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>813</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="11"/>
@@ -13501,11 +13503,11 @@
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
       <c r="C20" s="27" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="22" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="11"/>
@@ -13557,15 +13559,15 @@
       <c r="Y21" s="11"/>
       <c r="Z21" s="27"/>
     </row>
-    <row r="22" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="27" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E22" s="22" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -13589,15 +13591,15 @@
       <c r="Y22" s="11"/>
       <c r="Z22" s="27"/>
     </row>
-    <row r="23" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
       <c r="D23" s="27" t="s">
+        <v>816</v>
+      </c>
+      <c r="E23" s="55" t="s">
         <v>817</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>818</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -13653,11 +13655,11 @@
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="27" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="22" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
@@ -13709,15 +13711,15 @@
       <c r="Y26" s="27"/>
       <c r="Z26" s="27"/>
     </row>
-    <row r="27" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="28" t="s">
+        <v>820</v>
+      </c>
+      <c r="E27" s="55" t="s">
         <v>821</v>
-      </c>
-      <c r="E27" s="22" t="s">
-        <v>822</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
@@ -13741,15 +13743,15 @@
       <c r="Y27" s="11"/>
       <c r="Z27" s="27"/>
     </row>
-    <row r="28" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
       <c r="D28" s="28" t="s">
+        <v>822</v>
+      </c>
+      <c r="E28" s="22" t="s">
         <v>823</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>824</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
@@ -13773,15 +13775,15 @@
       <c r="Y28" s="11"/>
       <c r="Z28" s="27"/>
     </row>
-    <row r="29" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
       <c r="D29" s="28" t="s">
+        <v>824</v>
+      </c>
+      <c r="E29" s="22" t="s">
         <v>825</v>
-      </c>
-      <c r="E29" s="22" t="s">
-        <v>826</v>
       </c>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -13805,15 +13807,15 @@
       <c r="Y29" s="11"/>
       <c r="Z29" s="27"/>
     </row>
-    <row r="30" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
       <c r="D30" s="28" t="s">
+        <v>826</v>
+      </c>
+      <c r="E30" s="22" t="s">
         <v>827</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>828</v>
       </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
@@ -13837,15 +13839,15 @@
       <c r="Y30" s="11"/>
       <c r="Z30" s="27"/>
     </row>
-    <row r="31" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
       <c r="D31" s="28" t="s">
+        <v>828</v>
+      </c>
+      <c r="E31" s="22" t="s">
         <v>829</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>830</v>
       </c>
       <c r="F31" s="11"/>
       <c r="G31" s="11"/>
@@ -13897,15 +13899,15 @@
       <c r="Y32" s="27"/>
       <c r="Z32" s="27"/>
     </row>
-    <row r="33" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
       <c r="B33" s="11"/>
       <c r="C33" s="27" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D33" s="11"/>
       <c r="E33" s="22" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -13957,15 +13959,15 @@
       <c r="Y34" s="27"/>
       <c r="Z34" s="27"/>
     </row>
-    <row r="35" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="27" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E35" s="22" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -13994,10 +13996,10 @@
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="27" t="s">
+        <v>833</v>
+      </c>
+      <c r="E36" s="22" t="s">
         <v>834</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>835</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
@@ -14026,10 +14028,10 @@
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="27" t="s">
+        <v>835</v>
+      </c>
+      <c r="E37" s="22" t="s">
         <v>836</v>
-      </c>
-      <c r="E37" s="22" t="s">
-        <v>837</v>
       </c>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
@@ -14058,10 +14060,10 @@
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="27" t="s">
+        <v>837</v>
+      </c>
+      <c r="E38" s="22" t="s">
         <v>838</v>
-      </c>
-      <c r="E38" s="22" t="s">
-        <v>839</v>
       </c>
       <c r="F38" s="11"/>
       <c r="G38" s="11"/>
@@ -14090,10 +14092,10 @@
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
       <c r="D39" s="27" t="s">
+        <v>839</v>
+      </c>
+      <c r="E39" s="22" t="s">
         <v>840</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>841</v>
       </c>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
@@ -14145,15 +14147,15 @@
       <c r="Y40" s="11"/>
       <c r="Z40" s="27"/>
     </row>
-    <row r="41" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
       <c r="B41" s="11"/>
       <c r="C41" s="11" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="22" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F41" s="11"/>
       <c r="G41" s="11"/>
@@ -14210,10 +14212,10 @@
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
       <c r="D43" s="27" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
@@ -14242,10 +14244,10 @@
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
       <c r="D44" s="28" t="s">
+        <v>844</v>
+      </c>
+      <c r="E44" s="22" t="s">
         <v>845</v>
-      </c>
-      <c r="E44" s="22" t="s">
-        <v>846</v>
       </c>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
@@ -14269,15 +14271,15 @@
       <c r="Y44" s="11"/>
       <c r="Z44" s="27"/>
     </row>
-    <row r="45" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
       <c r="D45" s="27" t="s">
+        <v>846</v>
+      </c>
+      <c r="E45" s="20" t="s">
         <v>847</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>848</v>
       </c>
       <c r="F45" s="11"/>
       <c r="G45" s="11"/>
@@ -14332,14 +14334,14 @@
     <row r="47" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="27"/>
       <c r="B47" s="27" t="s">
+        <v>848</v>
+      </c>
+      <c r="C47" s="27" t="s">
         <v>849</v>
-      </c>
-      <c r="C47" s="27" t="s">
-        <v>850</v>
       </c>
       <c r="D47" s="27"/>
       <c r="E47" s="22" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F47" s="27"/>
       <c r="G47" s="27"/>
@@ -14369,7 +14371,7 @@
       <c r="C48" s="27"/>
       <c r="D48" s="27"/>
       <c r="E48" s="22" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F48" s="27"/>
       <c r="G48" s="27"/>
@@ -14399,7 +14401,7 @@
       <c r="C49" s="27"/>
       <c r="D49" s="27"/>
       <c r="E49" s="22" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F49" s="27"/>
       <c r="G49" s="27"/>
@@ -15428,7 +15430,7 @@
         <v>235</v>
       </c>
       <c r="D2" s="58" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E2" s="58" t="s">
         <v>236</v>
@@ -15449,7 +15451,7 @@
         <v>272</v>
       </c>
       <c r="D3" s="58" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E3" s="58" t="s">
         <v>209</v>
@@ -15470,7 +15472,7 @@
         <v>284</v>
       </c>
       <c r="D4" s="58" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="E4" s="58" t="s">
         <v>236</v>
@@ -15491,7 +15493,7 @@
         <v>431</v>
       </c>
       <c r="D5" s="58" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="E5" s="58" t="s">
         <v>305</v>
@@ -15510,7 +15512,7 @@
         <v>512</v>
       </c>
       <c r="D6" s="58" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="E6" s="58" t="s">
         <v>305</v>
@@ -15529,7 +15531,7 @@
         <v>399</v>
       </c>
       <c r="D7" s="58" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="E7" s="58" t="s">
         <v>305</v>
@@ -15548,7 +15550,7 @@
         <v>403</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="E8" s="58" t="s">
         <v>305</v>
@@ -15567,7 +15569,7 @@
         <v>412</v>
       </c>
       <c r="D9" s="58" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="E9" s="58" t="s">
         <v>305</v>
@@ -15577,16 +15579,16 @@
     </row>
     <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="58" t="s">
+        <v>860</v>
+      </c>
+      <c r="B10" s="58" t="s">
         <v>861</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="C10" s="58" t="s">
         <v>862</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="D10" s="58" t="s">
         <v>863</v>
-      </c>
-      <c r="D10" s="58" t="s">
-        <v>864</v>
       </c>
       <c r="E10" s="58" t="s">
         <v>305</v>
@@ -15605,7 +15607,7 @@
         <v>372</v>
       </c>
       <c r="D11" s="58" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E11" s="58" t="s">
         <v>305</v>
@@ -15621,10 +15623,10 @@
         <v>435</v>
       </c>
       <c r="C12" s="58" t="s">
+        <v>865</v>
+      </c>
+      <c r="D12" s="58" t="s">
         <v>866</v>
-      </c>
-      <c r="D12" s="58" t="s">
-        <v>867</v>
       </c>
       <c r="E12" s="58" t="s">
         <v>305</v>
@@ -15681,7 +15683,7 @@
         <v>547</v>
       </c>
       <c r="D15" s="58" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E15" s="58" t="s">
         <v>305</v>
@@ -15691,16 +15693,16 @@
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="58" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B16" s="58" t="s">
+        <v>752</v>
+      </c>
+      <c r="C16" s="58" t="s">
         <v>753</v>
       </c>
-      <c r="C16" s="58" t="s">
-        <v>754</v>
-      </c>
       <c r="D16" s="58" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E16" s="58" t="s">
         <v>236</v>
@@ -15712,16 +15714,16 @@
     </row>
     <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="58" t="s">
+        <v>756</v>
+      </c>
+      <c r="B17" s="58" t="s">
         <v>757</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="C17" s="58" t="s">
         <v>758</v>
       </c>
-      <c r="C17" s="58" t="s">
-        <v>759</v>
-      </c>
       <c r="D17" s="58" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E17" s="58" t="s">
         <v>305</v>
@@ -15740,7 +15742,7 @@
         <v>571</v>
       </c>
       <c r="D18" s="58" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E18" s="58" t="s">
         <v>236</v>
@@ -15761,7 +15763,7 @@
         <v>506</v>
       </c>
       <c r="D19" s="59" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E19" s="59" t="s">
         <v>236</v>
@@ -15782,57 +15784,57 @@
     </row>
     <row r="21" spans="1:7" s="34" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="61" t="s">
+        <v>872</v>
+      </c>
+      <c r="B21" s="61" t="s">
         <v>873</v>
       </c>
-      <c r="B21" s="61" t="s">
-        <v>874</v>
-      </c>
       <c r="C21" s="61" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D21" s="61" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="E21" s="61" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F21" s="61"/>
       <c r="G21" s="61"/>
     </row>
     <row r="22" spans="1:7" s="34" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="61" t="s">
+        <v>874</v>
+      </c>
+      <c r="B22" s="61" t="s">
         <v>875</v>
       </c>
-      <c r="B22" s="61" t="s">
-        <v>876</v>
-      </c>
       <c r="C22" s="61" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D22" s="61" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="E22" s="61" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F22" s="61"/>
       <c r="G22" s="61"/>
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="62" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B23" s="62" t="s">
+        <v>953</v>
+      </c>
+      <c r="C23" s="62" t="s">
         <v>954</v>
       </c>
-      <c r="C23" s="62" t="s">
+      <c r="D23" s="62" t="s">
         <v>955</v>
       </c>
-      <c r="D23" s="62" t="s">
-        <v>956</v>
-      </c>
-      <c r="E23" s="59" t="s">
-        <v>941</v>
+      <c r="E23" s="62" t="s">
+        <v>940</v>
       </c>
       <c r="F23" s="59"/>
       <c r="G23" s="59"/>
@@ -15884,16 +15886,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>876</v>
+      </c>
+      <c r="B2" t="s">
         <v>877</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>878</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>879</v>
-      </c>
-      <c r="D2" t="s">
-        <v>880</v>
       </c>
       <c r="E2" t="s">
         <v>236</v>
@@ -15904,16 +15906,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>880</v>
+      </c>
+      <c r="B3" t="s">
         <v>881</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>882</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>883</v>
-      </c>
-      <c r="D3" t="s">
-        <v>884</v>
       </c>
       <c r="E3" t="s">
         <v>236</v>
@@ -15924,22 +15926,22 @@
     </row>
     <row r="4" spans="1:6" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>884</v>
+      </c>
+      <c r="B4" t="s">
         <v>885</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>886</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>887</v>
-      </c>
-      <c r="D4" t="s">
-        <v>888</v>
       </c>
       <c r="E4" t="s">
         <v>209</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -15953,7 +15955,7 @@
         <v>480</v>
       </c>
       <c r="D5" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E5" t="s">
         <v>248</v>
@@ -15964,16 +15966,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>889</v>
+      </c>
+      <c r="B6" t="s">
         <v>890</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>891</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>892</v>
-      </c>
-      <c r="D6" t="s">
-        <v>893</v>
       </c>
       <c r="E6" t="s">
         <v>305</v>
@@ -15981,19 +15983,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>893</v>
+      </c>
+      <c r="B7" t="s">
         <v>894</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>895</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>896</v>
       </c>
-      <c r="D7" t="s">
-        <v>897</v>
-      </c>
       <c r="E7" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -16001,13 +16003,13 @@
         <v>251</v>
       </c>
       <c r="B8" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C8" t="s">
         <v>253</v>
       </c>
       <c r="D8" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E8" t="s">
         <v>248</v>
@@ -16056,16 +16058,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>899</v>
+      </c>
+      <c r="B2" t="s">
         <v>900</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>901</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>902</v>
-      </c>
-      <c r="D2" t="s">
-        <v>903</v>
       </c>
       <c r="E2" t="s">
         <v>248</v>
@@ -16073,42 +16075,42 @@
     </row>
     <row r="3" spans="1:6" ht="399" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>903</v>
+      </c>
+      <c r="B3" t="s">
         <v>904</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>905</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>906</v>
-      </c>
-      <c r="D3" t="s">
-        <v>907</v>
       </c>
       <c r="E3" t="s">
         <v>209</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="385" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>908</v>
+      </c>
+      <c r="B4" t="s">
         <v>909</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>910</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>911</v>
-      </c>
-      <c r="D4" t="s">
-        <v>912</v>
       </c>
       <c r="E4" t="s">
         <v>209</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save version of actus-dictionary.xlsx now with all columns unhidden - this exposes the applicability formulae for each contract type
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisnparr/git/actus-dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891AA6C8-DD33-8941-ABF3-3CDBC6E56C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152D700D-2917-E146-9B08-93C29C03FBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13420" yWindow="500" windowWidth="27480" windowHeight="19040" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4860" yWindow="500" windowWidth="27480" windowHeight="19040" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -5989,9 +5989,9 @@
   </sheetPr>
   <dimension ref="A1:AC131"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A121" sqref="A121"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6005,26 +6005,22 @@
     <col min="7" max="7" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="65.6640625" style="47" customWidth="1"/>
-    <col min="10" max="10" width="5.33203125" hidden="1" customWidth="1"/>
-    <col min="11" max="12" width="8.83203125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1640625" hidden="1" customWidth="1"/>
-    <col min="15" max="19" width="6" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="10.33203125" hidden="1" customWidth="1"/>
-    <col min="21" max="22" width="6" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="7" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="6.1640625" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="6" hidden="1" customWidth="1"/>
-    <col min="26" max="27" width="6" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" customWidth="1"/>
+    <col min="11" max="12" width="8.83203125" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" customWidth="1"/>
+    <col min="15" max="19" width="6" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" customWidth="1"/>
+    <col min="21" max="22" width="6" customWidth="1"/>
+    <col min="23" max="23" width="7" customWidth="1"/>
+    <col min="24" max="24" width="6.1640625" customWidth="1"/>
+    <col min="25" max="27" width="6" customWidth="1"/>
     <col min="28" max="28" width="26.83203125" style="54" customWidth="1"/>
     <col min="29" max="29" width="14.5" style="47" customWidth="1"/>
     <col min="30" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>19</v>
-      </c>
       <c r="B1" s="17" t="s">
         <v>192</v>
       </c>
@@ -6108,8 +6104,8 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>206</v>
+      <c r="A2" s="16" t="s">
+        <v>19</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>207</v>
@@ -6185,7 +6181,7 @@
     </row>
     <row r="3" spans="1:29" ht="191.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>207</v>
@@ -6261,7 +6257,7 @@
     </row>
     <row r="4" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>207</v>
@@ -6337,7 +6333,7 @@
     </row>
     <row r="5" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>227</v>
@@ -6419,7 +6415,7 @@
     </row>
     <row r="6" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>227</v>
@@ -6501,7 +6497,7 @@
     </row>
     <row r="7" spans="1:29" ht="156" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>227</v>
@@ -6583,7 +6579,7 @@
     </row>
     <row r="8" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>227</v>
@@ -6668,7 +6664,7 @@
     </row>
     <row r="9" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>227</v>
@@ -6748,7 +6744,7 @@
     </row>
     <row r="10" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>227</v>
@@ -6818,7 +6814,7 @@
     </row>
     <row r="11" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>227</v>
@@ -6874,7 +6870,7 @@
     </row>
     <row r="12" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>265</v>
@@ -6955,7 +6951,7 @@
     </row>
     <row r="13" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>265</v>
@@ -7034,7 +7030,7 @@
     </row>
     <row r="14" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>265</v>
@@ -7106,7 +7102,7 @@
     </row>
     <row r="15" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>265</v>
@@ -7180,7 +7176,7 @@
     </row>
     <row r="16" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B16" s="20" t="s">
         <v>265</v>
@@ -7240,7 +7236,7 @@
     </row>
     <row r="17" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>265</v>
@@ -7314,7 +7310,7 @@
     </row>
     <row r="18" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>265</v>
@@ -7388,7 +7384,7 @@
     </row>
     <row r="19" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>265</v>
@@ -7462,7 +7458,7 @@
     </row>
     <row r="20" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>265</v>
@@ -7509,7 +7505,7 @@
     </row>
     <row r="21" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>265</v>
@@ -7558,7 +7554,7 @@
     </row>
     <row r="22" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>265</v>
@@ -7607,7 +7603,7 @@
     </row>
     <row r="23" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>326</v>
@@ -7652,7 +7648,7 @@
     </row>
     <row r="24" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>326</v>
@@ -7697,7 +7693,7 @@
     </row>
     <row r="25" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>326</v>
@@ -7746,7 +7742,7 @@
     </row>
     <row r="26" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>326</v>
@@ -7791,7 +7787,7 @@
     </row>
     <row r="27" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>350</v>
@@ -7850,7 +7846,7 @@
     </row>
     <row r="28" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B28" s="20" t="s">
         <v>350</v>
@@ -7909,7 +7905,7 @@
     </row>
     <row r="29" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>350</v>
@@ -7968,7 +7964,7 @@
     </row>
     <row r="30" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>350</v>
@@ -8025,7 +8021,7 @@
     </row>
     <row r="31" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B31" s="20" t="s">
         <v>350</v>
@@ -8082,7 +8078,7 @@
     </row>
     <row r="32" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>376</v>
@@ -8139,7 +8135,7 @@
     </row>
     <row r="33" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B33" s="20" t="s">
         <v>376</v>
@@ -8184,7 +8180,7 @@
     </row>
     <row r="34" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>376</v>
@@ -8241,7 +8237,7 @@
     </row>
     <row r="35" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B35" s="20" t="s">
         <v>376</v>
@@ -8284,7 +8280,7 @@
     </row>
     <row r="36" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B36" s="20" t="s">
         <v>376</v>
@@ -8341,7 +8337,7 @@
     </row>
     <row r="37" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>376</v>
@@ -8384,7 +8380,7 @@
     </row>
     <row r="38" spans="1:27" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>376</v>
@@ -8443,7 +8439,7 @@
     </row>
     <row r="39" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>376</v>
@@ -8500,7 +8496,7 @@
     </row>
     <row r="40" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B40" s="20" t="s">
         <v>376</v>
@@ -8553,7 +8549,7 @@
     </row>
     <row r="41" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B41" s="20" t="s">
         <v>376</v>
@@ -8604,7 +8600,7 @@
     </row>
     <row r="42" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>376</v>
@@ -8655,7 +8651,7 @@
     </row>
     <row r="43" spans="1:27" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="B43" s="20" t="s">
         <v>376</v>
@@ -8710,7 +8706,7 @@
     </row>
     <row r="44" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B44" s="20" t="s">
         <v>376</v>
@@ -8763,7 +8759,7 @@
     </row>
     <row r="45" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="B45" s="20" t="s">
         <v>376</v>
@@ -8814,7 +8810,7 @@
     </row>
     <row r="46" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="B46" s="20" t="s">
         <v>180</v>
@@ -8859,7 +8855,7 @@
     </row>
     <row r="47" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="B47" s="20" t="s">
         <v>180</v>
@@ -8908,7 +8904,7 @@
     </row>
     <row r="48" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>180</v>
@@ -8953,7 +8949,7 @@
     </row>
     <row r="49" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>180</v>
@@ -8998,7 +8994,7 @@
     </row>
     <row r="50" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B50" s="20" t="s">
         <v>180</v>
@@ -9043,7 +9039,7 @@
     </row>
     <row r="51" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>180</v>
@@ -9088,7 +9084,7 @@
     </row>
     <row r="52" spans="1:29" ht="136.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>180</v>
@@ -9133,7 +9129,7 @@
     </row>
     <row r="53" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B53" s="20" t="s">
         <v>478</v>
@@ -9210,7 +9206,7 @@
     </row>
     <row r="54" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>478</v>
@@ -9255,7 +9251,7 @@
     </row>
     <row r="55" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>478</v>
@@ -9300,7 +9296,7 @@
     </row>
     <row r="56" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B56" s="20" t="s">
         <v>478</v>
@@ -9380,7 +9376,7 @@
     </row>
     <row r="57" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="B57" s="20" t="s">
         <v>478</v>
@@ -9439,7 +9435,7 @@
     </row>
     <row r="58" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>478</v>
@@ -9494,7 +9490,7 @@
     </row>
     <row r="59" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B59" s="20" t="s">
         <v>478</v>
@@ -9562,7 +9558,7 @@
     </row>
     <row r="60" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B60" s="20" t="s">
         <v>478</v>
@@ -9631,7 +9627,7 @@
     </row>
     <row r="61" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="20" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B61" s="20" t="s">
         <v>478</v>
@@ -9678,7 +9674,7 @@
     </row>
     <row r="62" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="B62" s="20" t="s">
         <v>478</v>
@@ -9733,7 +9729,7 @@
     </row>
     <row r="63" spans="1:29" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="B63" s="20" t="s">
         <v>478</v>
@@ -9778,7 +9774,7 @@
     </row>
     <row r="64" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="B64" s="20" t="s">
         <v>478</v>
@@ -9827,7 +9823,7 @@
     </row>
     <row r="65" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="B65" s="20" t="s">
         <v>478</v>
@@ -9870,7 +9866,7 @@
     </row>
     <row r="66" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="B66" s="20" t="s">
         <v>478</v>
@@ -9919,7 +9915,7 @@
     </row>
     <row r="67" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="B67" s="20" t="s">
         <v>478</v>
@@ -9962,7 +9958,7 @@
     </row>
     <row r="68" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="B68" s="20" t="s">
         <v>478</v>
@@ -10013,7 +10009,7 @@
     </row>
     <row r="69" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B69" s="20" t="s">
         <v>478</v>
@@ -10056,7 +10052,7 @@
     </row>
     <row r="70" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="20" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="B70" s="20" t="s">
         <v>478</v>
@@ -10101,7 +10097,7 @@
     </row>
     <row r="71" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="20" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="B71" s="20" t="s">
         <v>478</v>
@@ -10175,7 +10171,7 @@
     </row>
     <row r="72" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="B72" s="20" t="s">
         <v>478</v>
@@ -10249,7 +10245,7 @@
     </row>
     <row r="73" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="20" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="B73" s="20" t="s">
         <v>478</v>
@@ -10328,7 +10324,7 @@
     </row>
     <row r="74" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="20" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="B74" s="20" t="s">
         <v>478</v>
@@ -10405,7 +10401,7 @@
     </row>
     <row r="75" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="B75" s="20" t="s">
         <v>478</v>
@@ -10452,7 +10448,7 @@
     </row>
     <row r="76" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="B76" s="20" t="s">
         <v>478</v>
@@ -10505,7 +10501,7 @@
     </row>
     <row r="77" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="20" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="B77" s="20" t="s">
         <v>478</v>
@@ -10554,7 +10550,7 @@
     </row>
     <row r="78" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="20" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="B78" s="20" t="s">
         <v>478</v>
@@ -10605,7 +10601,7 @@
     </row>
     <row r="79" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="20" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="B79" s="20" t="s">
         <v>478</v>
@@ -10658,7 +10654,7 @@
     </row>
     <row r="80" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="20" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="B80" s="20" t="s">
         <v>478</v>
@@ -10711,7 +10707,7 @@
     </row>
     <row r="81" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="20" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="B81" s="20" t="s">
         <v>478</v>
@@ -10764,7 +10760,7 @@
     </row>
     <row r="82" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="20" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="B82" s="20" t="s">
         <v>478</v>
@@ -10817,7 +10813,7 @@
     </row>
     <row r="83" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="20" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B83" s="20" t="s">
         <v>478</v>
@@ -10872,7 +10868,7 @@
     </row>
     <row r="84" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="20" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="B84" s="20" t="s">
         <v>478</v>
@@ -10944,7 +10940,7 @@
     </row>
     <row r="85" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="20" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B85" s="20" t="s">
         <v>624</v>
@@ -10989,7 +10985,7 @@
     </row>
     <row r="86" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="20" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="B86" s="20" t="s">
         <v>624</v>
@@ -11044,7 +11040,7 @@
     </row>
     <row r="87" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="20" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="B87" s="20" t="s">
         <v>624</v>
@@ -11091,7 +11087,7 @@
     </row>
     <row r="88" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="20" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B88" s="20" t="s">
         <v>624</v>
@@ -11138,7 +11134,7 @@
     </row>
     <row r="89" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="20" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="B89" s="20" t="s">
         <v>624</v>
@@ -11183,7 +11179,7 @@
     </row>
     <row r="90" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="20" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="B90" s="20" t="s">
         <v>624</v>
@@ -11238,7 +11234,7 @@
     </row>
     <row r="91" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="20" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B91" s="20" t="s">
         <v>624</v>
@@ -11293,7 +11289,7 @@
     </row>
     <row r="92" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="20" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="B92" s="20" t="s">
         <v>624</v>
@@ -11348,7 +11344,7 @@
     </row>
     <row r="93" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="20" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="B93" s="20" t="s">
         <v>624</v>
@@ -11405,7 +11401,7 @@
     </row>
     <row r="94" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="20" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="B94" s="20" t="s">
         <v>624</v>
@@ -11460,7 +11456,7 @@
     </row>
     <row r="95" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="20" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="B95" s="20" t="s">
         <v>624</v>
@@ -11507,7 +11503,7 @@
     </row>
     <row r="96" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="20" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="B96" s="20" t="s">
         <v>677</v>
@@ -11564,7 +11560,7 @@
     </row>
     <row r="97" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="20" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="B97" s="20" t="s">
         <v>677</v>
@@ -11607,7 +11603,7 @@
     </row>
     <row r="98" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="20" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="B98" s="20" t="s">
         <v>677</v>
@@ -11664,7 +11660,7 @@
     </row>
     <row r="99" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="20" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="B99" s="20" t="s">
         <v>677</v>
@@ -11707,7 +11703,7 @@
     </row>
     <row r="100" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="20" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="B100" s="20" t="s">
         <v>677</v>
@@ -11764,7 +11760,7 @@
     </row>
     <row r="101" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="20" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="B101" s="20" t="s">
         <v>677</v>
@@ -11807,7 +11803,7 @@
     </row>
     <row r="102" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="20" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B102" s="20" t="s">
         <v>677</v>
@@ -11852,7 +11848,7 @@
     </row>
     <row r="103" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="20" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="B103" s="20" t="s">
         <v>677</v>
@@ -11909,7 +11905,7 @@
     </row>
     <row r="104" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="20" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="B104" s="20" t="s">
         <v>677</v>
@@ -11962,7 +11958,7 @@
     </row>
     <row r="105" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="20" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="B105" s="20" t="s">
         <v>677</v>
@@ -12015,7 +12011,7 @@
     </row>
     <row r="106" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="20" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="B106" s="20" t="s">
         <v>677</v>
@@ -12068,7 +12064,7 @@
     </row>
     <row r="107" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="20" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="B107" s="20" t="s">
         <v>677</v>
@@ -12121,7 +12117,7 @@
     </row>
     <row r="108" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="20" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
       <c r="B108" s="20" t="s">
         <v>677</v>
@@ -12174,7 +12170,7 @@
     </row>
     <row r="109" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="20" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
       <c r="B109" s="20" t="s">
         <v>677</v>
@@ -12233,7 +12229,7 @@
     </row>
     <row r="110" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="20" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="B110" s="20" t="s">
         <v>677</v>
@@ -12288,7 +12284,7 @@
     </row>
     <row r="111" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="20" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="B111" s="20" t="s">
         <v>677</v>
@@ -12345,7 +12341,7 @@
     </row>
     <row r="112" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="20" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="B112" s="20" t="s">
         <v>751</v>
@@ -12398,7 +12394,7 @@
     </row>
     <row r="113" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="20" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="B113" s="20" t="s">
         <v>751</v>
@@ -12451,7 +12447,7 @@
     </row>
     <row r="114" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="20" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
       <c r="B114" s="20" t="s">
         <v>751</v>
@@ -12509,7 +12505,7 @@
     </row>
     <row r="115" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="20" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="B115" s="20" t="s">
         <v>751</v>
@@ -12567,7 +12563,7 @@
     </row>
     <row r="116" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="20" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
       <c r="B116" s="20" t="s">
         <v>751</v>
@@ -12610,7 +12606,7 @@
     </row>
     <row r="117" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="20" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
       <c r="B117" s="20" t="s">
         <v>751</v>
@@ -12682,8 +12678,8 @@
       </c>
     </row>
     <row r="118" spans="1:29" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="34" t="s">
-        <v>779</v>
+      <c r="A118" s="20" t="s">
+        <v>775</v>
       </c>
       <c r="B118" s="34" t="s">
         <v>920</v>
@@ -12713,7 +12709,7 @@
     </row>
     <row r="119" spans="1:29" ht="148" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="34" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="B119" s="34" t="s">
         <v>920</v>
@@ -12743,7 +12739,7 @@
     </row>
     <row r="120" spans="1:29" ht="243" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="34" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="B120" s="34" t="s">
         <v>920</v>
@@ -12770,7 +12766,7 @@
     </row>
     <row r="121" spans="1:29" ht="186" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="34" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="B121" s="34" t="s">
         <v>920</v>
@@ -12797,7 +12793,7 @@
     </row>
     <row r="122" spans="1:29" ht="28" x14ac:dyDescent="0.2">
       <c r="A122" s="34" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="B122" s="34" t="s">
         <v>920</v>
@@ -12824,7 +12820,7 @@
     </row>
     <row r="123" spans="1:29" ht="28" x14ac:dyDescent="0.2">
       <c r="A123" s="34" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="B123" s="34" t="s">
         <v>920</v>
@@ -12851,7 +12847,7 @@
     </row>
     <row r="124" spans="1:29" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="34" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B124" s="34" t="s">
         <v>920</v>
@@ -12872,6 +12868,11 @@
       <c r="H124" s="34"/>
       <c r="I124" s="49" t="s">
         <v>947</v>
+      </c>
+    </row>
+    <row r="125" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A125" s="34" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="126" spans="1:29" x14ac:dyDescent="0.2">
@@ -15849,7 +15850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Now all columns unhidden in spreadsheet ; actus-dictionary-applicability.json generated using create-dictionary.R with applicability information from Shirish entered including boundary controlled switch Type
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisnparr/git/actus-dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152D700D-2917-E146-9B08-93C29C03FBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADF81A1-B13E-E749-95B8-04D71324941F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="500" windowWidth="27480" windowHeight="19040" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7740" yWindow="500" windowWidth="27480" windowHeight="19040" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -5989,9 +5989,9 @@
   </sheetPr>
   <dimension ref="A1:AC131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC1" sqref="AC1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6021,6 +6021,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>19</v>
+      </c>
       <c r="B1" s="17" t="s">
         <v>192</v>
       </c>
@@ -6104,8 +6107,8 @@
       </c>
     </row>
     <row r="2" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
-        <v>19</v>
+      <c r="A2" s="20" t="s">
+        <v>206</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>207</v>
@@ -6181,7 +6184,7 @@
     </row>
     <row r="3" spans="1:29" ht="191.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>207</v>
@@ -6257,7 +6260,7 @@
     </row>
     <row r="4" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>207</v>
@@ -6333,7 +6336,7 @@
     </row>
     <row r="5" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="B5" s="20" t="s">
         <v>227</v>
@@ -6415,7 +6418,7 @@
     </row>
     <row r="6" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="B6" s="20" t="s">
         <v>227</v>
@@ -6497,7 +6500,7 @@
     </row>
     <row r="7" spans="1:29" ht="156" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="B7" s="20" t="s">
         <v>227</v>
@@ -6579,7 +6582,7 @@
     </row>
     <row r="8" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="B8" s="20" t="s">
         <v>227</v>
@@ -6664,7 +6667,7 @@
     </row>
     <row r="9" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>227</v>
@@ -6744,7 +6747,7 @@
     </row>
     <row r="10" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>227</v>
@@ -6814,7 +6817,7 @@
     </row>
     <row r="11" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>227</v>
@@ -6870,7 +6873,7 @@
     </row>
     <row r="12" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>265</v>
@@ -6951,7 +6954,7 @@
     </row>
     <row r="13" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>265</v>
@@ -7030,7 +7033,7 @@
     </row>
     <row r="14" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>265</v>
@@ -7102,7 +7105,7 @@
     </row>
     <row r="15" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="B15" s="20" t="s">
         <v>265</v>
@@ -7176,7 +7179,7 @@
     </row>
     <row r="16" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="B16" s="20" t="s">
         <v>265</v>
@@ -7236,7 +7239,7 @@
     </row>
     <row r="17" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>265</v>
@@ -7310,7 +7313,7 @@
     </row>
     <row r="18" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B18" s="20" t="s">
         <v>265</v>
@@ -7384,7 +7387,7 @@
     </row>
     <row r="19" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>265</v>
@@ -7458,7 +7461,7 @@
     </row>
     <row r="20" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>302</v>
+        <v>308</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>265</v>
@@ -7505,7 +7508,7 @@
     </row>
     <row r="21" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="B21" s="20" t="s">
         <v>265</v>
@@ -7554,7 +7557,7 @@
     </row>
     <row r="22" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="B22" s="20" t="s">
         <v>265</v>
@@ -7603,7 +7606,7 @@
     </row>
     <row r="23" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>326</v>
@@ -7648,7 +7651,7 @@
     </row>
     <row r="24" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>325</v>
+        <v>331</v>
       </c>
       <c r="B24" s="20" t="s">
         <v>326</v>
@@ -7693,7 +7696,7 @@
     </row>
     <row r="25" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="B25" s="20" t="s">
         <v>326</v>
@@ -7742,7 +7745,7 @@
     </row>
     <row r="26" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="B26" s="20" t="s">
         <v>326</v>
@@ -7787,7 +7790,7 @@
     </row>
     <row r="27" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="B27" s="20" t="s">
         <v>350</v>
@@ -7846,7 +7849,7 @@
     </row>
     <row r="28" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="B28" s="20" t="s">
         <v>350</v>
@@ -7905,7 +7908,7 @@
     </row>
     <row r="29" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="B29" s="20" t="s">
         <v>350</v>
@@ -7964,7 +7967,7 @@
     </row>
     <row r="30" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="B30" s="20" t="s">
         <v>350</v>
@@ -8021,7 +8024,7 @@
     </row>
     <row r="31" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="B31" s="20" t="s">
         <v>350</v>
@@ -8078,7 +8081,7 @@
     </row>
     <row r="32" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="B32" s="20" t="s">
         <v>376</v>
@@ -8135,7 +8138,7 @@
     </row>
     <row r="33" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="B33" s="20" t="s">
         <v>376</v>
@@ -8180,7 +8183,7 @@
     </row>
     <row r="34" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="B34" s="20" t="s">
         <v>376</v>
@@ -8237,7 +8240,7 @@
     </row>
     <row r="35" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="B35" s="20" t="s">
         <v>376</v>
@@ -8280,7 +8283,7 @@
     </row>
     <row r="36" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="B36" s="20" t="s">
         <v>376</v>
@@ -8337,7 +8340,7 @@
     </row>
     <row r="37" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="B37" s="20" t="s">
         <v>376</v>
@@ -8380,7 +8383,7 @@
     </row>
     <row r="38" spans="1:27" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="B38" s="20" t="s">
         <v>376</v>
@@ -8439,7 +8442,7 @@
     </row>
     <row r="39" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="B39" s="20" t="s">
         <v>376</v>
@@ -8496,7 +8499,7 @@
     </row>
     <row r="40" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="B40" s="20" t="s">
         <v>376</v>
@@ -8549,7 +8552,7 @@
     </row>
     <row r="41" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="B41" s="20" t="s">
         <v>376</v>
@@ -8600,7 +8603,7 @@
     </row>
     <row r="42" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="B42" s="20" t="s">
         <v>376</v>
@@ -8651,7 +8654,7 @@
     </row>
     <row r="43" spans="1:27" ht="142.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="B43" s="20" t="s">
         <v>376</v>
@@ -8706,7 +8709,7 @@
     </row>
     <row r="44" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="B44" s="20" t="s">
         <v>376</v>
@@ -8759,7 +8762,7 @@
     </row>
     <row r="45" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="B45" s="20" t="s">
         <v>376</v>
@@ -8810,7 +8813,7 @@
     </row>
     <row r="46" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="B46" s="20" t="s">
         <v>180</v>
@@ -8855,7 +8858,7 @@
     </row>
     <row r="47" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="B47" s="20" t="s">
         <v>180</v>
@@ -8904,7 +8907,7 @@
     </row>
     <row r="48" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="B48" s="20" t="s">
         <v>180</v>
@@ -8949,7 +8952,7 @@
     </row>
     <row r="49" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="B49" s="20" t="s">
         <v>180</v>
@@ -8994,7 +8997,7 @@
     </row>
     <row r="50" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B50" s="20" t="s">
         <v>180</v>
@@ -9039,7 +9042,7 @@
     </row>
     <row r="51" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B51" s="20" t="s">
         <v>180</v>
@@ -9084,7 +9087,7 @@
     </row>
     <row r="52" spans="1:29" ht="136.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>180</v>
@@ -9129,7 +9132,7 @@
     </row>
     <row r="53" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="B53" s="20" t="s">
         <v>478</v>
@@ -9206,7 +9209,7 @@
     </row>
     <row r="54" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>478</v>
@@ -9251,7 +9254,7 @@
     </row>
     <row r="55" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="B55" s="20" t="s">
         <v>478</v>
@@ -9296,7 +9299,7 @@
     </row>
     <row r="56" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="B56" s="20" t="s">
         <v>478</v>
@@ -9376,7 +9379,7 @@
     </row>
     <row r="57" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="B57" s="20" t="s">
         <v>478</v>
@@ -9435,7 +9438,7 @@
     </row>
     <row r="58" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="B58" s="20" t="s">
         <v>478</v>
@@ -9490,7 +9493,7 @@
     </row>
     <row r="59" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="B59" s="20" t="s">
         <v>478</v>
@@ -9558,7 +9561,7 @@
     </row>
     <row r="60" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="B60" s="20" t="s">
         <v>478</v>
@@ -9627,7 +9630,7 @@
     </row>
     <row r="61" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="20" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B61" s="20" t="s">
         <v>478</v>
@@ -9674,7 +9677,7 @@
     </row>
     <row r="62" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="B62" s="20" t="s">
         <v>478</v>
@@ -9729,7 +9732,7 @@
     </row>
     <row r="63" spans="1:29" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="B63" s="20" t="s">
         <v>478</v>
@@ -9774,7 +9777,7 @@
     </row>
     <row r="64" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
-        <v>520</v>
+        <v>525</v>
       </c>
       <c r="B64" s="20" t="s">
         <v>478</v>
@@ -9823,7 +9826,7 @@
     </row>
     <row r="65" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="B65" s="20" t="s">
         <v>478</v>
@@ -9866,7 +9869,7 @@
     </row>
     <row r="66" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
       <c r="B66" s="20" t="s">
         <v>478</v>
@@ -9915,7 +9918,7 @@
     </row>
     <row r="67" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
-        <v>536</v>
+        <v>540</v>
       </c>
       <c r="B67" s="20" t="s">
         <v>478</v>
@@ -9958,7 +9961,7 @@
     </row>
     <row r="68" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="B68" s="20" t="s">
         <v>478</v>
@@ -10009,7 +10012,7 @@
     </row>
     <row r="69" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="B69" s="20" t="s">
         <v>478</v>
@@ -10052,7 +10055,7 @@
     </row>
     <row r="70" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="20" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="B70" s="20" t="s">
         <v>478</v>
@@ -10097,7 +10100,7 @@
     </row>
     <row r="71" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="20" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="B71" s="20" t="s">
         <v>478</v>
@@ -10171,7 +10174,7 @@
     </row>
     <row r="72" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
       <c r="B72" s="20" t="s">
         <v>478</v>
@@ -10245,7 +10248,7 @@
     </row>
     <row r="73" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="20" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="B73" s="20" t="s">
         <v>478</v>
@@ -10324,7 +10327,7 @@
     </row>
     <row r="74" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="20" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
       <c r="B74" s="20" t="s">
         <v>478</v>
@@ -10401,7 +10404,7 @@
     </row>
     <row r="75" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="B75" s="20" t="s">
         <v>478</v>
@@ -10448,7 +10451,7 @@
     </row>
     <row r="76" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="B76" s="20" t="s">
         <v>478</v>
@@ -10501,7 +10504,7 @@
     </row>
     <row r="77" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="20" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="B77" s="20" t="s">
         <v>478</v>
@@ -10550,7 +10553,7 @@
     </row>
     <row r="78" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="20" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="B78" s="20" t="s">
         <v>478</v>
@@ -10601,7 +10604,7 @@
     </row>
     <row r="79" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="20" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="B79" s="20" t="s">
         <v>478</v>
@@ -10654,7 +10657,7 @@
     </row>
     <row r="80" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="20" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="B80" s="20" t="s">
         <v>478</v>
@@ -10707,7 +10710,7 @@
     </row>
     <row r="81" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="20" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="B81" s="20" t="s">
         <v>478</v>
@@ -10760,7 +10763,7 @@
     </row>
     <row r="82" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="20" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
       <c r="B82" s="20" t="s">
         <v>478</v>
@@ -10813,7 +10816,7 @@
     </row>
     <row r="83" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="20" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
       <c r="B83" s="20" t="s">
         <v>478</v>
@@ -10868,7 +10871,7 @@
     </row>
     <row r="84" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="20" t="s">
-        <v>612</v>
+        <v>619</v>
       </c>
       <c r="B84" s="20" t="s">
         <v>478</v>
@@ -10940,7 +10943,7 @@
     </row>
     <row r="85" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="20" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="B85" s="20" t="s">
         <v>624</v>
@@ -10985,7 +10988,7 @@
     </row>
     <row r="86" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="20" t="s">
-        <v>623</v>
+        <v>629</v>
       </c>
       <c r="B86" s="20" t="s">
         <v>624</v>
@@ -11040,7 +11043,7 @@
     </row>
     <row r="87" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="20" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
       <c r="B87" s="20" t="s">
         <v>624</v>
@@ -11087,7 +11090,7 @@
     </row>
     <row r="88" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="20" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="B88" s="20" t="s">
         <v>624</v>
@@ -11134,7 +11137,7 @@
     </row>
     <row r="89" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="20" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B89" s="20" t="s">
         <v>624</v>
@@ -11179,7 +11182,7 @@
     </row>
     <row r="90" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="20" t="s">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="B90" s="20" t="s">
         <v>624</v>
@@ -11234,7 +11237,7 @@
     </row>
     <row r="91" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="20" t="s">
-        <v>646</v>
+        <v>650</v>
       </c>
       <c r="B91" s="20" t="s">
         <v>624</v>
@@ -11289,7 +11292,7 @@
     </row>
     <row r="92" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="20" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
       <c r="B92" s="20" t="s">
         <v>624</v>
@@ -11344,7 +11347,7 @@
     </row>
     <row r="93" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="20" t="s">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="B93" s="20" t="s">
         <v>624</v>
@@ -11401,7 +11404,7 @@
     </row>
     <row r="94" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="20" t="s">
-        <v>660</v>
+        <v>664</v>
       </c>
       <c r="B94" s="20" t="s">
         <v>624</v>
@@ -11456,7 +11459,7 @@
     </row>
     <row r="95" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="20" t="s">
-        <v>664</v>
+        <v>671</v>
       </c>
       <c r="B95" s="20" t="s">
         <v>624</v>
@@ -11503,7 +11506,7 @@
     </row>
     <row r="96" spans="1:28" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="20" t="s">
-        <v>671</v>
+        <v>676</v>
       </c>
       <c r="B96" s="20" t="s">
         <v>677</v>
@@ -11560,7 +11563,7 @@
     </row>
     <row r="97" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="20" t="s">
-        <v>676</v>
+        <v>684</v>
       </c>
       <c r="B97" s="20" t="s">
         <v>677</v>
@@ -11603,7 +11606,7 @@
     </row>
     <row r="98" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="20" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="B98" s="20" t="s">
         <v>677</v>
@@ -11660,7 +11663,7 @@
     </row>
     <row r="99" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="20" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="B99" s="20" t="s">
         <v>677</v>
@@ -11703,7 +11706,7 @@
     </row>
     <row r="100" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="20" t="s">
-        <v>692</v>
+        <v>697</v>
       </c>
       <c r="B100" s="20" t="s">
         <v>677</v>
@@ -11760,7 +11763,7 @@
     </row>
     <row r="101" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="20" t="s">
-        <v>697</v>
+        <v>702</v>
       </c>
       <c r="B101" s="20" t="s">
         <v>677</v>
@@ -11803,7 +11806,7 @@
     </row>
     <row r="102" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="20" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="B102" s="20" t="s">
         <v>677</v>
@@ -11848,7 +11851,7 @@
     </row>
     <row r="103" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="20" t="s">
-        <v>706</v>
+        <v>711</v>
       </c>
       <c r="B103" s="20" t="s">
         <v>677</v>
@@ -11905,7 +11908,7 @@
     </row>
     <row r="104" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="20" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="B104" s="20" t="s">
         <v>677</v>
@@ -11958,7 +11961,7 @@
     </row>
     <row r="105" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="20" t="s">
-        <v>715</v>
+        <v>719</v>
       </c>
       <c r="B105" s="20" t="s">
         <v>677</v>
@@ -12011,7 +12014,7 @@
     </row>
     <row r="106" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="20" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="B106" s="20" t="s">
         <v>677</v>
@@ -12064,7 +12067,7 @@
     </row>
     <row r="107" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="20" t="s">
-        <v>723</v>
+        <v>727</v>
       </c>
       <c r="B107" s="20" t="s">
         <v>677</v>
@@ -12117,7 +12120,7 @@
     </row>
     <row r="108" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="20" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
       <c r="B108" s="20" t="s">
         <v>677</v>
@@ -12170,7 +12173,7 @@
     </row>
     <row r="109" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="20" t="s">
-        <v>731</v>
+        <v>738</v>
       </c>
       <c r="B109" s="20" t="s">
         <v>677</v>
@@ -12229,7 +12232,7 @@
     </row>
     <row r="110" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="20" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c r="B110" s="20" t="s">
         <v>677</v>
@@ -12284,7 +12287,7 @@
     </row>
     <row r="111" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="20" t="s">
-        <v>742</v>
+        <v>746</v>
       </c>
       <c r="B111" s="20" t="s">
         <v>677</v>
@@ -12341,7 +12344,7 @@
     </row>
     <row r="112" spans="1:27" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="20" t="s">
-        <v>746</v>
+        <v>750</v>
       </c>
       <c r="B112" s="20" t="s">
         <v>751</v>
@@ -12394,7 +12397,7 @@
     </row>
     <row r="113" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="20" t="s">
-        <v>750</v>
+        <v>756</v>
       </c>
       <c r="B113" s="20" t="s">
         <v>751</v>
@@ -12447,7 +12450,7 @@
     </row>
     <row r="114" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="20" t="s">
-        <v>756</v>
+        <v>761</v>
       </c>
       <c r="B114" s="20" t="s">
         <v>751</v>
@@ -12505,7 +12508,7 @@
     </row>
     <row r="115" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="20" t="s">
-        <v>761</v>
+        <v>765</v>
       </c>
       <c r="B115" s="20" t="s">
         <v>751</v>
@@ -12563,7 +12566,7 @@
     </row>
     <row r="116" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="20" t="s">
-        <v>765</v>
+        <v>771</v>
       </c>
       <c r="B116" s="20" t="s">
         <v>751</v>
@@ -12606,7 +12609,7 @@
     </row>
     <row r="117" spans="1:29" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="20" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="B117" s="20" t="s">
         <v>751</v>
@@ -12678,8 +12681,8 @@
       </c>
     </row>
     <row r="118" spans="1:29" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="20" t="s">
-        <v>775</v>
+      <c r="A118" s="34" t="s">
+        <v>779</v>
       </c>
       <c r="B118" s="34" t="s">
         <v>920</v>
@@ -12709,7 +12712,7 @@
     </row>
     <row r="119" spans="1:29" ht="148" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="34" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="B119" s="34" t="s">
         <v>920</v>
@@ -12739,7 +12742,7 @@
     </row>
     <row r="120" spans="1:29" ht="243" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="34" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="B120" s="34" t="s">
         <v>920</v>
@@ -12766,7 +12769,7 @@
     </row>
     <row r="121" spans="1:29" ht="186" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="34" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="B121" s="34" t="s">
         <v>920</v>
@@ -12793,7 +12796,7 @@
     </row>
     <row r="122" spans="1:29" ht="28" x14ac:dyDescent="0.2">
       <c r="A122" s="34" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="B122" s="34" t="s">
         <v>920</v>
@@ -12820,7 +12823,7 @@
     </row>
     <row r="123" spans="1:29" ht="28" x14ac:dyDescent="0.2">
       <c r="A123" s="34" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="B123" s="34" t="s">
         <v>920</v>
@@ -12847,7 +12850,7 @@
     </row>
     <row r="124" spans="1:29" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="34" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="B124" s="34" t="s">
         <v>920</v>
@@ -12868,11 +12871,6 @@
       <c r="H124" s="34"/>
       <c r="I124" s="49" t="s">
         <v>947</v>
-      </c>
-    </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A125" s="34" t="s">
-        <v>791</v>
       </c>
     </row>
     <row r="126" spans="1:29" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Version1.4 of dictionary now being installed with all changes for single boundary boundary controlledswitch contract type. Also spreadsheed is modified to add a version tab with history. the README tab now has current version, current (Version) date and copyright notice. New actus-dictionary-versions.json file is manually created but matches and could be automatically transcribed to/from the version tab in the actus-dictionary.xlsx .  Itemized updateItem lists are included for this and some previous versions of the dictionary.
</commit_message>
<xml_diff>
--- a/actus-dictionary.xlsx
+++ b/actus-dictionary.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francisnparr/git/actus-dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21504A08-4431-084E-99D4-1914D66D7A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233C4F13-8731-BA42-A840-E5DFE35DAAE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="2020" windowWidth="31600" windowHeight="16220" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4400" yWindow="640" windowWidth="27160" windowHeight="17600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Versions" sheetId="1" r:id="rId1"/>
-    <sheet name="Taxonomy" sheetId="2" r:id="rId2"/>
-    <sheet name="Terms" sheetId="3" r:id="rId3"/>
-    <sheet name="Term Applicability Rules" sheetId="4" r:id="rId4"/>
-    <sheet name="State" sheetId="5" r:id="rId5"/>
-    <sheet name="Event" sheetId="6" r:id="rId6"/>
-    <sheet name="ContractStructure" sheetId="7" r:id="rId7"/>
+    <sheet name="README" sheetId="8" r:id="rId1"/>
+    <sheet name="Versions" sheetId="1" r:id="rId2"/>
+    <sheet name="Taxonomy" sheetId="2" r:id="rId3"/>
+    <sheet name="Terms" sheetId="3" r:id="rId4"/>
+    <sheet name="Term Applicability Rules" sheetId="4" r:id="rId5"/>
+    <sheet name="State" sheetId="5" r:id="rId6"/>
+    <sheet name="Event" sheetId="6" r:id="rId7"/>
+    <sheet name="ContractStructure" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Terms!$T$1:$T$117</definedName>
-    <definedName name="Z_29585F7E_9463_4993_8067_5C2E42B28159_.wvu.FilterData" localSheetId="2">Terms!$T$1:$T$117</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Terms!$T$1:$T$117</definedName>
+    <definedName name="Z_29585F7E_9463_4993_8067_5C2E42B28159_.wvu.FilterData" localSheetId="3">Terms!$T$1:$T$117</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2198" uniqueCount="973">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="984">
   <si>
     <t>Version</t>
   </si>
@@ -3248,9 +3249,6 @@
     <t xml:space="preserve">Fixed missing options in the contract performance state variable </t>
   </si>
   <si>
-    <t xml:space="preserve">Fixed various typos </t>
-  </si>
-  <si>
     <t>Added underlying contract roles: UDL, UDLP, UDLM</t>
   </si>
   <si>
@@ -3267,6 +3265,42 @@
   </si>
   <si>
     <t>Summary of updates this version</t>
+  </si>
+  <si>
+    <t>The ACTUS dictionary</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Copyright</t>
+  </si>
+  <si>
+    <t>2018-present by ACTUS Financial Research Foundation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>BoundaryControlledSwitch (BCRSW) contract type added to Taxonomy</t>
+  </si>
+  <si>
+    <t>New terms boundaryValue, boundaryDirection, boundaryEffect, boundaryLegInitiallyActive, boundaryMonitoringAnchorDate, boundaryMonitoringEndDate, boundaryMonitoringCyle added to Terms</t>
+  </si>
+  <si>
+    <t>New term group 'Boundary' added to Terms</t>
+  </si>
+  <si>
+    <t>New states boundaryLeg1Active, boundaryLeg2Active, boundaryCrossed added to States</t>
+  </si>
+  <si>
+    <t>New events boundaryMonitor, boundary added to Events</t>
+  </si>
+  <si>
+    <t>BCRSW contracts with one boundary defined at this time ( multiple boundaryBCRSW contracts are a possible future extension )</t>
   </si>
 </sst>
 </file>
@@ -3277,7 +3311,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3519,6 +3553,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -3600,7 +3645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3772,6 +3817,11 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4159,10 +4209,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73CBEB43-BE58-C240-A9EC-D96D0AE4F7CC}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="70" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="70" t="s">
+        <v>973</v>
+      </c>
+      <c r="B4" s="71" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="70" t="s">
+        <v>974</v>
+      </c>
+      <c r="B6" s="70" t="s">
+        <v>975</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1048573"/>
   <sheetViews>
-    <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4181,10 +4275,10 @@
         <v>950</v>
       </c>
       <c r="C1" s="57" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D1" s="57" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E1" s="58"/>
       <c r="F1" s="58"/>
@@ -4436,7 +4530,7 @@
       <c r="B9" s="65"/>
       <c r="C9" s="2"/>
       <c r="D9" s="61" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="28" customHeight="1" x14ac:dyDescent="0.3">
@@ -4479,12 +4573,12 @@
     <row r="15" spans="1:26" ht="24" x14ac:dyDescent="0.3">
       <c r="A15" s="55"/>
       <c r="D15" s="62" t="s">
-        <v>966</v>
+        <v>976</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="24" x14ac:dyDescent="0.3">
       <c r="A16" s="64" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B16" s="64" t="s">
         <v>951</v>
@@ -4518,13 +4612,13 @@
     </row>
     <row r="17" spans="1:26" ht="24" x14ac:dyDescent="0.3">
       <c r="A17" s="64" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B17" s="64" t="s">
         <v>952</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="D17" s="60"/>
       <c r="E17" s="2"/>
@@ -4550,23 +4644,44 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="1:26" ht="24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="55"/>
-      <c r="D18" s="62"/>
-    </row>
-    <row r="19" spans="1:26" ht="24" x14ac:dyDescent="0.3">
+      <c r="D18" s="72" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="55"/>
-      <c r="D19" s="62"/>
-    </row>
-    <row r="20" spans="1:26" ht="24" x14ac:dyDescent="0.3">
+      <c r="D19" s="72" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="55"/>
-      <c r="D20" s="62"/>
-    </row>
-    <row r="21" spans="1:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="D21" s="62"/>
-    </row>
-    <row r="22" spans="1:26" ht="24" x14ac:dyDescent="0.3">
-      <c r="D22" s="62"/>
+      <c r="D20" s="63" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="25" x14ac:dyDescent="0.3">
+      <c r="D21" s="72" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="50" x14ac:dyDescent="0.3">
+      <c r="D22" s="72" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="25" x14ac:dyDescent="0.3">
+      <c r="D23" s="72" t="s">
+        <v>982</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="D24" s="19"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="D25" s="19"/>
     </row>
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -4575,7 +4690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AA34"/>
   <sheetViews>
@@ -6071,16 +6186,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AD124"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+    <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB124" sqref="AB124"/>
+      <selection pane="bottomLeft" activeCell="A123" sqref="A123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12994,11 +13109,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
       <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -15469,7 +15584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G23"/>
   <sheetViews>
@@ -15921,7 +16036,7 @@
         <v>910</v>
       </c>
       <c r="E23" s="46" t="s">
-        <v>902</v>
+        <v>976</v>
       </c>
       <c r="F23" s="43"/>
       <c r="G23" s="43"/>
@@ -15932,9 +16047,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
@@ -16102,18 +16217,23 @@
         <v>240</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="70" t="s">
+        <v>977</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>